<commit_message>
added daily Position information
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\Git\SMA_GTAA\"/>
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
+    <sheet name="Daily" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Symbol</t>
   </si>
@@ -90,14 +91,57 @@
   </si>
   <si>
     <t>TLT</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Realtime +/-</t>
+  </si>
+  <si>
+    <t>PnL</t>
+  </si>
+  <si>
+    <t>AGG</t>
+  </si>
+  <si>
+    <t>ACWI</t>
+  </si>
+  <si>
+    <t>60/40</t>
+  </si>
+  <si>
+    <t>Market Value</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Porfolio Value</t>
+  </si>
+  <si>
+    <t>Position MV</t>
+  </si>
+  <si>
+    <t>NAV</t>
+  </si>
+  <si>
+    <t>Daily Returns</t>
+  </si>
+  <si>
+    <t>MTD</t>
+  </si>
+  <si>
+    <t>YTD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -151,7 +195,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -166,6 +210,13 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -190,7 +241,16 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp t="s">
+        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>description</stp>
+        <tr r="B7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp t="s">
         <v>ISHARES TR-20 YR TR BD ETF</v>
         <stp/>
@@ -198,13 +258,44 @@
         <stp>description</stp>
         <tr r="B11" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp t="s">
-        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
-        <stp/>
-        <stp>RWX</stp>
+        <v>ISHARES TR-MSCI EMG MKT ETF</v>
+        <stp/>
+        <stp>EEM</stp>
         <stp>description</stp>
-        <tr r="B7" s="1"/>
-      </tp>
+        <tr r="B8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp t="s">
+        <v>ISHARES INC-MSCI JPN ETF NEW</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>description</stp>
+        <tr r="B3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp t="s">
+        <v>POWERSHARES DB CMDTY IDX TRA-UNIT BEN INT</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>description</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp t="s">
+        <v>SPDR GOLD TRUST-GOLD SHS</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>description</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp t="s">
         <v>ISHARES TR-EUROPE ETF</v>
         <stp/>
@@ -219,6 +310,8 @@
         <stp>description</stp>
         <tr r="B10" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp t="s">
         <v>ISHARES TR-U.S. REAL ES ETF</v>
         <stp/>
@@ -233,36 +326,42 @@
         <stp>description</stp>
         <tr r="B6" s="1"/>
       </tp>
-      <tp t="s">
-        <v>SPDR GOLD TRUST-GOLD SHS</v>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>AGG</stp>
+        <stp>change in percent</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+      <tp>
+        <v>-4.1718815185648314E-3</v>
+        <stp/>
+        <stp>ACWI</stp>
+        <stp>change in percent</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>-6.9707304276129369E-3</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>change in percent</stp>
+        <tr r="K24" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>123.65</v>
         <stp/>
         <stp>GLD</stp>
-        <stp>description</stp>
-        <tr r="B4" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ISHARES TR-MSCI EMG MKT ETF</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>description</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ISHARES INC-MSCI JPN ETF NEW</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>description</stp>
-        <tr r="B3" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>POWERSHARES DB CMDTY IDX TRA-UNIT BEN INT</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>description</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
+        <stp>last</stp>
+        <tr r="J4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp>
         <v>47.34</v>
         <stp/>
@@ -278,7 +377,16 @@
         <tr r="G6" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>47.36</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>last</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp>
         <v>40.729999999999997</v>
         <stp/>
@@ -287,7 +395,25 @@
         <tr r="G7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>17.46</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>last</stp>
+        <tr r="J2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>123.71</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>close</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp>
         <v>17.46</v>
         <stp/>
@@ -296,16 +422,34 @@
         <tr r="G2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
-      <tp>
-        <v>123.71</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>close</stp>
-        <tr r="G4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.a300462a3ad444eb9e3d8c7486fcb3c4">
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>60.23</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>last</stp>
+        <tr r="J3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>40.409999999999997</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>last</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+      <tp>
+        <v>264.97000000000003</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>last</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
       <tp>
         <v>60.59</v>
         <stp/>
@@ -581,10 +725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,9 +743,10 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -628,8 +774,14 @@
       <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -644,11 +796,11 @@
         <v>17.469000000000001</v>
       </c>
       <c r="E2" s="5">
-        <f>G2/D2-1</f>
+        <f t="shared" ref="E2:E7" si="0">G2/D2-1</f>
         <v>-5.1519835136526471E-4</v>
       </c>
       <c r="F2" s="5">
-        <f>I2/$I$21</f>
+        <f t="shared" ref="F2:F7" si="1">I2/$I$21</f>
         <v>0.11367802345078762</v>
       </c>
       <c r="G2" s="4">
@@ -659,11 +811,19 @@
         <v>130</v>
       </c>
       <c r="I2" s="4">
-        <f>H2*G2</f>
+        <f t="shared" ref="I2:I7" si="2">H2*G2</f>
         <v>2269.8000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>_xll.RealtimeData(A2,"Last")</f>
+        <v>17.46</v>
+      </c>
+      <c r="K2" s="5">
+        <f>J2/D2-1</f>
+        <v>-5.1519835136526471E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -678,11 +838,11 @@
         <v>60.645000000000003</v>
       </c>
       <c r="E3" s="5">
-        <f>G3/D3-1</f>
+        <f t="shared" si="0"/>
         <v>-9.0691730563108308E-4</v>
       </c>
       <c r="F3" s="5">
-        <f>I3/$I$21</f>
+        <f t="shared" si="1"/>
         <v>0.24883056575576004</v>
       </c>
       <c r="G3" s="4">
@@ -693,11 +853,19 @@
         <v>82</v>
       </c>
       <c r="I3" s="4">
-        <f>H3*G3</f>
+        <f t="shared" si="2"/>
         <v>4968.38</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>_xll.RealtimeData(A3,"Last")</f>
+        <v>60.23</v>
+      </c>
+      <c r="K3" s="5">
+        <f t="shared" ref="K3:K7" si="3">J3/D3-1</f>
+        <v>-6.8431033061259194E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -712,11 +880,11 @@
         <v>123.8145</v>
       </c>
       <c r="E4" s="5">
-        <f>G4/D4-1</f>
+        <f t="shared" si="0"/>
         <v>-8.4400453904831529E-4</v>
       </c>
       <c r="F4" s="5">
-        <f>I4/$I$21</f>
+        <f t="shared" si="1"/>
         <v>0.27880864950628342</v>
       </c>
       <c r="G4" s="4">
@@ -727,11 +895,19 @@
         <v>45</v>
       </c>
       <c r="I4" s="4">
-        <f>H4*G4</f>
+        <f t="shared" si="2"/>
         <v>5566.95</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>_xll.RealtimeData(A4,"Last")</f>
+        <v>123.65</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" si="3"/>
+        <v>-1.3286004466358525E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -746,11 +922,11 @@
         <v>47.325000000000003</v>
       </c>
       <c r="E5" s="5">
-        <f>G5/D5-1</f>
+        <f t="shared" si="0"/>
         <v>3.1695721077662498E-4</v>
       </c>
       <c r="F5" s="5">
-        <f>I5/$I$21</f>
+        <f t="shared" si="1"/>
         <v>9.0095017158379975E-2</v>
       </c>
       <c r="G5" s="4">
@@ -761,11 +937,19 @@
         <v>38</v>
       </c>
       <c r="I5" s="4">
-        <f>H5*G5</f>
+        <f t="shared" si="2"/>
         <v>1798.92</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>_xll.RealtimeData(A5,"Last")</f>
+        <v>47.36</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" si="3"/>
+        <v>7.3956682514531025E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -780,11 +964,11 @@
         <v>266.35950000000003</v>
       </c>
       <c r="E6" s="5">
-        <f>G6/D6-1</f>
+        <f t="shared" si="0"/>
         <v>1.7664096831535581E-3</v>
       </c>
       <c r="F6" s="5">
-        <f>I6/$I$21</f>
+        <f t="shared" si="1"/>
         <v>0.17372684420030732</v>
       </c>
       <c r="G6" s="4">
@@ -795,11 +979,19 @@
         <v>13</v>
       </c>
       <c r="I6" s="4">
-        <f>H6*G6</f>
+        <f t="shared" si="2"/>
         <v>3468.79</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>_xll.RealtimeData(A6,"Last")</f>
+        <v>264.97000000000003</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="3"/>
+        <v>-5.2166339101853421E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -814,11 +1006,11 @@
         <v>40.709899999999998</v>
       </c>
       <c r="E7" s="5">
-        <f>G7/D7-1</f>
+        <f t="shared" si="0"/>
         <v>4.9373739557201368E-4</v>
       </c>
       <c r="F7" s="5">
-        <f>I7/$I$21</f>
+        <f t="shared" si="1"/>
         <v>7.3435462254569067E-2</v>
       </c>
       <c r="G7" s="4">
@@ -829,11 +1021,19 @@
         <v>36</v>
       </c>
       <c r="I7" s="4">
-        <f>H7*G7</f>
+        <f t="shared" si="2"/>
         <v>1466.28</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>_xll.RealtimeData(A7,"Last")</f>
+        <v>40.409999999999997</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="3"/>
+        <v>-7.3667584543317677E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -842,7 +1042,7 @@
         <v>ISHARES TR-MSCI EMG MKT ETF</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -851,7 +1051,7 @@
         <v>ISHARES TR-U.S. REAL ES ETF</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -860,7 +1060,7 @@
         <v>ISHARES TR-BARCLAYS 7 10 YR</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -869,8 +1069,8 @@
         <v>ISHARES TR-20 YR TR BD ETF</v>
       </c>
     </row>
-    <row r="19" spans="8:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
@@ -878,7 +1078,7 @@
         <v>427.8</v>
       </c>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
@@ -886,13 +1086,69 @@
         <f>SUM(I2:I20)</f>
         <v>19966.919999999998</v>
       </c>
-    </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="8">
+        <f>SUMPRODUCT(K2:K7,F2:F7)</f>
+        <v>-3.512384666891901E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>17</v>
       </c>
       <c r="I22">
         <v>20000</v>
+      </c>
+      <c r="J22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="8">
+        <f>_xll.RealtimeData(J22,"Change in Percent")</f>
+        <v>-4.1718815185648314E-3</v>
+      </c>
+      <c r="L22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="8">
+        <f>_xll.RealtimeData(J23,"Change in Percent")</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="8">
+        <f>_xll.RealtimeData(J24,"Change in Percent")</f>
+        <v>-6.9707304276129369E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="8">
+        <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
+        <v>-2.5031289111388986E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="6">
+        <f>SUM(I2:I18)</f>
+        <v>19539.12</v>
       </c>
     </row>
   </sheetData>
@@ -901,4 +1157,108 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>43220</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>20000</v>
+      </c>
+      <c r="D2" s="4">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>43221</v>
+      </c>
+      <c r="B3" s="4">
+        <v>19539.12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>427.8</v>
+      </c>
+      <c r="D3" s="4">
+        <f>B3+C3</f>
+        <v>19966.919999999998</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3/D2-1</f>
+        <v>-1.6540000000000443E-3</v>
+      </c>
+      <c r="F3" s="10">
+        <f>F2*(1+E3)</f>
+        <v>0.99834599999999996</v>
+      </c>
+      <c r="G3" s="5">
+        <f>F3/$F$2-1</f>
+        <v>-1.6540000000000443E-3</v>
+      </c>
+      <c r="H3" s="8">
+        <f>F3/$F$2-1</f>
+        <v>-1.6540000000000443E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new column names and orders, 1Yr,3Yr,5Yr risk and returns
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Symbol</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Realtime +/-</t>
   </si>
   <si>
-    <t>PnL</t>
-  </si>
-  <si>
     <t>AGG</t>
   </si>
   <si>
@@ -133,6 +130,63 @@
   </si>
   <si>
     <t>YTD</t>
+  </si>
+  <si>
+    <t>Total PnL</t>
+  </si>
+  <si>
+    <t>Daily Pnl</t>
+  </si>
+  <si>
+    <t>Daily Change</t>
+  </si>
+  <si>
+    <t>NAV_ACWI</t>
+  </si>
+  <si>
+    <t>NAV_AGG</t>
+  </si>
+  <si>
+    <t>NAV_SPY</t>
+  </si>
+  <si>
+    <t>ACWI_Daily</t>
+  </si>
+  <si>
+    <t>AGG_Daily</t>
+  </si>
+  <si>
+    <t>SPY_Daily</t>
+  </si>
+  <si>
+    <t>60/40Index</t>
+  </si>
+  <si>
+    <t>NAV_6040</t>
+  </si>
+  <si>
+    <t>MTD_ACWI</t>
+  </si>
+  <si>
+    <t>MTD_AGG</t>
+  </si>
+  <si>
+    <t>MTD_SPY</t>
+  </si>
+  <si>
+    <t>MTD_60/40</t>
+  </si>
+  <si>
+    <t>YTD_ACWI</t>
+  </si>
+  <si>
+    <t>YTD_AGG</t>
+  </si>
+  <si>
+    <t>YTD_SPY</t>
+  </si>
+  <si>
+    <t>YTD_60/40</t>
   </si>
 </sst>
 </file>
@@ -195,7 +249,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -219,6 +273,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -241,7 +297,245 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>-3.1500572737685967E-3</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>change in percent</stp>
+        <tr r="L2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>6.712494945410416E-3</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>change in percent</stp>
+        <tr r="L4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>1.9873190120184916E-3</v>
+        <stp/>
+        <stp>AGG</stp>
+        <stp>change in percent</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>-6.842619745845482E-3</v>
+        <stp/>
+        <stp>ACWI</stp>
+        <stp>change in percent</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>-2.1583928274945211E-3</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>change in percent</stp>
+        <tr r="L3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>-1.4780405405405469E-3</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>change in percent</stp>
+        <tr r="L5" s="1"/>
+      </tp>
+      <tp>
+        <v>-9.7746914745066599E-3</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>change in percent</stp>
+        <tr r="K24" s="1"/>
+        <tr r="L6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>-1.6085127443701485E-3</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>change in percent</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>POWERSHARES DB CMDTY IDX TRA-UNIT BEN INT</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>description</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>47.29</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>last</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES TR-MSCI EMG MKT ETF</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>description</stp>
+        <tr r="B8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES INC-MSCI JPN ETF NEW</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>description</stp>
+        <tr r="B3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>40.409999999999997</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>close</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>SPDR GOLD TRUST-GOLD SHS</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>description</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>17.405000000000001</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>last</stp>
+        <tr r="J2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>124.48</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>last</stp>
+        <tr r="J4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>47.36</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>close</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+      <tp>
+        <v>264.97000000000003</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>close</stp>
+        <tr r="G6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES TR-EUROPE ETF</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>description</stp>
+        <tr r="B5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>description</stp>
+        <tr r="B10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>description</stp>
+        <tr r="B6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES TR-U.S. REAL ES ETF</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>description</stp>
+        <tr r="B9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>60.23</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>close</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp t="s">
+        <v>ISHARES TR-20 YR TR BD ETF</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>description</stp>
+        <tr r="B11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>60.1</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>last</stp>
+        <tr r="J3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>40.344999999999999</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>last</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>262.38</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>last</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
       <tp t="s">
         <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
         <stp/>
@@ -250,212 +544,22 @@
         <tr r="B7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>ISHARES TR-20 YR TR BD ETF</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>description</stp>
-        <tr r="B11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>ISHARES TR-MSCI EMG MKT ETF</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>description</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>ISHARES INC-MSCI JPN ETF NEW</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>description</stp>
-        <tr r="B3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>POWERSHARES DB CMDTY IDX TRA-UNIT BEN INT</v>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+      <tp>
+        <v>17.46</v>
         <stp/>
         <stp>DBC</stp>
-        <stp>description</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>SPDR GOLD TRUST-GOLD SHS</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>description</stp>
-        <tr r="B4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>ISHARES TR-EUROPE ETF</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>description</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>description</stp>
-        <tr r="B10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp t="s">
-        <v>ISHARES TR-U.S. REAL ES ETF</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>description</stp>
-        <tr r="B9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>description</stp>
-        <tr r="B6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>AGG</stp>
-        <stp>change in percent</stp>
-        <tr r="K23" s="1"/>
-      </tp>
-      <tp>
-        <v>-4.1718815185648314E-3</v>
-        <stp/>
-        <stp>ACWI</stp>
-        <stp>change in percent</stp>
-        <tr r="K22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>-6.9707304276129369E-3</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>change in percent</stp>
-        <tr r="K24" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
+        <stp>close</stp>
+        <tr r="G2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
       <tp>
         <v>123.65</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>last</stp>
-        <tr r="J4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>47.34</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>close</stp>
-        <tr r="G5" s="1"/>
-      </tp>
-      <tp>
-        <v>266.83</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>close</stp>
-        <tr r="G6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>47.36</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>last</stp>
-        <tr r="J5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>40.729999999999997</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>close</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>17.46</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>last</stp>
-        <tr r="J2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>123.71</v>
         <stp/>
         <stp>GLD</stp>
         <stp>close</stp>
         <tr r="G4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>17.46</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>close</stp>
-        <tr r="G2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>60.23</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>last</stp>
-        <tr r="J3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>40.409999999999997</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>last</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>264.97000000000003</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>last</stp>
-        <tr r="J6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.3b81a987f74b4eea988e6d2f004204c2">
-      <tp>
-        <v>60.59</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>close</stp>
-        <tr r="G3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -726,10 +830,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,9 +848,10 @@
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -780,8 +885,11 @@
       <c r="K1" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -801,7 +909,7 @@
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F7" si="1">I2/$I$21</f>
-        <v>0.11367802345078762</v>
+        <v>0.1140616771257543</v>
       </c>
       <c r="G2" s="4">
         <f>_xll.RealtimeData(A2,"Close")</f>
@@ -816,14 +924,18 @@
       </c>
       <c r="J2">
         <f>_xll.RealtimeData(A2,"Last")</f>
-        <v>17.46</v>
+        <v>17.405000000000001</v>
       </c>
       <c r="K2" s="5">
         <f>J2/D2-1</f>
-        <v>-5.1519835136526471E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-3.6636327208197095E-3</v>
+      </c>
+      <c r="L2" s="8">
+        <f>_xll.RealtimeData(A2,"Change in Percent")</f>
+        <v>-3.1500572737685967E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -839,33 +951,37 @@
       </c>
       <c r="E3" s="5">
         <f t="shared" si="0"/>
-        <v>-9.0691730563108308E-4</v>
+        <v>-6.8431033061259194E-3</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="1"/>
-        <v>0.24883056575576004</v>
+        <v>0.24818691280698862</v>
       </c>
       <c r="G3" s="4">
         <f>_xll.RealtimeData(A3,"Close")</f>
-        <v>60.59</v>
+        <v>60.23</v>
       </c>
       <c r="H3" s="4">
         <v>82</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" si="2"/>
-        <v>4968.38</v>
+        <v>4938.8599999999997</v>
       </c>
       <c r="J3">
         <f>_xll.RealtimeData(A3,"Last")</f>
-        <v>60.23</v>
+        <v>60.1</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K7" si="3">J3/D3-1</f>
-        <v>-6.8431033061259194E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <f>J3/D3-1</f>
+        <v>-8.9867260285266815E-3</v>
+      </c>
+      <c r="L3" s="8">
+        <f>_xll.RealtimeData(A3,"Change in Percent")</f>
+        <v>-2.1583928274945211E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -881,33 +997,37 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>-8.4400453904831529E-4</v>
+        <v>-1.3286004466358525E-3</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>0.27880864950628342</v>
+        <v>0.27961392499206023</v>
       </c>
       <c r="G4" s="4">
         <f>_xll.RealtimeData(A4,"Close")</f>
-        <v>123.71</v>
+        <v>123.65</v>
       </c>
       <c r="H4" s="4">
         <v>45</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="2"/>
-        <v>5566.95</v>
+        <v>5564.25</v>
       </c>
       <c r="J4">
         <f>_xll.RealtimeData(A4,"Last")</f>
-        <v>123.65</v>
+        <v>124.48</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" si="3"/>
-        <v>-1.3286004466358525E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" ref="K4:K7" si="3">J4/D4-1</f>
+        <v>5.3749762749921715E-3</v>
+      </c>
+      <c r="L4" s="8">
+        <f>_xll.RealtimeData(A4,"Change in Percent")</f>
+        <v>6.712494945410416E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -923,33 +1043,37 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>3.1695721077662498E-4</v>
+        <v>7.3956682514531025E-4</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="1"/>
-        <v>9.0095017158379975E-2</v>
+        <v>9.0437271605285696E-2</v>
       </c>
       <c r="G5" s="4">
         <f>_xll.RealtimeData(A5,"Close")</f>
-        <v>47.34</v>
+        <v>47.36</v>
       </c>
       <c r="H5" s="4">
         <v>38</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="2"/>
-        <v>1798.92</v>
+        <v>1799.68</v>
       </c>
       <c r="J5">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>47.36</v>
+        <v>47.29</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="3"/>
-        <v>7.3956682514531025E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-7.3956682514531025E-4</v>
+      </c>
+      <c r="L5" s="8">
+        <f>_xll.RealtimeData(A5,"Change in Percent")</f>
+        <v>-1.4780405405405469E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -965,33 +1089,37 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>1.7664096831535581E-3</v>
+        <v>-5.2166339101853421E-3</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>0.17372684420030732</v>
+        <v>0.17309806751438211</v>
       </c>
       <c r="G6" s="4">
         <f>_xll.RealtimeData(A6,"Close")</f>
-        <v>266.83</v>
+        <v>264.97000000000003</v>
       </c>
       <c r="H6" s="4">
         <v>13</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="2"/>
-        <v>3468.79</v>
+        <v>3444.6100000000006</v>
       </c>
       <c r="J6">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>264.97000000000003</v>
+        <v>262.38</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="3"/>
-        <v>-5.2166339101853421E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-1.4940334397684496E-2</v>
+      </c>
+      <c r="L6" s="8">
+        <f>_xll.RealtimeData(A6,"Change in Percent")</f>
+        <v>-9.7746914745066599E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1007,33 +1135,37 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>4.9373739557201368E-4</v>
+        <v>-7.3667584543317677E-3</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="1"/>
-        <v>7.3435462254569067E-2</v>
+        <v>7.3104399249036167E-2</v>
       </c>
       <c r="G7" s="4">
         <f>_xll.RealtimeData(A7,"Close")</f>
-        <v>40.729999999999997</v>
+        <v>40.409999999999997</v>
       </c>
       <c r="H7" s="4">
         <v>36</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="2"/>
-        <v>1466.28</v>
+        <v>1454.7599999999998</v>
       </c>
       <c r="J7">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>40.409999999999997</v>
+        <v>40.344999999999999</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="3"/>
-        <v>-7.3667584543317677E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>-8.9634216738434525E-3</v>
+      </c>
+      <c r="L7" s="8">
+        <f>_xll.RealtimeData(A7,"Change in Percent")</f>
+        <v>-1.6085127443701485E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1042,7 +1174,7 @@
         <v>ISHARES TR-MSCI EMG MKT ETF</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1051,7 +1183,7 @@
         <v>ISHARES TR-U.S. REAL ES ETF</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1192,7 @@
         <v>ISHARES TR-BARCLAYS 7 10 YR</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1069,8 +1201,8 @@
         <v>ISHARES TR-20 YR TR BD ETF</v>
       </c>
     </row>
-    <row r="19" spans="8:12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1078,23 +1210,30 @@
         <v>427.8</v>
       </c>
     </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="6">
         <f>SUM(I2:I20)</f>
-        <v>19966.919999999998</v>
+        <v>19899.759999999998</v>
       </c>
       <c r="J21" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="K21" s="8">
         <f>SUMPRODUCT(K2:K7,F2:F7)</f>
-        <v>-3.512384666891901E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.25">
+        <v>-4.4536426435578457E-3</v>
+      </c>
+      <c r="M21" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="8">
+        <f t="array" ref="N21">SUMPRODUCT(F2:F7,L2:L7)</f>
+        <v>-9.6131812644976436E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>17</v>
       </c>
@@ -1102,53 +1241,53 @@
         <v>20000</v>
       </c>
       <c r="J22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K22" s="8">
         <f>_xll.RealtimeData(J22,"Change in Percent")</f>
-        <v>-4.1718815185648314E-3</v>
+        <v>-6.842619745845482E-3</v>
       </c>
       <c r="L22">
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K23" s="8">
         <f>_xll.RealtimeData(J23,"Change in Percent")</f>
-        <v>0</v>
+        <v>1.9873190120184916E-3</v>
       </c>
       <c r="L23">
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="8">
         <f>_xll.RealtimeData(J24,"Change in Percent")</f>
-        <v>-6.9707304276129369E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.25">
+        <v>-9.7746914745066599E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K25" s="8">
         <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
-        <v>-2.5031289111388986E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="8:12" x14ac:dyDescent="0.25">
+        <v>-3.310644242699892E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I26" s="6">
         <f>SUM(I2:I18)</f>
-        <v>19539.12</v>
+        <v>19471.96</v>
       </c>
     </row>
   </sheetData>
@@ -1162,10 +1301,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,35 +1312,85 @@
     <col min="1" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>43220</v>
       </c>
@@ -1215,19 +1404,67 @@
         <v>20000</v>
       </c>
       <c r="E2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="10">
         <v>1</v>
       </c>
       <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="H2" s="4">
+      <c r="P2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>43221</v>
       </c>
@@ -1257,6 +1494,768 @@
         <f>F3/$F$2-1</f>
         <v>-1.6540000000000443E-3</v>
       </c>
+      <c r="J3" s="11">
+        <v>-1.1100000000000001E-3</v>
+      </c>
+      <c r="K3" s="11">
+        <v>-8.4999999999999995E-4</v>
+      </c>
+      <c r="L3" s="11">
+        <v>1.7700000000000001E-3</v>
+      </c>
+      <c r="M3" s="11">
+        <f>0.6*J3 + 0.4*K3</f>
+        <v>-1.0059999999999999E-3</v>
+      </c>
+      <c r="O3" s="10">
+        <f>O2*(1+J3)</f>
+        <v>0.99888999999999994</v>
+      </c>
+      <c r="P3" s="10">
+        <f>P2*(1+K3)</f>
+        <v>0.99914999999999998</v>
+      </c>
+      <c r="Q3" s="10">
+        <f>Q2*(1+L3)</f>
+        <v>1.00177</v>
+      </c>
+      <c r="R3" s="10">
+        <f>R2*(1+M3)</f>
+        <v>0.99899400000000005</v>
+      </c>
+      <c r="T3" s="5">
+        <f>O3/$O$2-1</f>
+        <v>-1.1100000000000554E-3</v>
+      </c>
+      <c r="U3" s="5">
+        <f t="shared" ref="U3:W3" si="0">P3/$O$2-1</f>
+        <v>-8.5000000000001741E-4</v>
+      </c>
+      <c r="V3" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7700000000000493E-3</v>
+      </c>
+      <c r="W3" s="5">
+        <f t="shared" si="0"/>
+        <v>-1.0059999999999514E-3</v>
+      </c>
+      <c r="Y3" s="8">
+        <f>O3/$O$2-1</f>
+        <v>-1.1100000000000554E-3</v>
+      </c>
+      <c r="Z3" s="8">
+        <f t="shared" ref="Z3:AB3" si="1">P3/$O$2-1</f>
+        <v>-8.5000000000001741E-4</v>
+      </c>
+      <c r="AA3" s="8">
+        <f t="shared" si="1"/>
+        <v>1.7700000000000493E-3</v>
+      </c>
+      <c r="AB3" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.0059999999999514E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>43222</v>
+      </c>
+      <c r="B4" s="4">
+        <v>19471.96</v>
+      </c>
+      <c r="C4" s="4">
+        <v>427.7</v>
+      </c>
+      <c r="D4" s="4">
+        <f>B4+C4</f>
+        <v>19899.66</v>
+      </c>
+      <c r="E4" s="5">
+        <f>D4/D3-1</f>
+        <v>-3.368571617455185E-3</v>
+      </c>
+      <c r="F4" s="10">
+        <f>F3*(1+E4)</f>
+        <v>0.99498300000000006</v>
+      </c>
+      <c r="G4" s="5">
+        <f>F4/$F$2-1</f>
+        <v>-5.0169999999999382E-3</v>
+      </c>
+      <c r="H4" s="8">
+        <f>F4/$F$2-1</f>
+        <v>-5.0169999999999382E-3</v>
+      </c>
+      <c r="J4" s="11">
+        <v>-4.1700000000000001E-3</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>-6.7000000000000002E-3</v>
+      </c>
+      <c r="M4" s="11">
+        <f t="shared" ref="M4" si="2">0.6*J4 + 0.4*K4</f>
+        <v>-2.5019999999999999E-3</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" ref="O4" si="3">O3*(1+J4)</f>
+        <v>0.99472462869999989</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" ref="P4" si="4">P3*(1+K4)</f>
+        <v>0.99914999999999998</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" ref="Q4" si="5">Q3*(1+L4)</f>
+        <v>0.99505814100000001</v>
+      </c>
+      <c r="R4" s="10">
+        <f t="shared" ref="R4" si="6">R3*(1+M4)</f>
+        <v>0.99649451701200009</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" ref="T4" si="7">O4/$O$2-1</f>
+        <v>-5.275371300000109E-3</v>
+      </c>
+      <c r="U4" s="5">
+        <f t="shared" ref="U4" si="8">P4/$O$2-1</f>
+        <v>-8.5000000000001741E-4</v>
+      </c>
+      <c r="V4" s="5">
+        <f t="shared" ref="V4" si="9">Q4/$O$2-1</f>
+        <v>-4.9418589999999929E-3</v>
+      </c>
+      <c r="W4" s="5">
+        <f t="shared" ref="W4" si="10">R4/$O$2-1</f>
+        <v>-3.5054829879999083E-3</v>
+      </c>
+      <c r="Y4" s="8">
+        <f>O4/$O$2-1</f>
+        <v>-5.275371300000109E-3</v>
+      </c>
+      <c r="Z4" s="8">
+        <f t="shared" ref="Z4" si="11">P4/$O$2-1</f>
+        <v>-8.5000000000001741E-4</v>
+      </c>
+      <c r="AA4" s="8">
+        <f t="shared" ref="AA4" si="12">Q4/$O$2-1</f>
+        <v>-4.9418589999999929E-3</v>
+      </c>
+      <c r="AB4" s="8">
+        <f t="shared" ref="AB4" si="13">R4/$O$2-1</f>
+        <v>-3.5054829879999083E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="8"/>
+      <c r="M5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="8"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="8"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="8"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="8"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="8"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="8"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="8"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="8"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="8"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="8"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="8"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="8"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="8"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="8"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="8"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="8"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="8"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="8"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="8"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correlation Analysis added 05082018
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
     <sheet name="Daily" sheetId="2" r:id="rId2"/>
+    <sheet name="Prices" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Symbol</t>
   </si>
@@ -105,9 +106,6 @@
     <t>ACWI</t>
   </si>
   <si>
-    <t>60/40</t>
-  </si>
-  <si>
     <t>Market Value</t>
   </si>
   <si>
@@ -187,6 +185,36 @@
   </si>
   <si>
     <t>YTD_60/40</t>
+  </si>
+  <si>
+    <t>GYLD_Daily</t>
+  </si>
+  <si>
+    <t>NAV_GYLD</t>
+  </si>
+  <si>
+    <t>MTD_GYLD</t>
+  </si>
+  <si>
+    <t>YTD_GLYD</t>
+  </si>
+  <si>
+    <t>GYLD</t>
+  </si>
+  <si>
+    <t>60/40 ACWI/AGG</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>ACWI/AGG</t>
+  </si>
+  <si>
+    <t>SPY</t>
+  </si>
+  <si>
+    <t>Daily</t>
   </si>
 </sst>
 </file>
@@ -235,12 +263,252 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -249,7 +517,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,7 +542,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -297,78 +608,162 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>-3.1500572737685967E-3</v>
+        <v>0</v>
+        <stp/>
+        <stp>GYLD</stp>
+        <stp>change in percent</stp>
+        <tr r="K26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>ACWI</stp>
+        <stp>change in percent</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>268.79000000000002</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>last</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+      <tp>
+        <v>60.8</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>last</stp>
+        <tr r="J3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>40.520000000000003</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>last</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>124.57</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>last</stp>
+        <tr r="J4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>47.66</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>last</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp t="s">
+        <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
+        <stp/>
+        <stp>GYLD</stp>
+        <stp>description</stp>
+        <tr r="L26" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>17.68</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>last</stp>
+        <tr r="J2" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>change in percent</stp>
+        <tr r="L3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>DBC</stp>
         <stp>change in percent</stp>
         <tr r="L2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>6.712494945410416E-3</v>
+        <v>0</v>
+        <stp/>
+        <stp>AGG</stp>
+        <stp>change in percent</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>GLD</stp>
         <stp>change in percent</stp>
         <tr r="L4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>1.9873190120184916E-3</v>
+        <v>0</v>
         <stp/>
-        <stp>AGG</stp>
+        <stp>RWX</stp>
         <stp>change in percent</stp>
-        <tr r="K23" s="1"/>
+        <tr r="L7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>-6.842619745845482E-3</v>
-        <stp/>
-        <stp>ACWI</stp>
-        <stp>change in percent</stp>
-        <tr r="K22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>-2.1583928274945211E-3</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>change in percent</stp>
-        <tr r="L3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>-1.4780405405405469E-3</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>change in percent</stp>
-        <tr r="L5" s="1"/>
-      </tp>
-      <tp>
-        <v>-9.7746914745066599E-3</v>
+        <v>0</v>
         <stp/>
         <stp>IVV</stp>
         <stp>change in percent</stp>
         <tr r="K24" s="1"/>
         <tr r="L6" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
       <tp>
-        <v>-1.6085127443701485E-3</v>
+        <v>0</v>
         <stp/>
-        <stp>RWX</stp>
+        <stp>IEV</stp>
         <stp>change in percent</stp>
-        <tr r="L7" s="1"/>
+        <tr r="L5" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp t="s">
+        <v>ISHARES INC-MSCI JPN ETF NEW</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>description</stp>
+        <tr r="B3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-MSCI EMG MKT ETF</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>description</stp>
+        <tr r="B8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp t="s">
         <v>POWERSHARES DB CMDTY IDX TRA-UNIT BEN INT</v>
         <stp/>
@@ -377,43 +772,7 @@
         <tr r="B2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>47.29</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>last</stp>
-        <tr r="J5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp t="s">
-        <v>ISHARES TR-MSCI EMG MKT ETF</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>description</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp t="s">
-        <v>ISHARES INC-MSCI JPN ETF NEW</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>description</stp>
-        <tr r="B3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>40.409999999999997</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>close</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp t="s">
         <v>SPDR GOLD TRUST-GOLD SHS</v>
         <stp/>
@@ -422,41 +781,37 @@
         <tr r="B4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>17.405000000000001</v>
+        <v>268.79000000000002</v>
         <stp/>
-        <stp>DBC</stp>
-        <stp>last</stp>
-        <tr r="J2" s="1"/>
+        <stp>IVV</stp>
+        <stp>close</stp>
+        <tr r="G6" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
       <tp>
-        <v>124.48</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>last</stp>
-        <tr r="J4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>47.36</v>
+        <v>47.66</v>
         <stp/>
         <stp>IEV</stp>
         <stp>close</stp>
         <tr r="G5" s="1"/>
       </tp>
-      <tp>
-        <v>264.97000000000003</v>
+    </main>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp t="s">
+        <v>ISHARES TR-U.S. REAL ES ETF</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>description</stp>
+        <tr r="B9" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
         <stp/>
         <stp>IVV</stp>
-        <stp>close</stp>
-        <tr r="G6" s="1"/>
+        <stp>description</stp>
+        <tr r="B6" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
       <tp t="s">
         <v>ISHARES TR-EUROPE ETF</v>
         <stp/>
@@ -472,34 +827,41 @@
         <tr r="B10" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp t="s">
-        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>40.520000000000003</v>
         <stp/>
-        <stp>IVV</stp>
-        <stp>description</stp>
-        <tr r="B6" s="1"/>
+        <stp>RWX</stp>
+        <stp>close</stp>
+        <tr r="G7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp t="s">
-        <v>ISHARES TR-U.S. REAL ES ETF</v>
+        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
         <stp/>
-        <stp>IYR</stp>
+        <stp>RWX</stp>
         <stp>description</stp>
-        <tr r="B9" s="1"/>
+        <tr r="B7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>60.23</v>
+        <v>17.68</v>
         <stp/>
-        <stp>EWJ</stp>
+        <stp>DBC</stp>
         <stp>close</stp>
-        <tr r="G3" s="1"/>
+        <tr r="G2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
+      <tp>
+        <v>124.57</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>close</stp>
+        <tr r="G4" s="1"/>
+      </tp>
       <tp t="s">
         <v>ISHARES TR-20 YR TR BD ETF</v>
         <stp/>
@@ -508,58 +870,13 @@
         <tr r="B11" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
+    <main first="rtdsrv.fa54dbfa7d1a43488c694bd2669a0ba1">
       <tp>
-        <v>60.1</v>
+        <v>60.8</v>
         <stp/>
         <stp>EWJ</stp>
-        <stp>last</stp>
-        <tr r="J3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>40.344999999999999</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>last</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>262.38</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>last</stp>
-        <tr r="J6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp t="s">
-        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>description</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>17.46</v>
-        <stp/>
-        <stp>DBC</stp>
         <stp>close</stp>
-        <tr r="G2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.cf9b9f1097d041b2af10a25271d9a27e">
-      <tp>
-        <v>123.65</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>close</stp>
-        <tr r="G4" s="1"/>
+        <tr r="G3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -830,10 +1147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,6 +1164,7 @@
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -886,7 +1204,7 @@
         <v>23</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -905,34 +1223,34 @@
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E7" si="0">G2/D2-1</f>
-        <v>-5.1519835136526471E-4</v>
+        <v>1.2078539126452403E-2</v>
       </c>
       <c r="F2" s="5">
-        <f t="shared" ref="F2:F7" si="1">I2/$I$21</f>
-        <v>0.1140616771257543</v>
+        <f>I2/$I$21</f>
+        <v>0.11445405753178808</v>
       </c>
       <c r="G2" s="4">
         <f>_xll.RealtimeData(A2,"Close")</f>
-        <v>17.46</v>
+        <v>17.68</v>
       </c>
       <c r="H2" s="4">
         <v>130</v>
       </c>
       <c r="I2" s="4">
-        <f t="shared" ref="I2:I7" si="2">H2*G2</f>
-        <v>2269.8000000000002</v>
+        <f t="shared" ref="I2:I7" si="1">H2*G2</f>
+        <v>2298.4</v>
       </c>
       <c r="J2">
         <f>_xll.RealtimeData(A2,"Last")</f>
-        <v>17.405000000000001</v>
+        <v>17.68</v>
       </c>
       <c r="K2" s="5">
         <f>J2/D2-1</f>
-        <v>-3.6636327208197095E-3</v>
+        <v>1.2078539126452403E-2</v>
       </c>
       <c r="L2" s="8">
         <f>_xll.RealtimeData(A2,"Change in Percent")</f>
-        <v>-3.1500572737685967E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -951,34 +1269,34 @@
       </c>
       <c r="E3" s="5">
         <f t="shared" si="0"/>
-        <v>-6.8431033061259194E-3</v>
+        <v>2.5558578613240623E-3</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" si="1"/>
-        <v>0.24818691280698862</v>
+        <f t="shared" ref="F3:F7" si="2">I3/$I$21</f>
+        <v>0.24826929569721659</v>
       </c>
       <c r="G3" s="4">
         <f>_xll.RealtimeData(A3,"Close")</f>
-        <v>60.23</v>
+        <v>60.8</v>
       </c>
       <c r="H3" s="4">
         <v>82</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" si="2"/>
-        <v>4938.8599999999997</v>
+        <f t="shared" si="1"/>
+        <v>4985.5999999999995</v>
       </c>
       <c r="J3">
         <f>_xll.RealtimeData(A3,"Last")</f>
-        <v>60.1</v>
+        <v>60.8</v>
       </c>
       <c r="K3" s="5">
         <f>J3/D3-1</f>
-        <v>-8.9867260285266815E-3</v>
+        <v>2.5558578613240623E-3</v>
       </c>
       <c r="L3" s="8">
         <f>_xll.RealtimeData(A3,"Change in Percent")</f>
-        <v>-2.1583928274945211E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -997,34 +1315,34 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>-1.3286004466358525E-3</v>
+        <v>6.1018701363733108E-3</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="1"/>
-        <v>0.27961392499206023</v>
+        <f t="shared" si="2"/>
+        <v>0.27914609624219799</v>
       </c>
       <c r="G4" s="4">
         <f>_xll.RealtimeData(A4,"Close")</f>
-        <v>123.65</v>
+        <v>124.57</v>
       </c>
       <c r="H4" s="4">
         <v>45</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="2"/>
-        <v>5564.25</v>
+        <f t="shared" si="1"/>
+        <v>5605.65</v>
       </c>
       <c r="J4">
         <f>_xll.RealtimeData(A4,"Last")</f>
-        <v>124.48</v>
+        <v>124.57</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K7" si="3">J4/D4-1</f>
-        <v>5.3749762749921715E-3</v>
+        <v>6.1018701363733108E-3</v>
       </c>
       <c r="L4" s="8">
         <f>_xll.RealtimeData(A4,"Change in Percent")</f>
-        <v>6.712494945410416E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1043,34 +1361,34 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>7.3956682514531025E-4</v>
+        <v>7.0787110406760334E-3</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="1"/>
-        <v>9.0437271605285696E-2</v>
+        <f t="shared" si="2"/>
+        <v>9.0186849336351696E-2</v>
       </c>
       <c r="G5" s="4">
         <f>_xll.RealtimeData(A5,"Close")</f>
-        <v>47.36</v>
+        <v>47.66</v>
       </c>
       <c r="H5" s="4">
         <v>38</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="2"/>
-        <v>1799.68</v>
+        <f t="shared" si="1"/>
+        <v>1811.08</v>
       </c>
       <c r="J5">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>47.29</v>
+        <v>47.66</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="3"/>
-        <v>-7.3956682514531025E-4</v>
+        <v>7.0787110406760334E-3</v>
       </c>
       <c r="L5" s="8">
         <f>_xll.RealtimeData(A5,"Change in Percent")</f>
-        <v>-1.4780405405405469E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1089,34 +1407,34 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>-5.2166339101853421E-3</v>
+        <v>9.1248857277477224E-3</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="1"/>
-        <v>0.17309806751438211</v>
+        <f t="shared" si="2"/>
+        <v>0.17400512513557309</v>
       </c>
       <c r="G6" s="4">
         <f>_xll.RealtimeData(A6,"Close")</f>
-        <v>264.97000000000003</v>
+        <v>268.79000000000002</v>
       </c>
       <c r="H6" s="4">
         <v>13</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="2"/>
-        <v>3444.6100000000006</v>
+        <f t="shared" si="1"/>
+        <v>3494.2700000000004</v>
       </c>
       <c r="J6">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>262.38</v>
+        <v>268.79000000000002</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="3"/>
-        <v>-1.4940334397684496E-2</v>
+        <v>9.1248857277477224E-3</v>
       </c>
       <c r="L6" s="8">
         <f>_xll.RealtimeData(A6,"Change in Percent")</f>
-        <v>-9.7746914745066599E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1135,34 +1453,34 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>-7.3667584543317677E-3</v>
+        <v>-4.6647130059271902E-3</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="1"/>
-        <v>7.3104399249036167E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.2640281414362129E-2</v>
       </c>
       <c r="G7" s="4">
         <f>_xll.RealtimeData(A7,"Close")</f>
-        <v>40.409999999999997</v>
+        <v>40.520000000000003</v>
       </c>
       <c r="H7" s="4">
         <v>36</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
-        <v>1454.7599999999998</v>
+        <f t="shared" si="1"/>
+        <v>1458.72</v>
       </c>
       <c r="J7">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>40.344999999999999</v>
+        <v>40.520000000000003</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="3"/>
-        <v>-8.9634216738434525E-3</v>
+        <v>-4.6647130059271902E-3</v>
       </c>
       <c r="L7" s="8">
         <f>_xll.RealtimeData(A7,"Change in Percent")</f>
-        <v>-1.6085127443701485E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1207,7 +1525,7 @@
         <v>14</v>
       </c>
       <c r="I20" s="6">
-        <v>427.8</v>
+        <v>427.7</v>
       </c>
     </row>
     <row r="21" spans="8:14" x14ac:dyDescent="0.25">
@@ -1216,21 +1534,21 @@
       </c>
       <c r="I21" s="6">
         <f>SUM(I2:I20)</f>
-        <v>19899.759999999998</v>
+        <v>20081.420000000002</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" s="8">
         <f>SUMPRODUCT(K2:K7,F2:F7)</f>
-        <v>-4.4536426435578457E-3</v>
+        <v>5.6076295351152935E-3</v>
       </c>
       <c r="M21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N21" s="8">
         <f t="array" ref="N21">SUMPRODUCT(F2:F7,L2:L7)</f>
-        <v>-9.6131812644976436E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="8:14" x14ac:dyDescent="0.25">
@@ -1245,9 +1563,9 @@
       </c>
       <c r="K22" s="8">
         <f>_xll.RealtimeData(J22,"Change in Percent")</f>
-        <v>-6.842619745845482E-3</v>
-      </c>
-      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
         <v>0.6</v>
       </c>
     </row>
@@ -1257,9 +1575,9 @@
       </c>
       <c r="K23" s="8">
         <f>_xll.RealtimeData(J23,"Change in Percent")</f>
-        <v>1.9873190120184916E-3</v>
-      </c>
-      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
         <v>0.4</v>
       </c>
     </row>
@@ -1269,25 +1587,122 @@
       </c>
       <c r="K24" s="8">
         <f>_xll.RealtimeData(J24,"Change in Percent")</f>
-        <v>-9.7746914745066599E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="K25" s="8">
         <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
-        <v>-3.310644242699892E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I26" s="6">
         <f>SUM(I2:I18)</f>
-        <v>19471.96</v>
+        <v>19653.72</v>
+      </c>
+      <c r="J26" t="s">
+        <v>57</v>
+      </c>
+      <c r="K26" s="8">
+        <f>_xll.RealtimeData(J26,"Change in Percent")</f>
+        <v>0</v>
+      </c>
+      <c r="L26" t="str">
+        <f>_xll.RealtimeData(J26,"Description")</f>
+        <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
+      </c>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="29" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="29">
+        <v>43227</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="21">
+        <f>$N$21</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="22">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,7,0)</f>
+        <v>4.0815000000000712E-3</v>
+      </c>
+      <c r="K31" s="23">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,8,0)</f>
+        <v>4.0815000000000712E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H32" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="24">
+        <f>$K$25</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="14">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,25,0)</f>
+        <v>3.1160437189563517E-3</v>
+      </c>
+      <c r="K32" s="25">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,31,0)</f>
+        <v>3.1160437189563517E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I33" s="24">
+        <f>$K$24</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,24,0)</f>
+        <v>9.403621992640776E-3</v>
+      </c>
+      <c r="K33" s="25">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,30,0)</f>
+        <v>9.403621992640776E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="26">
+        <f>$K$26</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="27">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,26,0)</f>
+        <v>1.9466513843773292E-3</v>
+      </c>
+      <c r="K34" s="28">
+        <f>VLOOKUP($H$30,Daily!$A:$AF,32,0)</f>
+        <v>1.9466513843773292E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1301,10 +1716,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AB50"/>
+  <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,85 +1727,108 @@
     <col min="1" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>51</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>43220</v>
       </c>
@@ -1427,23 +1865,27 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>1</v>
+      <c r="N2">
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <f>P2</f>
+        <v>100</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <f t="shared" ref="R2:T2" si="0">Q2</f>
+        <v>100</v>
+      </c>
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -1451,20 +1893,32 @@
       <c r="W2">
         <v>0</v>
       </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>43221</v>
       </c>
@@ -1507,56 +1961,71 @@
         <f>0.6*J3 + 0.4*K3</f>
         <v>-1.0059999999999999E-3</v>
       </c>
-      <c r="O3" s="10">
-        <f>O2*(1+J3)</f>
-        <v>0.99888999999999994</v>
+      <c r="N3" s="11">
+        <v>-7.4799999999999997E-3</v>
       </c>
       <c r="P3" s="10">
-        <f>P2*(1+K3)</f>
-        <v>0.99914999999999998</v>
+        <f>P2*(1+J3)</f>
+        <v>99.888999999999996</v>
       </c>
       <c r="Q3" s="10">
-        <f>Q2*(1+L3)</f>
-        <v>1.00177</v>
+        <f>Q2*(1+K3)</f>
+        <v>99.914999999999992</v>
       </c>
       <c r="R3" s="10">
-        <f>R2*(1+M3)</f>
-        <v>0.99899400000000005</v>
-      </c>
-      <c r="T3" s="5">
-        <f>O3/$O$2-1</f>
+        <f>R2*(1+L3)</f>
+        <v>100.17700000000001</v>
+      </c>
+      <c r="S3" s="10">
+        <f>S2*(1+M3)</f>
+        <v>99.8994</v>
+      </c>
+      <c r="T3" s="10">
+        <f>T2*(1+N3)</f>
+        <v>99.251999999999995</v>
+      </c>
+      <c r="V3" s="5">
+        <f>P3/$P$2-1</f>
         <v>-1.1100000000000554E-3</v>
       </c>
-      <c r="U3" s="5">
-        <f t="shared" ref="U3:W3" si="0">P3/$O$2-1</f>
-        <v>-8.5000000000001741E-4</v>
-      </c>
-      <c r="V3" s="5">
-        <f t="shared" si="0"/>
+      <c r="W3" s="5">
+        <f>Q3/$Q$2-1</f>
+        <v>-8.5000000000012843E-4</v>
+      </c>
+      <c r="X3" s="5">
+        <f>R3/$R$2-1</f>
         <v>1.7700000000000493E-3</v>
       </c>
-      <c r="W3" s="5">
-        <f t="shared" si="0"/>
+      <c r="Y3" s="5">
+        <f>S3/$S$2-1</f>
         <v>-1.0059999999999514E-3</v>
       </c>
-      <c r="Y3" s="8">
-        <f>O3/$O$2-1</f>
+      <c r="Z3" s="5">
+        <f>T3/$T$2-1</f>
+        <v>-7.4800000000000422E-3</v>
+      </c>
+      <c r="AB3" s="8">
+        <f>P3/$P$2-1</f>
         <v>-1.1100000000000554E-3</v>
       </c>
-      <c r="Z3" s="8">
-        <f t="shared" ref="Z3:AB3" si="1">P3/$O$2-1</f>
-        <v>-8.5000000000001741E-4</v>
-      </c>
-      <c r="AA3" s="8">
+      <c r="AC3" s="8">
+        <f t="shared" ref="AC3:AE3" si="1">Q3/$P$2-1</f>
+        <v>-8.5000000000012843E-4</v>
+      </c>
+      <c r="AD3" s="8">
         <f t="shared" si="1"/>
         <v>1.7700000000000493E-3</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AE3" s="8">
         <f t="shared" si="1"/>
         <v>-1.0059999999999514E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF3" s="8">
+        <f>T3/$T$2-1</f>
+        <v>-7.4800000000000422E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>43222</v>
       </c>
@@ -1589,121 +2058,411 @@
       <c r="J4" s="11">
         <v>-4.1700000000000001E-3</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>0</v>
       </c>
       <c r="L4" s="11">
         <v>-6.7000000000000002E-3</v>
       </c>
       <c r="M4" s="11">
-        <f t="shared" ref="M4" si="2">0.6*J4 + 0.4*K4</f>
+        <f t="shared" ref="M4:M7" si="2">0.6*J4 + 0.4*K4</f>
         <v>-2.5019999999999999E-3</v>
       </c>
-      <c r="O4" s="10">
-        <f t="shared" ref="O4" si="3">O3*(1+J4)</f>
-        <v>0.99472462869999989</v>
+      <c r="N4" s="11">
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="P4" s="10">
-        <f t="shared" ref="P4" si="4">P3*(1+K4)</f>
-        <v>0.99914999999999998</v>
+        <f t="shared" ref="P4" si="3">P3*(1+J4)</f>
+        <v>99.472462870000001</v>
       </c>
       <c r="Q4" s="10">
-        <f t="shared" ref="Q4" si="5">Q3*(1+L4)</f>
-        <v>0.99505814100000001</v>
+        <f t="shared" ref="Q4" si="4">Q3*(1+K4)</f>
+        <v>99.914999999999992</v>
       </c>
       <c r="R4" s="10">
-        <f t="shared" ref="R4" si="6">R3*(1+M4)</f>
-        <v>0.99649451701200009</v>
-      </c>
-      <c r="T4" s="5">
-        <f t="shared" ref="T4" si="7">O4/$O$2-1</f>
-        <v>-5.275371300000109E-3</v>
-      </c>
-      <c r="U4" s="5">
-        <f t="shared" ref="U4" si="8">P4/$O$2-1</f>
-        <v>-8.5000000000001741E-4</v>
+        <f t="shared" ref="R4" si="5">R3*(1+L4)</f>
+        <v>99.505814100000009</v>
+      </c>
+      <c r="S4" s="10">
+        <f t="shared" ref="S4" si="6">S3*(1+M4)</f>
+        <v>99.649451701199993</v>
+      </c>
+      <c r="T4" s="10">
+        <f>T3*(1+N4)</f>
+        <v>100.57205160000001</v>
       </c>
       <c r="V4" s="5">
-        <f t="shared" ref="V4" si="9">Q4/$O$2-1</f>
-        <v>-4.9418589999999929E-3</v>
+        <f>P4/$P$2-1</f>
+        <v>-5.275371299999998E-3</v>
       </c>
       <c r="W4" s="5">
-        <f t="shared" ref="W4" si="10">R4/$O$2-1</f>
-        <v>-3.5054829879999083E-3</v>
-      </c>
-      <c r="Y4" s="8">
-        <f>O4/$O$2-1</f>
-        <v>-5.275371300000109E-3</v>
-      </c>
-      <c r="Z4" s="8">
-        <f t="shared" ref="Z4" si="11">P4/$O$2-1</f>
-        <v>-8.5000000000001741E-4</v>
-      </c>
-      <c r="AA4" s="8">
-        <f t="shared" ref="AA4" si="12">Q4/$O$2-1</f>
-        <v>-4.9418589999999929E-3</v>
+        <f>Q4/$Q$2-1</f>
+        <v>-8.5000000000012843E-4</v>
+      </c>
+      <c r="X4" s="5">
+        <f>R4/$R$2-1</f>
+        <v>-4.9418589999998819E-3</v>
+      </c>
+      <c r="Y4" s="5">
+        <f>S4/$S$2-1</f>
+        <v>-3.5054829880000193E-3</v>
+      </c>
+      <c r="Z4" s="5">
+        <f>T4/$T$2-1</f>
+        <v>5.7205160000000088E-3</v>
       </c>
       <c r="AB4" s="8">
-        <f t="shared" ref="AB4" si="13">R4/$O$2-1</f>
-        <v>-3.5054829879999083E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="8"/>
-      <c r="M5" s="11"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+        <f>P4/$P$2-1</f>
+        <v>-5.275371299999998E-3</v>
+      </c>
+      <c r="AC4" s="8">
+        <f t="shared" ref="AC4" si="7">Q4/$P$2-1</f>
+        <v>-8.5000000000012843E-4</v>
+      </c>
+      <c r="AD4" s="8">
+        <f t="shared" ref="AD4" si="8">R4/$P$2-1</f>
+        <v>-4.9418589999998819E-3</v>
+      </c>
+      <c r="AE4" s="8">
+        <f t="shared" ref="AE4" si="9">S4/$P$2-1</f>
+        <v>-3.5054829880000193E-3</v>
+      </c>
+      <c r="AF4" s="8">
+        <f>T4/$T$2-1</f>
+        <v>5.7205160000000088E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>43223</v>
+      </c>
+      <c r="B5" s="4">
+        <v>19525.419999999998</v>
+      </c>
+      <c r="C5" s="4">
+        <v>427.9</v>
+      </c>
+      <c r="D5" s="4">
+        <v>19953.32</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5/D4-1</f>
+        <v>2.6965284834012948E-3</v>
+      </c>
+      <c r="F5" s="10">
+        <f>F4*(1+E5)</f>
+        <v>0.99766600000000016</v>
+      </c>
+      <c r="G5" s="5">
+        <f>F5/$F$2-1</f>
+        <v>-2.3339999999998362E-3</v>
+      </c>
+      <c r="H5" s="8">
+        <f>F5/$F$2-1</f>
+        <v>-2.3339999999998362E-3</v>
+      </c>
+      <c r="J5" s="11">
+        <f>VLOOKUP($A5,Prices!$A:$J,MATCH(J$1,Prices!$1:$1,0),0)</f>
+        <v>1.3964530093568683E-4</v>
+      </c>
+      <c r="K5" s="11">
+        <f>VLOOKUP($A5,Prices!$A:$J,MATCH(K$1,Prices!$1:$1,0),0)</f>
+        <v>1.1356108640105944E-3</v>
+      </c>
+      <c r="L5" s="11">
+        <f>VLOOKUP($A5,Prices!$A:$J,MATCH(L$1,Prices!$1:$1,0),0)</f>
+        <v>-2.1511869268221462E-3</v>
+      </c>
+      <c r="M5" s="11">
+        <f t="shared" si="2"/>
+        <v>5.3803152616564991E-4</v>
+      </c>
+      <c r="N5" s="11">
+        <f>VLOOKUP($A5,Prices!$A:$J,MATCH(N$1,Prices!$1:$1,0),0)</f>
+        <v>-1.9220303056343258E-2</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" ref="P5" si="10">P4*(1+J5)</f>
+        <v>99.48635373201229</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" ref="Q5" si="11">Q4*(1+K5)</f>
+        <v>100.02846455947761</v>
+      </c>
+      <c r="R5" s="10">
+        <f t="shared" ref="R5" si="12">R4*(1+L5)</f>
+        <v>99.291758493565297</v>
+      </c>
+      <c r="S5" s="10">
+        <f t="shared" ref="S5" si="13">S4*(1+M5)</f>
+        <v>99.703066247780356</v>
+      </c>
+      <c r="T5" s="10">
+        <f>T4*(1+N5)</f>
+        <v>98.639026289249813</v>
+      </c>
+      <c r="V5" s="5">
+        <f>P5/$P$2-1</f>
+        <v>-5.1364626798771074E-3</v>
+      </c>
+      <c r="W5" s="5">
+        <f>Q5/$Q$2-1</f>
+        <v>2.8464559477603402E-4</v>
+      </c>
+      <c r="X5" s="5">
+        <f>R5/$R$2-1</f>
+        <v>-7.0824150643470363E-3</v>
+      </c>
+      <c r="Y5" s="5">
+        <f>S5/$S$2-1</f>
+        <v>-2.9693375221964136E-3</v>
+      </c>
+      <c r="Z5" s="5">
+        <f>T5/$T$2-1</f>
+        <v>-1.3609737107501907E-2</v>
+      </c>
+      <c r="AB5" s="8">
+        <f>P5/$P$2-1</f>
+        <v>-5.1364626798771074E-3</v>
+      </c>
+      <c r="AC5" s="8">
+        <f t="shared" ref="AC5" si="14">Q5/$P$2-1</f>
+        <v>2.8464559477603402E-4</v>
+      </c>
+      <c r="AD5" s="8">
+        <f t="shared" ref="AD5" si="15">R5/$P$2-1</f>
+        <v>-7.0824150643470363E-3</v>
+      </c>
+      <c r="AE5" s="8">
+        <f t="shared" ref="AE5" si="16">S5/$P$2-1</f>
+        <v>-2.9693375221964136E-3</v>
+      </c>
+      <c r="AF5" s="8">
+        <f>T5/$T$2-1</f>
+        <v>-1.3609737107501907E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>43224</v>
+      </c>
+      <c r="B6" s="4">
+        <v>19634.889999999996</v>
+      </c>
+      <c r="C6" s="4">
+        <v>427.9</v>
+      </c>
+      <c r="D6" s="4">
+        <v>20062.789999999997</v>
+      </c>
+      <c r="E6" s="5">
+        <f>D6/D5-1</f>
+        <v>5.4863050359537091E-3</v>
+      </c>
+      <c r="F6" s="10">
+        <f>F5*(1+E6)</f>
+        <v>1.0031394999999999</v>
+      </c>
+      <c r="G6" s="5">
+        <f>F6/$F$2-1</f>
+        <v>3.1394999999998507E-3</v>
+      </c>
+      <c r="H6" s="8">
+        <f>F6/$F$2-1</f>
+        <v>3.1394999999998507E-3</v>
+      </c>
+      <c r="J6" s="11">
+        <f>VLOOKUP($A6,Prices!$A:$J,MATCH(J$1,Prices!$1:$1,0),0)</f>
+        <v>8.3775481709018607E-3</v>
+      </c>
+      <c r="K6" s="11">
+        <f>VLOOKUP($A6,Prices!$A:$J,MATCH(K$1,Prices!$1:$1,0),0)</f>
+        <v>6.6168825030721301E-4</v>
+      </c>
+      <c r="L6" s="11">
+        <f>VLOOKUP($A6,Prices!$A:$J,MATCH(L$1,Prices!$1:$1,0),0)</f>
+        <v>1.2934947049924483E-2</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" si="2"/>
+        <v>5.2912042026640018E-3</v>
+      </c>
+      <c r="N6" s="11">
+        <f>VLOOKUP($A6,Prices!$A:$J,MATCH(N$1,Prices!$1:$1,0),0)</f>
+        <v>3.9193925233644844E-3</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" ref="P6" si="17">P5*(1+J6)</f>
+        <v>100.31980545274961</v>
+      </c>
+      <c r="Q6" s="10">
+        <f t="shared" ref="Q6" si="18">Q5*(1+K6)</f>
+        <v>100.09465221917289</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" ref="R6" si="19">R5*(1+L6)</f>
+        <v>100.57609213217346</v>
+      </c>
+      <c r="S6" s="10">
+        <f t="shared" ref="S6" si="20">S5*(1+M6)</f>
+        <v>100.2306155309291</v>
+      </c>
+      <c r="T6" s="10">
+        <f>T5*(1+N6)</f>
+        <v>99.025631351399852</v>
+      </c>
+      <c r="V6" s="5">
+        <f>P6/$P$2-1</f>
+        <v>3.1980545274961081E-3</v>
+      </c>
+      <c r="W6" s="5">
+        <f>Q6/$Q$2-1</f>
+        <v>9.4652219172886021E-4</v>
+      </c>
+      <c r="X6" s="5">
+        <f>R6/$R$2-1</f>
+        <v>5.7609213217346689E-3</v>
+      </c>
+      <c r="Y6" s="5">
+        <f>S6/$S$2-1</f>
+        <v>2.3061553092909026E-3</v>
+      </c>
+      <c r="Z6" s="5">
+        <f>T6/$T$2-1</f>
+        <v>-9.7436864860014349E-3</v>
+      </c>
+      <c r="AB6" s="8">
+        <f>P6/$P$2-1</f>
+        <v>3.1980545274961081E-3</v>
+      </c>
+      <c r="AC6" s="8">
+        <f t="shared" ref="AC6" si="21">Q6/$P$2-1</f>
+        <v>9.4652219172886021E-4</v>
+      </c>
+      <c r="AD6" s="8">
+        <f t="shared" ref="AD6" si="22">R6/$P$2-1</f>
+        <v>5.7609213217346689E-3</v>
+      </c>
+      <c r="AE6" s="8">
+        <f t="shared" ref="AE6" si="23">S6/$P$2-1</f>
+        <v>2.3061553092909026E-3</v>
+      </c>
+      <c r="AF6" s="8">
+        <f>T6/$T$2-1</f>
+        <v>-9.7436864860014349E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>43227</v>
+      </c>
+      <c r="B7" s="4">
+        <v>19653.72</v>
+      </c>
+      <c r="C7" s="4">
+        <v>427.7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>20081.63</v>
+      </c>
+      <c r="E7" s="5">
+        <f>D7/D6-1</f>
+        <v>9.3905184672737896E-4</v>
+      </c>
+      <c r="F7" s="10">
+        <f>F6*(1+E7)</f>
+        <v>1.0040815000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <f>F7/$F$2-1</f>
+        <v>4.0815000000000712E-3</v>
+      </c>
+      <c r="H7" s="8">
+        <f>F7/$F$2-1</f>
+        <v>4.0815000000000712E-3</v>
+      </c>
+      <c r="J7" s="11">
+        <f>VLOOKUP($A7,Prices!$A:$J,MATCH(J$1,Prices!$1:$1,0),0)</f>
+        <v>1.6615895873719477E-3</v>
+      </c>
+      <c r="K7" s="11">
+        <f>VLOOKUP($A7,Prices!$A:$J,MATCH(K$1,Prices!$1:$1,0),0)</f>
+        <v>-4.7232193463064842E-4</v>
+      </c>
+      <c r="L7" s="11">
+        <f>VLOOKUP($A7,Prices!$A:$J,MATCH(L$1,Prices!$1:$1,0),0)</f>
+        <v>3.6218355611978836E-3</v>
+      </c>
+      <c r="M7" s="11">
+        <f t="shared" si="2"/>
+        <v>8.0802497857090916E-4</v>
+      </c>
+      <c r="N7" s="11">
+        <f>VLOOKUP($A7,Prices!$A:$J,MATCH(N$1,Prices!$1:$1,0),0)</f>
+        <v>1.180536565214596E-2</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" ref="P7" si="24">P6*(1+J7)</f>
+        <v>100.48649579689707</v>
+      </c>
+      <c r="Q7" s="10">
+        <f t="shared" ref="Q7" si="25">Q6*(1+K7)</f>
+        <v>100.04737531939054</v>
+      </c>
+      <c r="R7" s="10">
+        <f t="shared" ref="R7" si="26">R6*(1+L7)</f>
+        <v>100.94036219926407</v>
+      </c>
+      <c r="S7" s="10">
+        <f t="shared" ref="S7" si="27">S6*(1+M7)</f>
+        <v>100.31160437189563</v>
+      </c>
+      <c r="T7" s="10">
+        <f>T6*(1+N7)</f>
+        <v>100.19466513843774</v>
+      </c>
+      <c r="V7" s="5">
+        <f>P7/$P$2-1</f>
+        <v>4.8649579689707956E-3</v>
+      </c>
+      <c r="W7" s="5">
+        <f>Q7/$Q$2-1</f>
+        <v>4.7375319390541293E-4</v>
+      </c>
+      <c r="X7" s="5">
+        <f>R7/$R$2-1</f>
+        <v>9.403621992640776E-3</v>
+      </c>
+      <c r="Y7" s="5">
+        <f>S7/$S$2-1</f>
+        <v>3.1160437189563517E-3</v>
+      </c>
+      <c r="Z7" s="5">
+        <f>T7/$T$2-1</f>
+        <v>1.9466513843773292E-3</v>
+      </c>
+      <c r="AB7" s="8">
+        <f>P7/$P$2-1</f>
+        <v>4.8649579689707956E-3</v>
+      </c>
+      <c r="AC7" s="8">
+        <f t="shared" ref="AC7" si="28">Q7/$P$2-1</f>
+        <v>4.7375319390541293E-4</v>
+      </c>
+      <c r="AD7" s="8">
+        <f t="shared" ref="AD7" si="29">R7/$P$2-1</f>
+        <v>9.403621992640776E-3</v>
+      </c>
+      <c r="AE7" s="8">
+        <f t="shared" ref="AE7" si="30">S7/$P$2-1</f>
+        <v>3.1160437189563517E-3</v>
+      </c>
+      <c r="AF7" s="8">
+        <f>T7/$T$2-1</f>
+        <v>1.9466513843773292E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1712,16 +2471,22 @@
       <c r="F8" s="10"/>
       <c r="G8" s="5"/>
       <c r="H8" s="8"/>
-      <c r="O8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
+      <c r="S8" s="10"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1730,16 +2495,22 @@
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
       <c r="H9" s="8"/>
-      <c r="O9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
+      <c r="S9" s="10"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1748,16 +2519,22 @@
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
       <c r="H10" s="8"/>
-      <c r="O10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
+      <c r="S10" s="10"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1766,16 +2543,22 @@
       <c r="F11" s="10"/>
       <c r="G11" s="5"/>
       <c r="H11" s="8"/>
-      <c r="O11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
+      <c r="S11" s="10"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1784,16 +2567,22 @@
       <c r="F12" s="10"/>
       <c r="G12" s="5"/>
       <c r="H12" s="8"/>
-      <c r="O12" s="10"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
+      <c r="S12" s="10"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1802,16 +2591,22 @@
       <c r="F13" s="10"/>
       <c r="G13" s="5"/>
       <c r="H13" s="8"/>
-      <c r="O13" s="10"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
+      <c r="S13" s="10"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1820,16 +2615,22 @@
       <c r="F14" s="10"/>
       <c r="G14" s="5"/>
       <c r="H14" s="8"/>
-      <c r="O14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
+      <c r="S14" s="10"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1838,16 +2639,22 @@
       <c r="F15" s="10"/>
       <c r="G15" s="5"/>
       <c r="H15" s="8"/>
-      <c r="O15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="S15" s="10"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1856,16 +2663,22 @@
       <c r="F16" s="10"/>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
-      <c r="O16" s="10"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="S16" s="10"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1874,15 +2687,21 @@
       <c r="F17" s="10"/>
       <c r="G17" s="5"/>
       <c r="H17" s="8"/>
-      <c r="O17" s="10"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
+      <c r="R17" s="10"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1891,15 +2710,21 @@
       <c r="F18" s="10"/>
       <c r="G18" s="5"/>
       <c r="H18" s="8"/>
-      <c r="O18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
+      <c r="R18" s="10"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1908,15 +2733,21 @@
       <c r="F19" s="10"/>
       <c r="G19" s="5"/>
       <c r="H19" s="8"/>
-      <c r="O19" s="10"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
+      <c r="R19" s="10"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1925,15 +2756,21 @@
       <c r="F20" s="10"/>
       <c r="G20" s="5"/>
       <c r="H20" s="8"/>
-      <c r="O20" s="10"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
+      <c r="R20" s="10"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1942,15 +2779,21 @@
       <c r="F21" s="10"/>
       <c r="G21" s="5"/>
       <c r="H21" s="8"/>
-      <c r="O21" s="10"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
+      <c r="R21" s="10"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1959,15 +2802,21 @@
       <c r="F22" s="10"/>
       <c r="G22" s="5"/>
       <c r="H22" s="8"/>
-      <c r="O22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
+      <c r="R22" s="10"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1976,15 +2825,21 @@
       <c r="F23" s="10"/>
       <c r="G23" s="5"/>
       <c r="H23" s="8"/>
-      <c r="O23" s="10"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
+      <c r="R23" s="10"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1993,11 +2848,16 @@
       <c r="F24" s="10"/>
       <c r="G24" s="5"/>
       <c r="H24" s="8"/>
-      <c r="O24" s="10"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2006,8 +2866,13 @@
       <c r="F25" s="10"/>
       <c r="G25" s="5"/>
       <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2016,8 +2881,13 @@
       <c r="F26" s="10"/>
       <c r="G26" s="5"/>
       <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2026,8 +2896,13 @@
       <c r="F27" s="10"/>
       <c r="G27" s="5"/>
       <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2036,8 +2911,13 @@
       <c r="F28" s="10"/>
       <c r="G28" s="5"/>
       <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2046,8 +2926,13 @@
       <c r="F29" s="10"/>
       <c r="G29" s="5"/>
       <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2056,8 +2941,13 @@
       <c r="F30" s="10"/>
       <c r="G30" s="5"/>
       <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2066,8 +2956,13 @@
       <c r="F31" s="10"/>
       <c r="G31" s="5"/>
       <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2076,6 +2971,11 @@
       <c r="F32" s="10"/>
       <c r="G32" s="5"/>
       <c r="H32" s="8"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
@@ -2260,4 +3160,270 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="10" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>43220</v>
+      </c>
+      <c r="B3">
+        <f t="array" ref="B3">_xll.HistoricalData(B$1,"Adj. Close",$A3,$A3,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>71.989999999999995</v>
+      </c>
+      <c r="C3">
+        <f t="array" ref="C3">_xll.HistoricalData(C$1,"Adj. Close",$A3,$A3,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.7599</v>
+      </c>
+      <c r="D3">
+        <f t="array" ref="D3">_xll.HistoricalData(D$1,"Adj. Close",$A3,$A3,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>266.31</v>
+      </c>
+      <c r="E3">
+        <f t="array" ref="E3">_xll.HistoricalData(E$1,"Adj. Close",$A3,$A3,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>43221</v>
+      </c>
+      <c r="B4">
+        <f t="array" ref="B4">_xll.HistoricalData(B$1,"Adj. Close",$A4,$A4,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>71.91</v>
+      </c>
+      <c r="C4">
+        <f t="array" ref="C4">_xll.HistoricalData(C$1,"Adj. Close",$A4,$A4,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.67</v>
+      </c>
+      <c r="D4">
+        <f t="array" ref="D4">_xll.HistoricalData(D$1,"Adj. Close",$A4,$A4,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>266.83</v>
+      </c>
+      <c r="E4">
+        <f t="array" ref="E4">_xll.HistoricalData(E$1,"Adj. Close",$A4,$A4,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.23</v>
+      </c>
+      <c r="G4" s="5">
+        <f>B4/B3-1</f>
+        <v>-1.1112654535352373E-3</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ref="H4:J4" si="0">C4/C3-1</f>
+        <v>-8.5003862522559093E-4</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9526116180390574E-3</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>-7.4884792626727092E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>43222</v>
+      </c>
+      <c r="B5">
+        <f t="array" ref="B5">_xll.HistoricalData(B$1,"Adj. Close",$A5,$A5,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>71.61</v>
+      </c>
+      <c r="C5">
+        <f t="array" ref="C5">_xll.HistoricalData(C$1,"Adj. Close",$A5,$A5,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.67</v>
+      </c>
+      <c r="D5">
+        <f t="array" ref="D5">_xll.HistoricalData(D$1,"Adj. Close",$A5,$A5,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>264.97000000000003</v>
+      </c>
+      <c r="E5">
+        <f t="array" ref="E5">_xll.HistoricalData(E$1,"Adj. Close",$A5,$A5,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.455500000000001</v>
+      </c>
+      <c r="G5" s="5">
+        <f>B5/B4-1</f>
+        <v>-4.1718815185648461E-3</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ref="H5" si="1">C5/C4-1</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5" si="2">D5/D4-1</f>
+        <v>-6.9707304276128701E-3</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ref="J5" si="3">E5/E4-1</f>
+        <v>1.3087637840974997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>43223</v>
+      </c>
+      <c r="B6">
+        <f t="array" ref="B6">_xll.HistoricalData(B$1,"Adj. Close",$A6,$A6,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>71.62</v>
+      </c>
+      <c r="C6">
+        <f t="array" ref="C6">_xll.HistoricalData(C$1,"Adj. Close",$A6,$A6,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.79</v>
+      </c>
+      <c r="D6">
+        <f t="array" ref="D6">_xll.HistoricalData(D$1,"Adj. Close",$A6,$A6,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>264.39999999999998</v>
+      </c>
+      <c r="E6">
+        <f t="array" ref="E6">_xll.HistoricalData(E$1,"Adj. Close",$A6,$A6,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.12</v>
+      </c>
+      <c r="G6" s="5">
+        <f>B6/B5-1</f>
+        <v>1.3964530093568683E-4</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6" si="4">C6/C5-1</f>
+        <v>1.1356108640105944E-3</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" ref="I6" si="5">D6/D5-1</f>
+        <v>-2.1511869268221462E-3</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6" si="6">E6/E5-1</f>
+        <v>-1.9220303056343258E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>43224</v>
+      </c>
+      <c r="B7">
+        <f t="array" ref="B7">_xll.HistoricalData(B$1,"Adj. Close",$A7,$A7,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>72.22</v>
+      </c>
+      <c r="C7">
+        <f t="array" ref="C7">_xll.HistoricalData(C$1,"Adj. Close",$A7,$A7,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.86</v>
+      </c>
+      <c r="D7">
+        <f t="array" ref="D7">_xll.HistoricalData(D$1,"Adj. Close",$A7,$A7,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>267.82</v>
+      </c>
+      <c r="E7">
+        <f t="array" ref="E7">_xll.HistoricalData(E$1,"Adj. Close",$A7,$A7,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.187100000000001</v>
+      </c>
+      <c r="G7" s="5">
+        <f>B7/B6-1</f>
+        <v>8.3775481709018607E-3</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" ref="H7" si="7">C7/C6-1</f>
+        <v>6.6168825030721301E-4</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" ref="I7" si="8">D7/D6-1</f>
+        <v>1.2934947049924483E-2</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" ref="J7" si="9">E7/E6-1</f>
+        <v>3.9193925233644844E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>43227</v>
+      </c>
+      <c r="B8">
+        <f t="array" ref="B8">_xll.HistoricalData(B$1,"Adj. Close",$A8,$A8,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>72.34</v>
+      </c>
+      <c r="C8">
+        <f t="array" ref="C8">_xll.HistoricalData(C$1,"Adj. Close",$A8,$A8,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.81</v>
+      </c>
+      <c r="D8">
+        <f t="array" ref="D8">_xll.HistoricalData(D$1,"Adj. Close",$A8,$A8,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>268.79000000000002</v>
+      </c>
+      <c r="E8">
+        <f t="array" ref="E8">_xll.HistoricalData(E$1,"Adj. Close",$A8,$A8,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.39</v>
+      </c>
+      <c r="G8" s="5">
+        <f>B8/B7-1</f>
+        <v>1.6615895873719477E-3</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ref="H8" si="10">C8/C7-1</f>
+        <v>-4.7232193463064842E-4</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ref="I8" si="11">D8/D7-1</f>
+        <v>3.6218355611978836E-3</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="12">E8/E7-1</f>
+        <v>1.180536565214596E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Commit for 08022018
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
   <si>
     <t>Symbol</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>Max DD (30 day)</t>
+  </si>
+  <si>
+    <t>SHY</t>
   </si>
 </sst>
 </file>
@@ -942,150 +945,27 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>-7.5490689481631599E-3</v>
+        <v>1.99</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>dividend yield</stp>
+        <tr r="M12" s="1"/>
+      </tp>
+      <tp>
+        <v>3.65</v>
         <stp/>
         <stp>RWX</stp>
-        <stp>change in percent</stp>
-        <tr r="L6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-8.9390142021721804E-3</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>change in percent</stp>
-        <tr r="L5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-7.5490830636461273E-3</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>change in percent</stp>
-        <tr r="L9" s="1"/>
+        <stp>dividend yield</stp>
+        <tr r="M6" s="1"/>
       </tp>
       <tp>
-        <v>-1.0590228748939392E-3</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>change in percent</stp>
-        <tr r="K24" s="1"/>
-        <tr r="L3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-3.8153846153846397E-3</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>change in percent</stp>
-        <tr r="L4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-9.6968345965225584E-3</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>change in percent</stp>
-        <tr r="L10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>5.1084913719459928E-3</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>change in percent</stp>
-        <tr r="L7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-4.7417880851797316E-3</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>change in percent</stp>
-        <tr r="L8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-9.4517958412092913E-4</v>
-        <stp/>
-        <stp>AGG</stp>
-        <stp>change in percent</stp>
-        <tr r="K23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-4.5195519748477894E-3</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>change in percent</stp>
-        <tr r="L11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>-1.4492753623188406E-2</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>change in percent</stp>
-        <tr r="L2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>17.25</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>close</stp>
-        <tr r="G2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>283.27999999999997</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>close</stp>
-        <tr r="G3" s="1"/>
-      </tp>
-      <tp>
-        <v>119.7</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>close</stp>
-        <tr r="G5" s="1"/>
-      </tp>
-      <tp>
-        <v>81.25</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>close</stp>
-        <tr r="G4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp t="s">
-        <v>--</v>
+        <v>2.7</v>
         <stp/>
         <stp>TLT</stp>
         <stp>dividend yield</stp>
         <tr r="M5" s="1"/>
-      </tp>
-      <tp>
-        <v>3.64</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>dividend yield</stp>
-        <tr r="M6" s="1"/>
       </tp>
       <tp>
         <v>0.49</v>
@@ -1095,25 +975,39 @@
         <tr r="M4" s="1"/>
       </tp>
       <tp>
-        <v>1.81</v>
+        <v>1.82</v>
         <stp/>
         <stp>IVV</stp>
         <stp>dividend yield</stp>
         <tr r="M3" s="1"/>
       </tp>
       <tp>
-        <v>4.59</v>
+        <v>2.36</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>dividend yield</stp>
+        <tr r="M11" s="1"/>
+      </tp>
+      <tp>
+        <v>4.66</v>
         <stp/>
         <stp>IEV</stp>
         <stp>dividend yield</stp>
         <tr r="M9" s="1"/>
       </tp>
-      <tp t="s">
-        <v>--</v>
+      <tp>
+        <v>1.58</v>
         <stp/>
-        <stp>IEF</stp>
+        <stp>EWJ</stp>
         <stp>dividend yield</stp>
-        <tr r="M11" s="1"/>
+        <tr r="M7" s="1"/>
+      </tp>
+      <tp>
+        <v>1.32</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>dividend yield</stp>
+        <tr r="M10" s="1"/>
       </tp>
       <tp t="s">
         <v>--</v>
@@ -1122,63 +1016,237 @@
         <stp>dividend yield</stp>
         <tr r="M2" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>1.56</v>
+        <v>-6.0261415718892717E-3</v>
         <stp/>
         <stp>EWJ</stp>
-        <stp>dividend yield</stp>
-        <tr r="M7" s="1"/>
+        <stp>change in percent</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>2.0655983999999998</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U4" s="1"/>
       </tp>
       <tp>
-        <v>1.3</v>
+        <v>0.73464172999999999</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U3" s="1"/>
+      </tp>
+      <tp>
+        <v>-1.34315425</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U9" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.17709563</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U11" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.69174232999999996</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U8" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.72058325000000001</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U7" s="1"/>
+      </tp>
+      <tp>
+        <v>-1.6808605999999999</v>
         <stp/>
         <stp>EEM</stp>
-        <stp>dividend yield</stp>
-        <tr r="M10" s="1"/>
+        <stp>mtd percent change</stp>
+        <tr r="U10" s="1"/>
+      </tp>
+      <tp>
+        <v>-1.2391930799999999</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U2" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.11419642000000001</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U12" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.40444893999999998</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U6" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.29399412000000003</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U5" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>-8.6797752808989888E-3</v>
+        <v>-1.32703553756186E-2</v>
         <stp/>
-        <stp>GYLD</stp>
+        <stp>EEM</stp>
         <stp>change in percent</stp>
-        <tr r="K26" s="1"/>
+        <tr r="L10" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>-2.3192360163711051E-3</v>
+        <v>-2.1875854525566997E-3</v>
         <stp/>
         <stp>ACWI</stp>
         <stp>change in percent</stp>
         <tr r="K22" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>118.63</v>
+        <v>7.2778720996037908E-3</v>
+        <stp/>
+        <stp>GYLD</stp>
+        <stp>change in percent</stp>
+        <tr r="K26" s="1"/>
+      </tp>
+      <tp>
+        <v>7.9411764705883542E-3</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>change in percent</stp>
+        <tr r="L2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>-2.5186729199236234E-3</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>change in percent</stp>
+        <tr r="L8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>1.1841326228536609E-3</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>change in percent</stp>
+        <tr r="L11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>3.074739829706613E-4</v>
+        <stp/>
+        <stp>AGG</stp>
+        <stp>change in percent</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>-2.5316455696202788E-3</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>change in percent</stp>
+        <tr r="L6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>4.2138213339750304E-4</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>change in percent</stp>
+        <tr r="L12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>1.2266928361144629E-4</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>change in percent</stp>
+        <tr r="L4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>2.0260003376667991E-3</v>
         <stp/>
         <stp>TLT</stp>
-        <stp>last</stp>
-        <tr r="J5" s="1"/>
+        <stp>change in percent</stp>
+        <tr r="L5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>-1.0000000000000023E-2</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>change in percent</stp>
+        <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>115.44</v>
+        <v>3.3936651583709701E-3</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>change in percent</stp>
+        <tr r="K24" s="1"/>
+        <tr r="L3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>114.85</v>
         <stp/>
         <stp>GLD</stp>
         <stp>last</stp>
         <tr r="J8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp t="s">
-        <v>7-10 Year Treas Bond Ishares ETF</v>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>118.7</v>
         <stp/>
-        <stp>IEF</stp>
-        <stp>description</stp>
-        <tr r="B11" s="1"/>
+        <stp>TLT</stp>
+        <stp>last</stp>
+        <tr r="J5" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>81.52</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>close</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>ISHARES TR-EUROPE ETF</v>
         <stp/>
@@ -1186,6 +1254,15 @@
         <stp>description</stp>
         <tr r="B9" s="1"/>
       </tp>
+      <tp t="s">
+        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>description</stp>
+        <tr r="B11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>ISHARES TR-U.S. REAL ES ETF</v>
         <stp/>
@@ -1201,7 +1278,59 @@
         <tr r="B3" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>83.094999999999999</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>last</stp>
+        <tr r="J12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>282.88</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>close</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>118.46</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>close</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>43.87</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>last</stp>
+        <tr r="J10" s="1"/>
+      </tp>
+      <tp>
+        <v>101.46</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>last</stp>
+        <tr r="J11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>45.54</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>last</stp>
+        <tr r="J9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
         <stp/>
@@ -1210,7 +1339,16 @@
         <tr r="L26" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp t="s">
+        <v>INVESCO DB COMMDY INDX TRCK-UNIT</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>description</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>ISHARES TR-MSCI EMG MKT ETF</v>
         <stp/>
@@ -1218,6 +1356,8 @@
         <stp>description</stp>
         <tr r="B10" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>ISHARES INC-MSCI JPN ETF NEW</v>
         <stp/>
@@ -1226,39 +1366,16 @@
         <tr r="B7" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp t="s">
-        <v>INVESCO DB COMMDY INDX TRCK-UNIT</v>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>17.135000000000002</v>
         <stp/>
         <stp>DBC</stp>
-        <stp>description</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-      <tp>
-        <v>46.000100000000003</v>
-        <stp/>
-        <stp>IEV</stp>
         <stp>last</stp>
-        <tr r="J9" s="1"/>
+        <tr r="J2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>44.424999999999997</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>last</stp>
-        <tr r="J10" s="1"/>
-      </tp>
-      <tp>
-        <v>101.32</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>last</stp>
-        <tr r="J11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp t="s">
         <v>SPDR GOLD TRUST-GOLD SHS</v>
         <stp/>
@@ -1267,63 +1384,72 @@
         <tr r="B8" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
         <v>17</v>
         <stp/>
         <stp>DBC</stp>
-        <stp>last</stp>
-        <tr r="J2" s="1"/>
+        <stp>close</stp>
+        <tr r="G2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>80.94</v>
+        <v>81.53</v>
         <stp/>
         <stp>IYR</stp>
         <stp>last</stp>
         <tr r="J4" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
       <tp>
-        <v>39.44</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>last</stp>
-        <tr r="J6" s="1"/>
-      </tp>
-      <tp>
-        <v>58.829000000000001</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>last</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp>
-        <v>282.98</v>
+        <v>283.83999999999997</v>
         <stp/>
         <stp>IVV</stp>
         <stp>last</stp>
         <tr r="J3" s="1"/>
       </tp>
       <tp t="s">
-        <v>20+ Year Treas Bond Ishares ETF</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>description</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.194ca04fd7fa411b89ccdcaf03001557">
-      <tp t="s">
         <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
         <stp/>
         <stp>RWX</stp>
         <stp>description</stp>
         <tr r="B6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>58.555</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>last</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-1 3 YR TREAS BD</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>description</stp>
+        <tr r="B12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp>
+        <v>39.4</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>last</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.8e8a415e349149ca90766c03467d8c22">
+      <tp t="s">
+        <v>ISHARES TR-20 YR TR BD ETF</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>description</stp>
+        <tr r="B5" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1594,10 +1720,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1748,7 @@
     <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1677,8 +1803,11 @@
       <c r="S1" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1694,68 +1823,72 @@
       </c>
       <c r="E2" s="5">
         <f>G2/D2-1</f>
-        <v>-3.2356918824730352E-2</v>
+        <v>-4.6380731595386471E-2</v>
       </c>
       <c r="F2" s="5">
         <f>I2/$I$21</f>
-        <v>0.15238301742466678</v>
+        <v>0.15081359701518116</v>
       </c>
       <c r="G2" s="4">
         <f>_xll.RealtimeData(A2,"Close")</f>
-        <v>17.25</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4">
         <v>176</v>
       </c>
       <c r="I2" s="4">
         <f>H2*G2</f>
-        <v>3036</v>
+        <v>2992</v>
       </c>
       <c r="J2" s="4">
         <f>_xll.RealtimeData(A2,"Last")</f>
-        <v>17</v>
+        <v>17.135000000000002</v>
       </c>
       <c r="K2" s="5">
         <f>J2/D2-1</f>
-        <v>-4.6380731595386471E-2</v>
+        <v>-3.8807872699232138E-2</v>
       </c>
       <c r="L2" s="8">
         <f>_xll.RealtimeData(A2,"Change in Percent")</f>
-        <v>-1.4492753623188406E-2</v>
+        <v>7.9411764705883542E-3</v>
       </c>
       <c r="M2" s="29" t="str">
         <f>_xll.RealtimeData(A2,"Dividend Yield")</f>
         <v>--</v>
       </c>
       <c r="N2" s="4" t="str">
-        <f t="shared" ref="N2:N11" si="0">A2</f>
+        <f t="shared" ref="N2:N12" si="0">A2</f>
         <v>DBC</v>
       </c>
       <c r="O2" s="5">
-        <v>0.189</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="P2" s="60">
-        <f t="shared" ref="P2:P11" si="1">O2-F2</f>
-        <v>3.6616982575333218E-2</v>
+        <f t="shared" ref="P2:P12" si="1">O2-F2</f>
+        <v>-8.8135970151811682E-3</v>
       </c>
       <c r="Q2" s="31">
         <f>O2*Daily!$D$66</f>
-        <v>3765.5414999999998</v>
+        <v>2829.1369999999997</v>
       </c>
       <c r="R2">
         <f t="shared" ref="R2:R11" si="2">ROUND(Q2/J2,0)</f>
-        <v>222</v>
+        <v>165</v>
       </c>
       <c r="S2">
         <f t="shared" ref="S2:S11" si="3">R2-H2</f>
-        <v>46</v>
+        <v>-11</v>
       </c>
       <c r="T2" t="str">
-        <f t="shared" ref="T2:T11" si="4">A2</f>
+        <f t="shared" ref="T2:T12" si="4">A2</f>
         <v>DBC</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <f>_xll.RealtimeData(T2,"MTD Percent Change")</f>
+        <v>-1.2391930799999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1771,68 +1904,72 @@
       </c>
       <c r="E3" s="5">
         <f>G3/D3-1</f>
-        <v>6.3525047914566368E-2</v>
+        <v>6.202331810954731E-2</v>
       </c>
       <c r="F3" s="5">
         <f>I3/$I$21</f>
-        <v>0.41233358830886968</v>
+        <v>0.413503462361624</v>
       </c>
       <c r="G3" s="4">
         <f>_xll.RealtimeData(A3,"Close")</f>
-        <v>283.27999999999997</v>
+        <v>282.88</v>
       </c>
       <c r="H3" s="4">
         <v>29</v>
       </c>
       <c r="I3" s="4">
         <f>H3*G3</f>
-        <v>8215.119999999999</v>
+        <v>8203.52</v>
       </c>
       <c r="J3" s="4">
         <f>_xll.RealtimeData(A3,"Last")</f>
-        <v>282.98</v>
+        <v>283.83999999999997</v>
       </c>
       <c r="K3" s="5">
         <f>J3/D3-1</f>
-        <v>6.239875056080213E-2</v>
+        <v>6.5627469641593272E-2</v>
       </c>
       <c r="L3" s="8">
         <f>_xll.RealtimeData(A3,"Change in Percent")</f>
-        <v>-1.0590228748939392E-3</v>
+        <v>3.3936651583709701E-3</v>
       </c>
       <c r="M3" s="29">
         <f>_xll.RealtimeData(A3,"Dividend Yield")</f>
-        <v>1.81</v>
+        <v>1.82</v>
       </c>
       <c r="N3" s="4" t="str">
         <f t="shared" si="0"/>
         <v>IVV</v>
       </c>
       <c r="O3" s="5">
-        <v>0.33600000000000002</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="P3" s="60">
         <f t="shared" si="1"/>
-        <v>-7.633358830886966E-2</v>
+        <v>-4.7503462361624005E-2</v>
       </c>
       <c r="Q3" s="31">
         <f>O3*Daily!$D$66</f>
-        <v>6694.2960000000003</v>
+        <v>7292.0010000000002</v>
       </c>
       <c r="R3">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="S3">
         <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="T3" t="str">
         <f t="shared" si="4"/>
         <v>IVV</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <f>_xll.RealtimeData(T3,"MTD Percent Change")</f>
+        <v>0.73464172999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1848,34 +1985,34 @@
       </c>
       <c r="E4" s="5">
         <f>G4/D4-1</f>
-        <v>3.5955629223511254E-2</v>
+        <v>3.9398189468315525E-2</v>
       </c>
       <c r="F4" s="5">
         <f>I4/$I$21</f>
-        <v>0.22021755235531143</v>
+        <v>0.22188954516998283</v>
       </c>
       <c r="G4" s="4">
         <f>_xll.RealtimeData(A4,"Close")</f>
-        <v>81.25</v>
+        <v>81.52</v>
       </c>
       <c r="H4" s="4">
         <v>54</v>
       </c>
       <c r="I4" s="4">
         <f>H4*G4</f>
-        <v>4387.5</v>
+        <v>4402.08</v>
       </c>
       <c r="J4" s="4">
         <f>_xll.RealtimeData(A4,"Last")</f>
-        <v>80.94</v>
+        <v>81.53</v>
       </c>
       <c r="K4" s="5">
         <f>J4/D4-1</f>
-        <v>3.2003060053550803E-2</v>
+        <v>3.9525691699604737E-2</v>
       </c>
       <c r="L4" s="8">
         <f t="array" ref="L4">_xll.RealtimeData(A4,"Change in Percent")</f>
-        <v>-3.8153846153846397E-3</v>
+        <v>1.2266928361144629E-4</v>
       </c>
       <c r="M4" s="29">
         <f>_xll.RealtimeData(A4,"Dividend Yield")</f>
@@ -1886,36 +2023,40 @@
         <v>IYR</v>
       </c>
       <c r="O4" s="5">
-        <v>0.314</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="P4" s="60">
         <f t="shared" si="1"/>
-        <v>9.3782447644688571E-2</v>
+        <v>0.17111045483001719</v>
       </c>
       <c r="Q4" s="31">
         <f>O4*Daily!$D$66</f>
-        <v>6255.9790000000003</v>
+        <v>7829.9355000000005</v>
       </c>
       <c r="R4">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="S4">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="T4" t="str">
         <f t="shared" si="4"/>
         <v>IYR</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <f>_xll.RealtimeData(T4,"MTD Percent Change")</f>
+        <v>2.0655983999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="str">
         <f>_xll.RealtimeData(A5,"Description")</f>
-        <v>20+ Year Treas Bond Ishares ETF</v>
+        <v>ISHARES TR-20 YR TR BD ETF</v>
       </c>
       <c r="C5" s="3">
         <v>43286</v>
@@ -1925,38 +2066,38 @@
       </c>
       <c r="E5" s="5">
         <f>G5/D5-1</f>
-        <v>-2.1209578899339165E-2</v>
+        <v>-3.134909537523578E-2</v>
       </c>
       <c r="F5" s="5">
         <f>I5/$I$21</f>
-        <v>0.21027952947978967</v>
+        <v>0.20898671610449282</v>
       </c>
       <c r="G5" s="4">
         <f>_xll.RealtimeData(A5,"Close")</f>
-        <v>119.7</v>
+        <v>118.46</v>
       </c>
       <c r="H5" s="4">
         <v>35</v>
       </c>
       <c r="I5" s="4">
         <f>H5*G5</f>
-        <v>4189.5</v>
+        <v>4146.0999999999995</v>
       </c>
       <c r="J5" s="31">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>118.63</v>
+        <v>118.7</v>
       </c>
       <c r="K5" s="5">
         <f>J5/D5-1</f>
-        <v>-2.9959000374508049E-2</v>
+        <v>-2.9386608315384755E-2</v>
       </c>
       <c r="L5" s="8">
         <f t="array" ref="L5">_xll.RealtimeData(A5,"Change in Percent")</f>
-        <v>-8.9390142021721804E-3</v>
-      </c>
-      <c r="M5" s="29" t="str">
+        <v>2.0260003376667991E-3</v>
+      </c>
+      <c r="M5" s="29">
         <f>_xll.RealtimeData(A5,"Dividend Yield")</f>
-        <v>--</v>
+        <v>2.7</v>
       </c>
       <c r="N5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1967,7 +2108,7 @@
       </c>
       <c r="P5" s="60">
         <f t="shared" si="1"/>
-        <v>-0.21027952947978967</v>
+        <v>-0.20898671610449282</v>
       </c>
       <c r="Q5" s="31">
         <f>O5*Daily!$D$66</f>
@@ -1985,8 +2126,12 @@
         <f t="shared" si="4"/>
         <v>TLT</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <f>_xll.RealtimeData(T5,"MTD Percent Change")</f>
+        <v>-0.29399412000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2003,16 +2148,16 @@
       <c r="I6" s="4"/>
       <c r="J6" s="31">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>39.44</v>
+        <v>39.4</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="8">
         <f>_xll.RealtimeData(A6,"Change in Percent")</f>
-        <v>-7.5490689481631599E-3</v>
+        <v>-2.5316455696202788E-3</v>
       </c>
       <c r="M6" s="29">
         <f>_xll.RealtimeData(A6,"Dividend Yield")</f>
-        <v>3.64</v>
+        <v>3.65</v>
       </c>
       <c r="N6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2041,8 +2186,12 @@
         <f t="shared" si="4"/>
         <v>RWX</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <f>_xll.RealtimeData(T6,"MTD Percent Change")</f>
+        <v>-0.40444893999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2059,16 +2208,16 @@
       <c r="I7" s="4"/>
       <c r="J7" s="31">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>58.829000000000001</v>
+        <v>58.555</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="8">
         <f>_xll.RealtimeData(A7,"Change in Percent")</f>
-        <v>5.1084913719459928E-3</v>
+        <v>-6.0261415718892717E-3</v>
       </c>
       <c r="M7" s="29">
         <f>_xll.RealtimeData(A7,"Dividend Yield")</f>
-        <v>1.56</v>
+        <v>1.58</v>
       </c>
       <c r="N7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2097,8 +2246,12 @@
         <f t="shared" si="4"/>
         <v>EWJ</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <f>_xll.RealtimeData(T7,"MTD Percent Change")</f>
+        <v>-0.72058325000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2115,12 +2268,12 @@
       <c r="I8" s="4"/>
       <c r="J8" s="31">
         <f>_xll.RealtimeData(A8,"Last")</f>
-        <v>115.44</v>
+        <v>114.85</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="8">
         <f>_xll.RealtimeData(A8,"Change in Percent")</f>
-        <v>-4.7417880851797316E-3</v>
+        <v>-2.5186729199236234E-3</v>
       </c>
       <c r="M8" s="29">
         <v>0</v>
@@ -2152,8 +2305,12 @@
         <f t="shared" si="4"/>
         <v>GLD</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <f>_xll.RealtimeData(T8,"MTD Percent Change")</f>
+        <v>-0.69174232999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2170,46 +2327,50 @@
       <c r="I9" s="4"/>
       <c r="J9" s="31">
         <f>_xll.RealtimeData(A9,"Last")</f>
-        <v>46.000100000000003</v>
+        <v>45.54</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="8">
         <f>_xll.RealtimeData(A9,"Change in Percent")</f>
-        <v>-7.5490830636461273E-3</v>
+        <v>-1.0000000000000023E-2</v>
       </c>
       <c r="M9" s="29">
         <f>_xll.RealtimeData(A9,"Dividend Yield")</f>
-        <v>4.59</v>
+        <v>4.66</v>
       </c>
       <c r="N9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>IEV</v>
       </c>
       <c r="O9" s="5">
-        <v>0.161</v>
+        <v>0</v>
       </c>
       <c r="P9" s="60">
         <f t="shared" si="1"/>
-        <v>0.161</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="31">
         <f>O9*Daily!$D$66</f>
-        <v>3207.6835000000001</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="4"/>
         <v>IEV</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <f>_xll.RealtimeData(T9,"MTD Percent Change")</f>
+        <v>-1.34315425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2220,16 +2381,16 @@
       <c r="G10" s="4"/>
       <c r="J10" s="31">
         <f>_xll.RealtimeData(A10,"Last")</f>
-        <v>44.424999999999997</v>
+        <v>43.87</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="8">
         <f t="array" ref="L10">_xll.RealtimeData(A10,"Change in Percent")</f>
-        <v>-9.6968345965225584E-3</v>
+        <v>-1.32703553756186E-2</v>
       </c>
       <c r="M10" s="29">
         <f>_xll.RealtimeData(A10,"Dividend Yield")</f>
-        <v>1.3</v>
+        <v>1.32</v>
       </c>
       <c r="N10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2258,28 +2419,32 @@
         <f t="shared" si="4"/>
         <v>EEM</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <f>_xll.RealtimeData(T10,"MTD Percent Change")</f>
+        <v>-1.6808605999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="str">
         <f>_xll.RealtimeData(A11,"Description")</f>
-        <v>7-10 Year Treas Bond Ishares ETF</v>
+        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
       </c>
       <c r="G11" s="4"/>
       <c r="J11" s="31">
         <f>_xll.RealtimeData(A11,"Last")</f>
-        <v>101.32</v>
+        <v>101.46</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="8">
         <f t="array" ref="L11">_xll.RealtimeData(A11,"Change in Percent")</f>
-        <v>-4.5195519748477894E-3</v>
-      </c>
-      <c r="M11" s="29" t="str">
+        <v>1.1841326228536609E-3</v>
+      </c>
+      <c r="M11" s="29">
         <f>_xll.RealtimeData(A11,"Dividend Yield")</f>
-        <v>--</v>
+        <v>2.36</v>
       </c>
       <c r="N11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2308,29 +2473,92 @@
         <f t="shared" si="4"/>
         <v>IEF</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="J12" s="31" t="str">
+      <c r="U11">
+        <f>_xll.RealtimeData(T11,"MTD Percent Change")</f>
+        <v>-0.17709563</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xll.RealtimeData(A12,"Description")</f>
+        <v>ISHARES TR-1 3 YR TREAS BD</v>
+      </c>
+      <c r="J12" s="31">
         <f>_xll.RealtimeData(A12,"Last")</f>
-        <v>--</v>
-      </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>83.094999999999999</v>
+      </c>
+      <c r="L12" s="8">
+        <f t="array" ref="L12">_xll.RealtimeData(A12,"Change in Percent")</f>
+        <v>4.2138213339750304E-4</v>
+      </c>
+      <c r="M12" s="29">
+        <f>_xll.RealtimeData(A12,"Dividend Yield")</f>
+        <v>1.99</v>
+      </c>
+      <c r="N12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>SHY</v>
+      </c>
+      <c r="O12" s="5">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="P12" s="60">
+        <f t="shared" si="1"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="Q12" s="31">
+        <f>O12*Daily!$D$66</f>
+        <v>1972.4265</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12" si="5">ROUND(Q12/J12,0)</f>
+        <v>24</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ref="S12" si="6">R12-H12</f>
+        <v>24</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="4"/>
+        <v>SHY</v>
+      </c>
+      <c r="U12">
+        <f>_xll.RealtimeData(T12,"MTD Percent Change")</f>
+        <v>-0.11419642000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" s="31" t="str">
         <f>_xll.RealtimeData(A13,"Last")</f>
         <v>--</v>
       </c>
+      <c r="L13" s="8" t="str">
+        <f t="array" ref="L13">_xll.RealtimeData(A13,"Change in Percent")</f>
+        <v>--</v>
+      </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="19" spans="5:15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U14" s="29">
+        <f t="array" ref="U14">MMULT(TRANSPOSE(O2:O12),U2:U12)</f>
+        <v>0.89338818143999998</v>
+      </c>
+      <c r="V14" s="8">
+        <f>U14*0.01</f>
+        <v>8.9338818144E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="5:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>70</v>
       </c>
       <c r="F20" s="11">
         <f>SUM(F2:F5)</f>
-        <v>0.99521368756863748</v>
+        <v>0.99519332065128085</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>14</v>
@@ -2339,41 +2567,45 @@
         <v>95.36</v>
       </c>
       <c r="O20" s="11">
-        <f>SUM(O2:O11)</f>
+        <f>SUM(O2:O12)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>71</v>
       </c>
       <c r="F21" s="11">
         <f>1-F20</f>
-        <v>4.7863124313625161E-3</v>
+        <v>4.806679348719145E-3</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="6">
         <f>SUM(I2:I20)</f>
-        <v>19923.48</v>
+        <v>19839.060000000001</v>
       </c>
       <c r="J21" t="s">
         <v>33</v>
       </c>
       <c r="K21" s="8">
         <f>SUMPRODUCT(K2:K7,F2:F7)</f>
-        <v>1.9409335944293671E-2</v>
+        <v>2.3913358033025755E-2</v>
       </c>
       <c r="M21" t="s">
         <v>34</v>
       </c>
       <c r="N21" s="8">
         <f t="array" ref="N21">MMULT(TRANSPOSE(F2:F5),L2:L5)</f>
-        <v>-5.3650265917399549E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+        <v>3.0515558700866053E-3</v>
+      </c>
+      <c r="P21" s="8">
+        <f t="array" ref="P21">SUMPRODUCT(L2:L12,O2:O12)</f>
+        <v>2.4596543664529721E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>17</v>
       </c>
@@ -2385,91 +2617,91 @@
       </c>
       <c r="K22" s="8">
         <f>_xll.RealtimeData(J22,"Change in Percent")</f>
-        <v>-2.3192360163711051E-3</v>
+        <v>-2.1875854525566997E-3</v>
       </c>
       <c r="L22" s="12">
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="8">
         <f>_xll.RealtimeData(J23,"Change in Percent")</f>
-        <v>-9.4517958412092913E-4</v>
+        <v>3.074739829706613E-4</v>
       </c>
       <c r="L23" s="12">
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="8">
         <f>_xll.RealtimeData(J24,"Change in Percent")</f>
-        <v>-1.0590228748939392E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+        <v>3.3936651583709701E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
         <v>57</v>
       </c>
       <c r="K25" s="8">
         <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
-        <v>-1.7696134434710348E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+        <v>-1.1895616783457552E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="6">
         <f>SUM(I2:I18)</f>
-        <v>19828.12</v>
+        <v>19743.7</v>
       </c>
       <c r="J26" t="s">
         <v>56</v>
       </c>
       <c r="K26" s="8">
         <f>_xll.RealtimeData(J26,"Change in Percent")</f>
-        <v>-8.6797752808989888E-3</v>
+        <v>7.2778720996037908E-3</v>
       </c>
       <c r="L26" t="str">
         <f>_xll.RealtimeData(J26,"Description")</f>
         <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>62</v>
       </c>
       <c r="K27" s="8">
         <f>AVERAGE(L2:L11)</f>
-        <v>-5.7254010612052533E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+        <v>-1.9679171563960567E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="5:16" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>64</v>
       </c>
       <c r="K28" s="8">
         <f>SUMPRODUCT(F2:F7,M2:M7)*0.01</f>
-        <v>8.5423039549315672E-3</v>
+        <v>1.425566312113578E-2</v>
       </c>
       <c r="L28" t="s">
         <v>65</v>
       </c>
       <c r="M28" s="8">
         <f>AVERAGE(M2:M11)*0.01</f>
-        <v>1.9128571428571432E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0644444444444444E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H30" s="30">
-        <v>43312</v>
+        <v>43313</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>61</v>
@@ -2484,46 +2716,46 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H31" s="18" t="s">
         <v>58</v>
       </c>
       <c r="I31" s="21">
         <f>$N$21</f>
-        <v>-5.3650265917399549E-3</v>
+        <v>3.0515558700866053E-3</v>
       </c>
       <c r="J31" s="21">
         <f>LOOKUP(2,1/(Daily!E:E&lt;&gt;""),Daily!E:E)</f>
-        <v>6.2078989605356405E-3</v>
+        <v>-4.2372073179913761E-3</v>
       </c>
       <c r="K31" s="22">
         <f>VLOOKUP($H$30,Daily!$A:$AF,7,0)</f>
-        <v>3.7857032016752612E-3</v>
+        <v>-4.675449256260622E-4</v>
       </c>
       <c r="L31" s="23">
         <f>VLOOKUP($H$30,Daily!$A:$AF,8,0)</f>
-        <v>-3.8250000000001894E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+        <v>-8.0460000000002196E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H32" s="19" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="24">
         <f>$K$25</f>
-        <v>-1.7696134434710348E-3</v>
+        <v>-1.1895616783457552E-3</v>
       </c>
       <c r="J32" s="24">
         <f>LOOKUP(2,1/(Daily!M:M&lt;&gt;""),Daily!M:M)</f>
-        <v>1.8990130025341224E-3</v>
+        <v>-2.6674082651354956E-3</v>
       </c>
       <c r="K32" s="14">
         <f>VLOOKUP($H$30,Daily!$A:$AF,25,0)</f>
-        <v>1.8243913577117965E-2</v>
+        <v>1.5527841346118398E-2</v>
       </c>
       <c r="L32" s="25">
         <f>VLOOKUP($H$30,Daily!$A:$AF,31,0)</f>
-        <v>1.2398039169946085E-2</v>
+        <v>9.6975602726572241E-3</v>
       </c>
     </row>
     <row r="33" spans="8:18" x14ac:dyDescent="0.25">
@@ -2532,19 +2764,19 @@
       </c>
       <c r="I33" s="24">
         <f>$K$24</f>
-        <v>-1.0590228748939392E-3</v>
+        <v>3.3936651583709701E-3</v>
       </c>
       <c r="J33" s="24">
         <f>LOOKUP(2,1/(Daily!L:L&lt;&gt;""),Daily!L:L)</f>
-        <v>5.3589807289633473E-3</v>
+        <v>-1.4120304998587185E-3</v>
       </c>
       <c r="K33" s="14">
         <f>VLOOKUP($H$30,Daily!$A:$AF,24,0)</f>
-        <v>3.7465665629005329E-2</v>
+        <v>3.6000732466580754E-2</v>
       </c>
       <c r="L33" s="25">
         <f>VLOOKUP($H$30,Daily!$A:$AF,30,0)</f>
-        <v>6.3818810365247947E-2</v>
+        <v>6.2316665758688661E-2</v>
       </c>
     </row>
     <row r="34" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2553,19 +2785,19 @@
       </c>
       <c r="I34" s="26">
         <f>$K$26</f>
-        <v>-8.6797752808989888E-3</v>
+        <v>7.2778720996037908E-3</v>
       </c>
       <c r="J34" s="26">
         <f>LOOKUP(2,1/(Daily!N:N&lt;&gt;""),Daily!N:N)</f>
-        <v>9.9863822060828333E-3</v>
+        <v>-7.3033707865167719E-3</v>
       </c>
       <c r="K34" s="27">
         <f>VLOOKUP($H$30,Daily!$A:$AF,26,0)</f>
-        <v>2.2988505747126853E-2</v>
+        <v>1.5517241379310764E-2</v>
       </c>
       <c r="L34" s="28">
         <f>VLOOKUP($H$30,Daily!$A:$AF,32,0)</f>
-        <v>3.2317182280555024E-2</v>
+        <v>2.4777787129067974E-2</v>
       </c>
     </row>
     <row r="35" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2600,7 +2832,7 @@
       </c>
       <c r="I37" s="46">
         <f>AVERAGE(Daily!E$3:E380)</f>
-        <v>-4.6872319399454687E-5</v>
+        <v>-1.1133901168548424E-4</v>
       </c>
       <c r="J37" s="44"/>
       <c r="K37" s="22"/>
@@ -2608,23 +2840,23 @@
       <c r="M37" s="50"/>
       <c r="N37" s="38">
         <f>AVERAGE(Daily!J$3:J380)</f>
-        <v>3.0150403310139344E-4</v>
+        <v>2.6328381154061477E-4</v>
       </c>
       <c r="O37" s="22">
         <f>AVERAGE(Daily!K$3:K380)</f>
-        <v>4.5822163370923881E-5</v>
+        <v>-7.1028716088581822E-6</v>
       </c>
       <c r="P37" s="22">
         <f>AVERAGE(Daily!L$3:L380)</f>
-        <v>9.8504127565031039E-4</v>
+        <v>9.4816324833478689E-4</v>
       </c>
       <c r="Q37" s="22">
         <f>AVERAGE(Daily!M$3:M380)</f>
-        <v>1.9923128520920558E-4</v>
+        <v>1.5512913828082556E-4</v>
       </c>
       <c r="R37" s="23">
         <f>AVERAGE(Daily!N$3:N380)</f>
-        <v>5.3153540554503394E-4</v>
+        <v>4.1099838720562155E-4</v>
       </c>
     </row>
     <row r="38" spans="8:18" x14ac:dyDescent="0.25">
@@ -2633,7 +2865,7 @@
       </c>
       <c r="I38" s="47">
         <f>STDEV(Daily!E$3:E380)</f>
-        <v>5.1385923318745608E-3</v>
+        <v>5.1247134569516071E-3</v>
       </c>
       <c r="J38" s="45"/>
       <c r="K38" s="14"/>
@@ -2641,23 +2873,23 @@
       <c r="M38" s="51"/>
       <c r="N38" s="40">
         <f>STDEV(Daily!J$3:J380)</f>
-        <v>6.3131389887279487E-3</v>
+        <v>6.2711983904234917E-3</v>
       </c>
       <c r="O38" s="14">
         <f>STDEV(Daily!K$3:K380)</f>
-        <v>1.7731150536771641E-3</v>
+        <v>1.8102159634548203E-3</v>
       </c>
       <c r="P38" s="14">
         <f>STDEV(Daily!L$3:L380)</f>
-        <v>6.0348242128998135E-3</v>
+        <v>5.9948689785730052E-3</v>
       </c>
       <c r="Q38" s="14">
         <f>STDEV(Daily!M$3:M380)</f>
-        <v>3.683969677972472E-3</v>
+        <v>3.6723290685435122E-3</v>
       </c>
       <c r="R38" s="25">
         <f>STDEV(Daily!N$3:N380)</f>
-        <v>8.3657105425102903E-3</v>
+        <v>8.3567931483112135E-3</v>
       </c>
     </row>
     <row r="39" spans="8:18" x14ac:dyDescent="0.25">
@@ -2732,7 +2964,7 @@
       </c>
       <c r="I41" s="47">
         <f>SUMIF(Daily!E$3:E380,"&lt;0")</f>
-        <v>-0.12119874479131054</v>
+        <v>-0.12543595210930192</v>
       </c>
       <c r="J41" s="45"/>
       <c r="K41" s="14"/>
@@ -2740,23 +2972,23 @@
       <c r="M41" s="51"/>
       <c r="N41" s="40">
         <f>SUMIF(Daily!J$3:J380,"&lt;0")</f>
-        <v>-0.14780541383235707</v>
+        <v>-0.14998822420070629</v>
       </c>
       <c r="O41" s="14">
         <f>SUMIF(Daily!K$3:K380,"&lt;0")</f>
-        <v>-4.1760739202887906E-2</v>
+        <v>-4.5155044313202816E-2</v>
       </c>
       <c r="P41" s="14">
         <f>SUMIF(Daily!L$3:L380,"&lt;0")</f>
-        <v>-0.12248983195218606</v>
+        <v>-0.12390186245204478</v>
       </c>
       <c r="Q41" s="14">
         <f>SUMIF(Daily!M$3:M380,"&lt;0")</f>
-        <v>-8.5062541961776678E-2</v>
+        <v>-8.7729950226912171E-2</v>
       </c>
       <c r="R41" s="25">
         <f>SUMIF(Daily!N$3:N380,"&lt;0")</f>
-        <v>-0.1942604005586252</v>
+        <v>-0.20156377134514197</v>
       </c>
     </row>
     <row r="42" spans="8:18" x14ac:dyDescent="0.25">
@@ -2765,7 +2997,7 @@
       </c>
       <c r="I42" s="48">
         <f>COUNT(Daily!E$3:E380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J42" s="45"/>
       <c r="K42" s="14"/>
@@ -2773,23 +3005,23 @@
       <c r="M42" s="51"/>
       <c r="N42" s="41">
         <f>COUNT(Daily!J$3:J380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O42" s="33">
         <f>COUNT(Daily!K$3:K380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P42" s="33">
         <f>COUNT(Daily!L$3:L380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q42" s="33">
         <f>COUNT(Daily!M$3:M380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R42" s="35">
         <f>COUNT(Daily!N$3:N380)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="8:18" x14ac:dyDescent="0.25">
@@ -2798,7 +3030,7 @@
       </c>
       <c r="I43" s="48">
         <f>I42-I39</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J43" s="45"/>
       <c r="K43" s="14"/>
@@ -2806,23 +3038,23 @@
       <c r="M43" s="51"/>
       <c r="N43" s="41">
         <f>N42-N39</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O43" s="33">
         <f>O42-O39</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P43" s="33">
         <f>P42-P39</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q43" s="33">
         <f>Q42-Q39</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R43" s="35">
         <f>R42-R39</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="8:18" x14ac:dyDescent="0.25">
@@ -2831,7 +3063,7 @@
       </c>
       <c r="I44" s="49">
         <f>(I40/I41)*(I39/I43)*-1</f>
-        <v>1.2538911650321911</v>
+        <v>1.1697578468882366</v>
       </c>
       <c r="J44" s="45"/>
       <c r="K44" s="14"/>
@@ -2839,23 +3071,23 @@
       <c r="M44" s="51"/>
       <c r="N44" s="42">
         <f>(N40/N41)*(N39/N43)*-1</f>
-        <v>1.2034905919054479</v>
+        <v>1.1489141905481586</v>
       </c>
       <c r="O44" s="34">
         <f>(O40/O41)*(O39/O43)*-1</f>
-        <v>1.0702242946776268</v>
+        <v>0.95978232656681628</v>
       </c>
       <c r="P44" s="34">
         <f>(P40/P41)*(P39/P43)*-1</f>
-        <v>2.0756678370962307</v>
+        <v>1.9787266041264102</v>
       </c>
       <c r="Q44" s="34">
         <f>(Q40/Q41)*(Q39/Q43)*-1</f>
-        <v>1.3032190302244664</v>
+        <v>1.2228338377302548</v>
       </c>
       <c r="R44" s="36">
         <f>(R40/R41)*(R39/R43)*-1</f>
-        <v>1.6103452884797413</v>
+        <v>1.4965683077145584</v>
       </c>
     </row>
     <row r="45" spans="8:18" x14ac:dyDescent="0.25">
@@ -2864,7 +3096,7 @@
       </c>
       <c r="I45" s="62">
         <f>I39/I42</f>
-        <v>0.5625</v>
+        <v>0.55384615384615388</v>
       </c>
       <c r="J45" s="63"/>
       <c r="K45" s="64"/>
@@ -2872,23 +3104,23 @@
       <c r="M45" s="66"/>
       <c r="N45" s="67">
         <f>N39/N42</f>
-        <v>0.515625</v>
+        <v>0.50769230769230766</v>
       </c>
       <c r="O45" s="64">
         <f>O39/O42</f>
-        <v>0.5</v>
+        <v>0.49230769230769234</v>
       </c>
       <c r="P45" s="64">
         <f>P39/P42</f>
-        <v>0.578125</v>
+        <v>0.56923076923076921</v>
       </c>
       <c r="Q45" s="64">
         <f>Q39/Q42</f>
-        <v>0.53125</v>
+        <v>0.52307692307692311</v>
       </c>
       <c r="R45" s="68">
         <f>R39/R42</f>
-        <v>0.578125</v>
+        <v>0.56923076923076921</v>
       </c>
     </row>
     <row r="46" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2942,7 +3174,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
+      <selection pane="bottomRight" activeCell="AH55" sqref="AH55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8957,7 +9189,7 @@
         <v>43291</v>
       </c>
       <c r="B51" s="4">
-        <f t="shared" ref="B51:B66" si="812">D51-C51</f>
+        <f t="shared" ref="B51:B67" si="812">D51-C51</f>
         <v>19902.79</v>
       </c>
       <c r="C51" s="4">
@@ -11129,33 +11361,140 @@
       </c>
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="4"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="P67" s="10"/>
-      <c r="Q67" s="10"/>
-      <c r="R67" s="10"/>
-      <c r="S67" s="10"/>
-      <c r="T67" s="10"/>
-      <c r="V67" s="5"/>
-      <c r="W67" s="5"/>
-      <c r="X67" s="5"/>
-      <c r="Y67" s="5"/>
-      <c r="Z67" s="5"/>
-      <c r="AB67" s="8"/>
-      <c r="AC67" s="8"/>
-      <c r="AD67" s="8"/>
-      <c r="AE67" s="8"/>
-      <c r="AF67" s="8"/>
+      <c r="A67" s="9">
+        <v>43313</v>
+      </c>
+      <c r="B67" s="4">
+        <f t="shared" si="812"/>
+        <v>19743.699999999997</v>
+      </c>
+      <c r="C67" s="4">
+        <v>95.38</v>
+      </c>
+      <c r="D67" s="4">
+        <f>19805.92+33.16</f>
+        <v>19839.079999999998</v>
+      </c>
+      <c r="E67" s="5">
+        <f t="shared" ref="E67" si="1128">D67/D66-1</f>
+        <v>-4.2372073179913761E-3</v>
+      </c>
+      <c r="F67" s="10">
+        <f t="shared" ref="F67" si="1129">F66*(1+E67)</f>
+        <v>99.195399999999978</v>
+      </c>
+      <c r="G67" s="5">
+        <f t="shared" ref="G67" si="1130">F67/F$45-1</f>
+        <v>-4.675449256260622E-4</v>
+      </c>
+      <c r="H67" s="8">
+        <f t="shared" ref="H67" si="1131">F67/$F$2-1</f>
+        <v>-8.0460000000002196E-3</v>
+      </c>
+      <c r="J67" s="11">
+        <f>VLOOKUP($A67,Prices!$A:$J,MATCH(J$1,Prices!$1:$1,0),0)</f>
+        <v>-2.1828103683492195E-3</v>
+      </c>
+      <c r="K67" s="11">
+        <f>VLOOKUP($A67,Prices!$A:$J,MATCH(K$1,Prices!$1:$1,0),0)</f>
+        <v>-3.3943051103149102E-3</v>
+      </c>
+      <c r="L67" s="11">
+        <f>VLOOKUP($A67,Prices!$A:$J,MATCH(L$1,Prices!$1:$1,0),0)</f>
+        <v>-1.4120304998587185E-3</v>
+      </c>
+      <c r="M67" s="11">
+        <f t="shared" ref="M67" si="1132">0.6*J67 + 0.4*K67</f>
+        <v>-2.6674082651354956E-3</v>
+      </c>
+      <c r="N67" s="11">
+        <f>VLOOKUP($A67,Prices!$A:$J,MATCH(N$1,Prices!$1:$1,0),0)</f>
+        <v>-7.3033707865167719E-3</v>
+      </c>
+      <c r="P67" s="10">
+        <f t="shared" ref="P67" si="1133">P66*(1+J67)</f>
+        <v>101.59776475788028</v>
+      </c>
+      <c r="Q67" s="10">
+        <f t="shared" ref="Q67" si="1134">Q66*(1+K67)</f>
+        <v>99.943366139869326</v>
+      </c>
+      <c r="R67" s="10">
+        <f t="shared" ref="R67" si="1135">R66*(1+L67)</f>
+        <v>106.23166657586887</v>
+      </c>
+      <c r="S67" s="10">
+        <f t="shared" ref="S67" si="1136">S66*(1+M67)</f>
+        <v>100.96975602726572</v>
+      </c>
+      <c r="T67" s="10">
+        <f t="shared" ref="T67" si="1137">T66*(1+N67)</f>
+        <v>102.4777787129068</v>
+      </c>
+      <c r="V67" s="5">
+        <f t="shared" ref="V67" si="1138">P67/P$45-1</f>
+        <v>2.8402699662542163E-2</v>
+      </c>
+      <c r="W67" s="5">
+        <f t="shared" ref="W67" si="1139">Q67/Q$45-1</f>
+        <v>-3.6836370354456083E-3</v>
+      </c>
+      <c r="X67" s="5">
+        <f t="shared" ref="X67" si="1140">R67/R$45-1</f>
+        <v>3.6000732466580754E-2</v>
+      </c>
+      <c r="Y67" s="5">
+        <f t="shared" ref="Y67" si="1141">S67/S$45-1</f>
+        <v>1.5527841346118398E-2</v>
+      </c>
+      <c r="Z67" s="5">
+        <f t="shared" ref="Z67" si="1142">T67/T$45-1</f>
+        <v>1.5517241379310764E-2</v>
+      </c>
+      <c r="AB67" s="8">
+        <f t="shared" ref="AB67" si="1143">P67/$P$2-1</f>
+        <v>1.5977647578802934E-2</v>
+      </c>
+      <c r="AC67" s="8">
+        <f t="shared" ref="AC67" si="1144">Q67/$P$2-1</f>
+        <v>-5.663386013067262E-4</v>
+      </c>
+      <c r="AD67" s="8">
+        <f t="shared" ref="AD67" si="1145">R67/$P$2-1</f>
+        <v>6.2316665758688661E-2</v>
+      </c>
+      <c r="AE67" s="8">
+        <f t="shared" ref="AE67" si="1146">S67/$P$2-1</f>
+        <v>9.6975602726572241E-3</v>
+      </c>
+      <c r="AF67" s="8">
+        <f t="shared" ref="AF67" si="1147">T67/$T$2-1</f>
+        <v>2.4777787129067974E-2</v>
+      </c>
+      <c r="AI67" s="8">
+        <f t="shared" ref="AI67" si="1148">MIN(0,(F67-MAX(F38:F67))/MAX(F38:F67))</f>
+        <v>-7.9542357668084228E-3</v>
+      </c>
+      <c r="AJ67" s="8">
+        <f t="shared" ref="AJ67" si="1149">MIN(0,(P67-MAX(P38:P67))/MAX(P38:P67))</f>
+        <v>-1.0016242555495311E-2</v>
+      </c>
+      <c r="AK67" s="8">
+        <f t="shared" ref="AK67" si="1150">MIN(0,(Q67-MAX(Q38:Q67))/MAX(Q38:Q67))</f>
+        <v>-7.6049197258472867E-3</v>
+      </c>
+      <c r="AL67" s="8">
+        <f t="shared" ref="AL67" si="1151">MIN(0,(R67-MAX(R38:R67))/MAX(R38:R67))</f>
+        <v>-1.1531204137256525E-2</v>
+      </c>
+      <c r="AM67" s="8">
+        <f t="shared" ref="AM67" si="1152">MIN(0,(S67-MAX(S38:S67))/MAX(S38:S67))</f>
+        <v>-7.3683746455965064E-3</v>
+      </c>
+      <c r="AN67" s="8">
+        <f t="shared" ref="AN67" si="1153">MIN(0,(T67-MAX(T38:T67))/MAX(T38:T67))</f>
+        <v>-1.2297372833985406E-2</v>
+      </c>
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
@@ -11183,10 +11522,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13625,6 +13964,179 @@
         <v>9.9863822060828333E-3</v>
       </c>
     </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="13">
+        <v>43313</v>
+      </c>
+      <c r="B68">
+        <f t="array" ref="B68">_xll.HistoricalData(B$1,"Adj. Close",$A68,$A68,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>73.14</v>
+      </c>
+      <c r="C68">
+        <f t="array" ref="C68">_xll.HistoricalData(C$1,"Adj. Close",$A68,$A68,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>105.7</v>
+      </c>
+      <c r="D68">
+        <f t="array" ref="D68">_xll.HistoricalData(D$1,"Adj. Close",$A68,$A68,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>282.88</v>
+      </c>
+      <c r="E68">
+        <f t="array" ref="E68">_xll.HistoricalData(E$1,"Adj. Close",$A68,$A68,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>17.670000000000002</v>
+      </c>
+      <c r="G68" s="5">
+        <f t="shared" ref="G68:G72" si="216">B68/B67-1</f>
+        <v>-2.1828103683492195E-3</v>
+      </c>
+      <c r="H68" s="5">
+        <f t="shared" ref="H68:H72" si="217">C68/C67-1</f>
+        <v>-3.3943051103149102E-3</v>
+      </c>
+      <c r="I68" s="5">
+        <f t="shared" ref="I68:I72" si="218">D68/D67-1</f>
+        <v>-1.4120304998587185E-3</v>
+      </c>
+      <c r="J68" s="5">
+        <f t="shared" ref="J68:J72" si="219">E68/E67-1</f>
+        <v>-7.3033707865167719E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="str">
+        <f t="array" ref="B69">_xll.HistoricalData(B$1,"Adj. Close",$A69,$A69,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="array" ref="C69">_xll.HistoricalData(C$1,"Adj. Close",$A69,$A69,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="array" ref="D69">_xll.HistoricalData(D$1,"Adj. Close",$A69,$A69,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="array" ref="E69">_xll.HistoricalData(E$1,"Adj. Close",$A69,$A69,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="G69" s="5" t="e">
+        <f t="shared" si="216"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H69" s="5" t="e">
+        <f t="shared" si="217"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I69" s="5" t="e">
+        <f t="shared" si="218"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J69" s="5" t="e">
+        <f t="shared" si="219"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="str">
+        <f t="array" ref="B70">_xll.HistoricalData(B$1,"Adj. Close",$A70,$A70,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="array" ref="C70">_xll.HistoricalData(C$1,"Adj. Close",$A70,$A70,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="array" ref="D70">_xll.HistoricalData(D$1,"Adj. Close",$A70,$A70,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="array" ref="E70">_xll.HistoricalData(E$1,"Adj. Close",$A70,$A70,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="G70" s="5" t="e">
+        <f t="shared" si="216"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H70" s="5" t="e">
+        <f t="shared" si="217"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I70" s="5" t="e">
+        <f t="shared" si="218"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J70" s="5" t="e">
+        <f t="shared" si="219"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="str">
+        <f t="array" ref="B71">_xll.HistoricalData(B$1,"Adj. Close",$A71,$A71,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="array" ref="C71">_xll.HistoricalData(C$1,"Adj. Close",$A71,$A71,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="array" ref="D71">_xll.HistoricalData(D$1,"Adj. Close",$A71,$A71,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="array" ref="E71">_xll.HistoricalData(E$1,"Adj. Close",$A71,$A71,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="G71" s="5" t="e">
+        <f t="shared" si="216"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H71" s="5" t="e">
+        <f t="shared" si="217"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I71" s="5" t="e">
+        <f t="shared" si="218"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J71" s="5" t="e">
+        <f t="shared" si="219"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="str">
+        <f t="array" ref="B72">_xll.HistoricalData(B$1,"Adj. Close",$A72,$A72,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="array" ref="C72">_xll.HistoricalData(C$1,"Adj. Close",$A72,$A72,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="array" ref="D72">_xll.HistoricalData(D$1,"Adj. Close",$A72,$A72,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="array" ref="E72">_xll.HistoricalData(E$1,"Adj. Close",$A72,$A72,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
+        <v>--</v>
+      </c>
+      <c r="G72" s="5" t="e">
+        <f t="shared" si="216"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H72" s="5" t="e">
+        <f t="shared" si="217"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I72" s="5" t="e">
+        <f t="shared" si="218"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J72" s="5" t="e">
+        <f t="shared" si="219"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sector Rotaion Model 08062018
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="112">
   <si>
     <t>Symbol</t>
   </si>
@@ -361,15 +361,19 @@
   <si>
     <t>QQQ</t>
   </si>
+  <si>
+    <t>IMV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -840,7 +844,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1004,6 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1028,7 +1033,7 @@
   <volType type="realTimeData">
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-2.58961428376718E-3</v>
+        <v>-1.362954886193962E-4</v>
         <stp/>
         <stp>ACWI</stp>
         <stp>change in percent</stp>
@@ -1037,56 +1042,56 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>1.13118352</v>
+        <v>0.81968596999999999</v>
         <stp/>
         <stp>TLT</stp>
         <stp>mtd percent change</stp>
         <tr r="U5" s="1"/>
       </tp>
       <tp>
-        <v>0.10835541</v>
+        <v>9.6315919999999999E-2</v>
         <stp/>
         <stp>SHY</stp>
         <stp>mtd percent change</stp>
         <tr r="U12" s="1"/>
       </tp>
       <tp>
-        <v>-0.44303797</v>
+        <v>-0.37974683999999997</v>
         <stp/>
         <stp>RWX</stp>
         <stp>mtd percent change</stp>
         <tr r="U6" s="1"/>
       </tp>
       <tp>
-        <v>0.97214367000000002</v>
+        <v>1.3009049800000001</v>
         <stp/>
         <stp>IVV</stp>
         <stp>mtd percent change</stp>
         <tr r="U3" s="1"/>
       </tp>
       <tp>
-        <v>0.79735034000000005</v>
+        <v>0.50294406000000003</v>
         <stp/>
         <stp>IYR</stp>
         <stp>mtd percent change</stp>
         <tr r="U4" s="1"/>
       </tp>
       <tp>
-        <v>-1.30434783</v>
+        <v>-1.19565217</v>
         <stp/>
         <stp>IEV</stp>
         <stp>mtd percent change</stp>
         <tr r="U9" s="1"/>
       </tp>
       <tp>
-        <v>0.59206630999999998</v>
+        <v>0.47858694000000002</v>
         <stp/>
         <stp>IEF</stp>
         <stp>mtd percent change</stp>
         <tr r="U11" s="1"/>
       </tp>
       <tp>
-        <v>-0.42991140999999999</v>
+        <v>-0.71955880000000005</v>
         <stp/>
         <stp>GLD</stp>
         <stp>mtd percent change</stp>
@@ -1095,21 +1100,21 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-1.4938041099999999</v>
+        <v>-1.3155661199999999</v>
         <stp/>
         <stp>EWJ</stp>
         <stp>mtd percent change</stp>
         <tr r="U7" s="1"/>
       </tp>
       <tp>
-        <v>-1.3495276700000001</v>
+        <v>-1.2145748999999999</v>
         <stp/>
         <stp>EEM</stp>
         <stp>mtd percent change</stp>
         <tr r="U10" s="1"/>
       </tp>
       <tp>
-        <v>1.29411765</v>
+        <v>1.14705882</v>
         <stp/>
         <stp>DBC</stp>
         <stp>mtd percent change</stp>
@@ -1118,7 +1123,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>1.1331444759208555E-3</v>
+        <v>2.8328611898017393E-3</v>
         <stp/>
         <stp>GYLD</stp>
         <stp>change in percent</stp>
@@ -1145,7 +1150,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>51.955800000000004</v>
+        <v>52.79</v>
         <stp/>
         <stp>MU</stp>
         <stp>last</stp>
@@ -1231,7 +1236,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>3.4965034965034206E-3</v>
+        <v>2.0396270396270456E-3</v>
         <stp/>
         <stp>DBC</stp>
         <stp>change in percent</stp>
@@ -1240,7 +1245,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>2.1627998427054562E-3</v>
+        <v>1.0322453794731027E-3</v>
         <stp/>
         <stp>IEF</stp>
         <stp>change in percent</stp>
@@ -1249,7 +1254,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>1.1333396244220819E-3</v>
+        <v>9.4366330093417295E-4</v>
         <stp/>
         <stp>AGG</stp>
         <stp>change in percent</stp>
@@ -1258,7 +1263,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-2.3929690219283502E-3</v>
+        <v>-5.2949878176123044E-3</v>
         <stp/>
         <stp>GLD</stp>
         <stp>change in percent</stp>
@@ -1267,7 +1272,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-9.2197370667577092E-3</v>
+        <v>-7.3416424790848558E-3</v>
         <stp/>
         <stp>EWJ</stp>
         <stp>change in percent</stp>
@@ -1276,7 +1281,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-7.916760913820424E-3</v>
+        <v>-6.6726984845058126E-3</v>
         <stp/>
         <stp>EEM</stp>
         <stp>change in percent</stp>
@@ -1285,7 +1290,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-4.8655881279639952E-4</v>
+        <v>-3.4059116895753193E-3</v>
         <stp/>
         <stp>IYR</stp>
         <stp>change in percent</stp>
@@ -1294,14 +1299,14 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-5.9119772279396321E-3</v>
+        <v>-4.8171666301729584E-3</v>
         <stp/>
         <stp>IEV</stp>
         <stp>change in percent</stp>
         <tr r="L9" s="1"/>
       </tp>
       <tp>
-        <v>2.8016109262820552E-4</v>
+        <v>3.5370337944317632E-3</v>
         <stp/>
         <stp>IVV</stp>
         <stp>change in percent</stp>
@@ -1311,7 +1316,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>4.8649555443717324E-3</v>
+        <v>1.7698372756248866E-3</v>
         <stp/>
         <stp>TLT</stp>
         <stp>change in percent</stp>
@@ -1320,7 +1325,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>-5.6890012642223523E-3</v>
+        <v>-5.056890012642124E-3</v>
         <stp/>
         <stp>RWX</stp>
         <stp>change in percent</stp>
@@ -1329,7 +1334,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>3.6092396535131253E-4</v>
+        <v>2.4061597690081809E-4</v>
         <stp/>
         <stp>SHY</stp>
         <stp>change in percent</stp>
@@ -1338,7 +1343,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>38.28</v>
+        <v>38.406599999999997</v>
         <stp/>
         <stp>GAL</stp>
         <stp>last</stp>
@@ -1347,7 +1352,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>17.22</v>
+        <v>17.195</v>
         <stp/>
         <stp>DBC</stp>
         <stp>last</stp>
@@ -1357,7 +1362,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>101.94</v>
+        <v>101.825</v>
         <stp/>
         <stp>IEF</stp>
         <stp>last</stp>
@@ -1366,14 +1371,14 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>43.86</v>
+        <v>43.914999999999999</v>
         <stp/>
         <stp>EEM</stp>
         <stp>last</stp>
         <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>45.4</v>
+        <v>45.45</v>
         <stp/>
         <stp>IEV</stp>
         <stp>last</stp>
@@ -1382,7 +1387,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>520.69000000000005</v>
+        <v>518.92499999999995</v>
         <stp/>
         <stp>ISRG</stp>
         <stp>last</stp>
@@ -1391,7 +1396,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>46.930399999999999</v>
+        <v>47.04</v>
         <stp/>
         <stp>QQQE</stp>
         <stp>last</stp>
@@ -1409,7 +1414,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>83.15</v>
+        <v>83.14</v>
         <stp/>
         <stp>SHY</stp>
         <stp>last</stp>
@@ -1428,7 +1433,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>1828.72</v>
+        <v>1845.2989</v>
         <stp/>
         <stp>AMZN</stp>
         <stp>last</stp>
@@ -1437,7 +1442,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>114.645</v>
+        <v>114.3115</v>
         <stp/>
         <stp>GLD</stp>
         <stp>last</stp>
@@ -1446,7 +1451,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>119.8</v>
+        <v>119.431</v>
         <stp/>
         <stp>TLT</stp>
         <stp>last</stp>
@@ -1476,7 +1481,7 @@
         <tr r="M4" s="1"/>
       </tp>
       <tp>
-        <v>2.35</v>
+        <v>2.36</v>
         <stp/>
         <stp>IEF</stp>
         <stp>dividend yield</stp>
@@ -1513,7 +1518,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>2.69</v>
+        <v>2.68</v>
         <stp/>
         <stp>TLT</stp>
         <stp>dividend yield</stp>
@@ -1527,7 +1532,7 @@
         <tr r="M12" s="1"/>
       </tp>
       <tp>
-        <v>3.66</v>
+        <v>3.65</v>
         <stp/>
         <stp>RWX</stp>
         <stp>dividend yield</stp>
@@ -1545,7 +1550,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>365.26100000000002</v>
+        <v>368.15</v>
         <stp/>
         <stp>ALGN</stp>
         <stp>last</stp>
@@ -1554,7 +1559,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>180.14</v>
+        <v>181.07</v>
         <stp/>
         <stp>QQQ</stp>
         <stp>last</stp>
@@ -1563,7 +1568,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>42.83</v>
+        <v>43.365000000000002</v>
         <stp/>
         <stp>CSCO</stp>
         <stp>last</stp>
@@ -1572,7 +1577,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>53.61</v>
+        <v>54.024999999999999</v>
         <stp/>
         <stp>STX</stp>
         <stp>last</stp>
@@ -1581,7 +1586,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>58.03</v>
+        <v>58.14</v>
         <stp/>
         <stp>EWJ</stp>
         <stp>last</stp>
@@ -1590,7 +1595,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>39.325000000000003</v>
+        <v>39.35</v>
         <stp/>
         <stp>RWX</stp>
         <stp>last</stp>
@@ -1599,7 +1604,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>285.63</v>
+        <v>286.56</v>
         <stp/>
         <stp>IVV</stp>
         <stp>last</stp>
@@ -1610,7 +1615,7 @@
     </main>
     <main first="rtdsrv.b680f398aee849e8bbd7e44ce06d14f2">
       <tp>
-        <v>82.17</v>
+        <v>81.93</v>
         <stp/>
         <stp>IYR</stp>
         <stp>last</stp>
@@ -1897,8 +1902,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,15 +2022,15 @@
       </c>
       <c r="J2" s="4">
         <f>_xll.RealtimeData(A2,"Last")</f>
-        <v>17.22</v>
+        <v>17.195</v>
       </c>
       <c r="K2" s="5">
         <f>J2/D2-1</f>
-        <v>-3.4039776357209228E-2</v>
+        <v>-3.5442157634274718E-2</v>
       </c>
       <c r="L2" s="8">
         <f>_xll.RealtimeData(A2,"Change in Percent")</f>
-        <v>3.4965034965034206E-3</v>
+        <v>2.0396270396270456E-3</v>
       </c>
       <c r="M2" s="29" t="str">
         <f>_xll.RealtimeData(A2,"Dividend Yield")</f>
@@ -2060,7 +2065,7 @@
       </c>
       <c r="U2">
         <f>_xll.RealtimeData(T2,"MTD Percent Change")</f>
-        <v>1.29411765</v>
+        <v>1.14705882</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2098,15 +2103,15 @@
       </c>
       <c r="J3" s="4">
         <f>_xll.RealtimeData(A3,"Last")</f>
-        <v>285.63</v>
+        <v>286.56</v>
       </c>
       <c r="K3" s="5">
         <f>J3/D3-1</f>
-        <v>7.2347710519053976E-2</v>
+        <v>7.5839232315723537E-2</v>
       </c>
       <c r="L3" s="8">
         <f>_xll.RealtimeData(A3,"Change in Percent")</f>
-        <v>2.8016109262820552E-4</v>
+        <v>3.5370337944317632E-3</v>
       </c>
       <c r="M3" s="29">
         <f>_xll.RealtimeData(A3,"Dividend Yield")</f>
@@ -2141,7 +2146,7 @@
       </c>
       <c r="U3">
         <f>_xll.RealtimeData(T3,"MTD Percent Change")</f>
-        <v>0.97214367000000002</v>
+        <v>1.3009049800000001</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -2179,15 +2184,15 @@
       </c>
       <c r="J4" s="4">
         <f>_xll.RealtimeData(A4,"Last")</f>
-        <v>82.17</v>
+        <v>81.93</v>
       </c>
       <c r="K4" s="5">
         <f>J4/D4-1</f>
-        <v>4.7685834502103619E-2</v>
+        <v>4.4625780951166538E-2</v>
       </c>
       <c r="L4" s="8">
         <f t="array" ref="L4">_xll.RealtimeData(A4,"Change in Percent")</f>
-        <v>-4.8655881279639952E-4</v>
+        <v>-3.4059116895753193E-3</v>
       </c>
       <c r="M4" s="29">
         <f>_xll.RealtimeData(A4,"Dividend Yield")</f>
@@ -2222,7 +2227,7 @@
       </c>
       <c r="U4">
         <f>_xll.RealtimeData(T4,"MTD Percent Change")</f>
-        <v>0.79735034000000005</v>
+        <v>0.50294406000000003</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2260,19 +2265,19 @@
       </c>
       <c r="J5" s="31">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>119.8</v>
+        <v>119.431</v>
       </c>
       <c r="K5" s="5">
         <f>J5/D5-1</f>
-        <v>-2.0391875957734618E-2</v>
+        <v>-2.3409199812255421E-2</v>
       </c>
       <c r="L5" s="8">
         <f t="array" ref="L5">_xll.RealtimeData(A5,"Change in Percent")</f>
-        <v>4.8649555443717324E-3</v>
+        <v>1.7698372756248866E-3</v>
       </c>
       <c r="M5" s="29">
         <f>_xll.RealtimeData(A5,"Dividend Yield")</f>
-        <v>2.69</v>
+        <v>2.68</v>
       </c>
       <c r="N5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2303,7 +2308,7 @@
       </c>
       <c r="U5">
         <f>_xll.RealtimeData(T5,"MTD Percent Change")</f>
-        <v>1.13118352</v>
+        <v>0.81968596999999999</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2323,16 +2328,16 @@
       <c r="I6" s="4"/>
       <c r="J6" s="31">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>39.325000000000003</v>
+        <v>39.35</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="8">
         <f>_xll.RealtimeData(A6,"Change in Percent")</f>
-        <v>-5.6890012642223523E-3</v>
+        <v>-5.056890012642124E-3</v>
       </c>
       <c r="M6" s="29">
         <f>_xll.RealtimeData(A6,"Dividend Yield")</f>
-        <v>3.66</v>
+        <v>3.65</v>
       </c>
       <c r="N6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2363,7 +2368,7 @@
       </c>
       <c r="U6">
         <f>_xll.RealtimeData(T6,"MTD Percent Change")</f>
-        <v>-0.44303797</v>
+        <v>-0.37974683999999997</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2383,12 +2388,12 @@
       <c r="I7" s="4"/>
       <c r="J7" s="31">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>58.03</v>
+        <v>58.14</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="8">
         <f>_xll.RealtimeData(A7,"Change in Percent")</f>
-        <v>-9.2197370667577092E-3</v>
+        <v>-7.3416424790848558E-3</v>
       </c>
       <c r="M7" s="29">
         <f>_xll.RealtimeData(A7,"Dividend Yield")</f>
@@ -2423,7 +2428,7 @@
       </c>
       <c r="U7">
         <f>_xll.RealtimeData(T7,"MTD Percent Change")</f>
-        <v>-1.4938041099999999</v>
+        <v>-1.3155661199999999</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2443,12 +2448,12 @@
       <c r="I8" s="4"/>
       <c r="J8" s="31">
         <f>_xll.RealtimeData(A8,"Last")</f>
-        <v>114.645</v>
+        <v>114.3115</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="8">
         <f>_xll.RealtimeData(A8,"Change in Percent")</f>
-        <v>-2.3929690219283502E-3</v>
+        <v>-5.2949878176123044E-3</v>
       </c>
       <c r="M8" s="29">
         <v>0</v>
@@ -2482,7 +2487,7 @@
       </c>
       <c r="U8">
         <f>_xll.RealtimeData(T8,"MTD Percent Change")</f>
-        <v>-0.42991140999999999</v>
+        <v>-0.71955880000000005</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2502,12 +2507,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="31">
         <f>_xll.RealtimeData(A9,"Last")</f>
-        <v>45.4</v>
+        <v>45.45</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="8">
         <f>_xll.RealtimeData(A9,"Change in Percent")</f>
-        <v>-5.9119772279396321E-3</v>
+        <v>-4.8171666301729584E-3</v>
       </c>
       <c r="M9" s="29">
         <f>_xll.RealtimeData(A9,"Dividend Yield")</f>
@@ -2542,7 +2547,7 @@
       </c>
       <c r="U9">
         <f>_xll.RealtimeData(T9,"MTD Percent Change")</f>
-        <v>-1.30434783</v>
+        <v>-1.19565217</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2556,12 +2561,12 @@
       <c r="G10" s="4"/>
       <c r="J10" s="31">
         <f>_xll.RealtimeData(A10,"Last")</f>
-        <v>43.86</v>
+        <v>43.914999999999999</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="8">
         <f t="array" ref="L10">_xll.RealtimeData(A10,"Change in Percent")</f>
-        <v>-7.916760913820424E-3</v>
+        <v>-6.6726984845058126E-3</v>
       </c>
       <c r="M10" s="29">
         <f>_xll.RealtimeData(A10,"Dividend Yield")</f>
@@ -2596,7 +2601,7 @@
       </c>
       <c r="U10">
         <f>_xll.RealtimeData(T10,"MTD Percent Change")</f>
-        <v>-1.3495276700000001</v>
+        <v>-1.2145748999999999</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2610,16 +2615,16 @@
       <c r="G11" s="4"/>
       <c r="J11" s="31">
         <f>_xll.RealtimeData(A11,"Last")</f>
-        <v>101.94</v>
+        <v>101.825</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="8">
         <f t="array" ref="L11">_xll.RealtimeData(A11,"Change in Percent")</f>
-        <v>2.1627998427054562E-3</v>
+        <v>1.0322453794731027E-3</v>
       </c>
       <c r="M11" s="29">
         <f>_xll.RealtimeData(A11,"Dividend Yield")</f>
-        <v>2.35</v>
+        <v>2.36</v>
       </c>
       <c r="N11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2650,7 +2655,7 @@
       </c>
       <c r="U11">
         <f>_xll.RealtimeData(T11,"MTD Percent Change")</f>
-        <v>0.59206630999999998</v>
+        <v>0.47858694000000002</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2663,11 +2668,11 @@
       </c>
       <c r="J12" s="31">
         <f>_xll.RealtimeData(A12,"Last")</f>
-        <v>83.15</v>
+        <v>83.14</v>
       </c>
       <c r="L12" s="8">
         <f t="array" ref="L12">_xll.RealtimeData(A12,"Change in Percent")</f>
-        <v>3.6092396535131253E-4</v>
+        <v>2.4061597690081809E-4</v>
       </c>
       <c r="M12" s="29">
         <f>_xll.RealtimeData(A12,"Dividend Yield")</f>
@@ -2702,7 +2707,7 @@
       </c>
       <c r="U12">
         <f>_xll.RealtimeData(T12,"MTD Percent Change")</f>
-        <v>0.10835541</v>
+        <v>9.6315919999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -2719,11 +2724,11 @@
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U14" s="29">
         <f t="array" ref="U14">MMULT(TRANSPOSE(O2:O12),U2:U12)</f>
-        <v>0.86365515872999987</v>
+        <v>0.84620586678000009</v>
       </c>
       <c r="V14" s="8">
         <f>U14*0.01</f>
-        <v>8.6365515872999996E-3</v>
+        <v>8.4620586678000008E-3</v>
       </c>
     </row>
     <row r="19" spans="5:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2766,18 +2771,18 @@
       </c>
       <c r="K21" s="8">
         <f>SUMPRODUCT(K2:K7,F2:F7)</f>
-        <v>3.1132086006879098E-2</v>
+        <v>3.1057252658759353E-2</v>
       </c>
       <c r="M21" t="s">
         <v>34</v>
       </c>
       <c r="N21" s="8">
         <f t="array" ref="N21">MMULT(TRANSPOSE(F2:F5),L2:L5)</f>
-        <v>1.5503403301894876E-3</v>
+        <v>1.3851606141586956E-3</v>
       </c>
       <c r="P21" s="8">
         <f t="array" ref="P21">SUMPRODUCT(L2:L12,O2:O12)</f>
-        <v>4.4355631554620386E-4</v>
+        <v>2.6947909609914604E-4</v>
       </c>
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
@@ -2792,7 +2797,7 @@
       </c>
       <c r="K22" s="8">
         <f>_xll.RealtimeData(J22,"Change in Percent")</f>
-        <v>-2.58961428376718E-3</v>
+        <v>-1.362954886193962E-4</v>
       </c>
       <c r="L22" s="12">
         <v>0.6</v>
@@ -2804,7 +2809,7 @@
       </c>
       <c r="K23" s="8">
         <f>_xll.RealtimeData(J23,"Change in Percent")</f>
-        <v>1.1333396244220819E-3</v>
+        <v>9.4366330093417295E-4</v>
       </c>
       <c r="L23" s="12">
         <v>0.4</v>
@@ -2816,7 +2821,7 @@
       </c>
       <c r="K24" s="8">
         <f>_xll.RealtimeData(J24,"Change in Percent")</f>
-        <v>2.8016109262820552E-4</v>
+        <v>3.5370337944317632E-3</v>
       </c>
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
@@ -2825,7 +2830,7 @@
       </c>
       <c r="K25" s="8">
         <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
-        <v>-1.1004327204914752E-3</v>
+        <v>2.9568802720203149E-4</v>
       </c>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
@@ -2841,7 +2846,7 @@
       </c>
       <c r="K26" s="8">
         <f>_xll.RealtimeData(J26,"Change in Percent")</f>
-        <v>1.1331444759208555E-3</v>
+        <v>2.8328611898017393E-3</v>
       </c>
       <c r="L26" t="str">
         <f>_xll.RealtimeData(J26,"Description")</f>
@@ -2854,7 +2859,7 @@
       </c>
       <c r="K27" s="8">
         <f>AVERAGE(L2:L11)</f>
-        <v>-2.0812584331256052E-3</v>
+        <v>-2.4210553624436576E-3</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
@@ -2863,14 +2868,14 @@
       </c>
       <c r="K28" s="8">
         <f>SUMPRODUCT(F2:F7,M2:M7)*0.01</f>
-        <v>1.4105368215824166E-2</v>
+        <v>1.4084513589467679E-2</v>
       </c>
       <c r="L28" t="s">
         <v>65</v>
       </c>
       <c r="M28" s="8">
         <f>AVERAGE(M2:M11)*0.01</f>
-        <v>2.0600000000000004E-2</v>
+        <v>2.0588888888888893E-2</v>
       </c>
     </row>
     <row r="29" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2897,7 +2902,7 @@
       </c>
       <c r="I31" s="21">
         <f>$N$21</f>
-        <v>1.5503403301894876E-3</v>
+        <v>1.3851606141586956E-3</v>
       </c>
       <c r="J31" s="21">
         <f>LOOKUP(2,1/(Daily!E:E&lt;&gt;""),Daily!E:E)</f>
@@ -2918,7 +2923,7 @@
       </c>
       <c r="I32" s="24">
         <f>$K$25</f>
-        <v>-1.1004327204914752E-3</v>
+        <v>2.9568802720203149E-4</v>
       </c>
       <c r="J32" s="24">
         <f>LOOKUP(2,1/(Daily!M:M&lt;&gt;""),Daily!M:M)</f>
@@ -2939,7 +2944,7 @@
       </c>
       <c r="I33" s="24">
         <f>$K$24</f>
-        <v>2.8016109262820552E-4</v>
+        <v>3.5370337944317632E-3</v>
       </c>
       <c r="J33" s="24">
         <f>LOOKUP(2,1/(Daily!L:L&lt;&gt;""),Daily!L:L)</f>
@@ -2960,7 +2965,7 @@
       </c>
       <c r="I34" s="26">
         <f>$K$26</f>
-        <v>1.1331444759208555E-3</v>
+        <v>2.8328611898017393E-3</v>
       </c>
       <c r="J34" s="26">
         <f>LOOKUP(2,1/(Daily!N:N&lt;&gt;""),Daily!N:N)</f>
@@ -14590,8 +14595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14629,7 +14634,7 @@
       </c>
       <c r="G2" s="74">
         <f>SUM(G5:G10)</f>
-        <v>1</v>
+        <v>0.99274023542198764</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -14637,11 +14642,12 @@
         <v>94</v>
       </c>
       <c r="B3" s="71">
-        <v>0.3</v>
+        <f>1-B2</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="C3">
         <f>B3*B1</f>
-        <v>30000</v>
+        <v>30000.000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -14666,6 +14672,9 @@
       <c r="H4" t="s">
         <v>104</v>
       </c>
+      <c r="I4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -14677,7 +14686,7 @@
       </c>
       <c r="C5">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>365.26100000000002</v>
+        <v>368.15</v>
       </c>
       <c r="D5">
         <f>ROUNDDOWN(($C$2/6)/B5,0)</f>
@@ -14685,19 +14694,23 @@
       </c>
       <c r="E5" s="8">
         <f>C5/B5-1</f>
-        <v>0.10034945021840658</v>
+        <v>0.10905256815785513</v>
       </c>
       <c r="F5">
         <f>C5*D5</f>
-        <v>12784.135</v>
+        <v>12885.25</v>
       </c>
       <c r="G5" s="73">
         <f>F5/$F$13</f>
-        <v>0.17762399860283193</v>
+        <v>0.17632156810892988</v>
       </c>
       <c r="H5" s="8">
         <f>F5/$F$31</f>
-        <v>0.12548882776145887</v>
+        <v>0.12470173141573514</v>
+      </c>
+      <c r="I5">
+        <f>B5*D5</f>
+        <v>11618.25</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -14710,7 +14723,7 @@
       </c>
       <c r="C6">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>1828.72</v>
+        <v>1845.2989</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D10" si="0">ROUNDDOWN(($C$2/6)/B6,0)</f>
@@ -14718,19 +14731,23 @@
       </c>
       <c r="E6" s="8">
         <f t="shared" ref="E6:E10" si="1">C6/B6-1</f>
-        <v>0.12217572194744797</v>
+        <v>0.13234919797253353</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F9" si="2">C6*D6</f>
-        <v>12801.04</v>
+        <v>12917.0923</v>
       </c>
       <c r="G6" s="73">
         <f t="shared" ref="G6:G10" si="3">F6/$F$13</f>
-        <v>0.17785887829523045</v>
+        <v>0.17675729766545342</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" ref="H6:H10" si="4">F6/$F$31</f>
-        <v>0.12565476692224739</v>
+        <v>0.12500989694936929</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I10" si="5">B6*D6</f>
+        <v>11407.34</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -14743,7 +14760,7 @@
       </c>
       <c r="C7">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>42.83</v>
+        <v>43.365000000000002</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -14751,19 +14768,23 @@
       </c>
       <c r="E7" s="8">
         <f t="shared" si="1"/>
-        <v>1.0618216139688386E-2</v>
+        <v>2.3242095327984824E-2</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>11778.25</v>
+        <v>11925.375</v>
       </c>
       <c r="G7" s="73">
         <f t="shared" si="3"/>
-        <v>0.16364813587652235</v>
+        <v>0.16318665297817503</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="4"/>
-        <v>0.11561507959524854</v>
+        <v>0.11541218915286257</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>11654.5</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -14776,7 +14797,7 @@
       </c>
       <c r="C8">
         <f>_xll.RealtimeData(A8,"Last")</f>
-        <v>520.69000000000005</v>
+        <v>518.92499999999995</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -14784,19 +14805,23 @@
       </c>
       <c r="E8" s="8">
         <f t="shared" si="1"/>
-        <v>0.13274740574760169</v>
+        <v>0.12890769465051011</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>13017.250000000002</v>
+        <v>12973.124999999998</v>
       </c>
       <c r="G8" s="73">
         <f t="shared" si="3"/>
-        <v>0.1808629207852322</v>
+        <v>0.17752404829344876</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="4"/>
-        <v>0.12777708019962636</v>
+        <v>0.12555217394872112</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>11491.75</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -14809,7 +14834,7 @@
       </c>
       <c r="C9">
         <f>_xll.RealtimeData(A9,"Last")</f>
-        <v>51.955800000000004</v>
+        <v>52.79</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -14817,19 +14842,23 @@
       </c>
       <c r="E9" s="8">
         <f t="shared" si="1"/>
-        <v>-9.7832957110609464E-2</v>
+        <v>-8.3347803438097001E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>10495.071600000001</v>
+        <v>10663.58</v>
       </c>
       <c r="G9" s="73">
         <f t="shared" si="3"/>
-        <v>0.1458195320383445</v>
+        <v>0.14592026908713626</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="4"/>
-        <v>0.10301942465067668</v>
+        <v>0.1032007053871834</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>11633.18</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -14842,7 +14871,7 @@
       </c>
       <c r="C10">
         <f>_xll.RealtimeData(A10,"Last")</f>
-        <v>53.61</v>
+        <v>54.024999999999999</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -14850,28 +14879,45 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" si="1"/>
-        <v>-4.8624667258207688E-2</v>
+        <v>-4.1259982253771144E-2</v>
       </c>
       <c r="F10">
         <f>C10*D10</f>
-        <v>11097.27</v>
+        <v>11183.174999999999</v>
       </c>
       <c r="G10" s="73">
         <f t="shared" si="3"/>
-        <v>0.1541865344018386</v>
+        <v>0.15303039928884438</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="4"/>
-        <v>0.1089305927739659</v>
+        <v>0.10822927651579625</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>11664.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>SUM(I5:I10)</f>
+        <v>69469.47</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>93</v>
       </c>
-      <c r="F13">
-        <f>SUM(F5:F10)</f>
-        <v>71973.016600000003</v>
+      <c r="F13" s="75">
+        <f>SUM(F5:F10)+I13</f>
+        <v>73078.127300000007</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13">
+        <f>C2-I12</f>
+        <v>530.52999999999884</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -14880,7 +14926,7 @@
       </c>
       <c r="F14" s="8">
         <f>F13/C2-1</f>
-        <v>2.8185951428571387E-2</v>
+        <v>4.397324714285733E-2</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -14888,13 +14934,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H17" s="11">
         <f>SUM(H20:H23)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.988278513726912</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>95</v>
       </c>
@@ -14919,8 +14965,11 @@
       <c r="I19" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -14930,7 +14979,7 @@
       </c>
       <c r="C20">
         <f>_xll.RealtimeData(A20,"Last")</f>
-        <v>17.22</v>
+        <v>17.195</v>
       </c>
       <c r="D20">
         <f>ROUNDDOWN(($C$3*E20)/B20,0)</f>
@@ -14941,22 +14990,26 @@
       </c>
       <c r="F20" s="8">
         <f>C20/B20-1</f>
-        <v>1.2941176470588234E-2</v>
+        <v>1.1470588235294121E-2</v>
       </c>
       <c r="G20">
         <f>D20*C20</f>
-        <v>4305</v>
+        <v>4298.75</v>
       </c>
       <c r="H20" s="8">
         <f>G20/$G$27</f>
-        <v>0.14397189187092227</v>
+        <v>0.14210541800562829</v>
       </c>
       <c r="I20" s="8">
         <f>G20/$F$31</f>
-        <v>4.225779871012629E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.1602729316341666E-2</v>
+      </c>
+      <c r="J20">
+        <f>B20*D20</f>
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -14966,33 +15019,37 @@
       </c>
       <c r="C21">
         <f>_xll.RealtimeData(A21,"Last")</f>
-        <v>285.63</v>
+        <v>286.56</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D22" si="5">ROUNDDOWN(($C$3*E21)/B21,0)</f>
+        <f t="shared" ref="D21:D22" si="6">ROUNDDOWN(($C$3*E21)/B21,0)</f>
         <v>38</v>
       </c>
       <c r="E21" s="11">
         <v>0.36599999999999999</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" ref="F21:F23" si="6">C21/B21-1</f>
-        <v>9.7214366515836481E-3</v>
+        <f t="shared" ref="F21:F23" si="7">C21/B21-1</f>
+        <v>1.300904977375561E-2</v>
       </c>
       <c r="G21">
-        <f t="shared" ref="G21:G22" si="7">D21*C21</f>
-        <v>10853.94</v>
+        <f t="shared" ref="G21:G22" si="8">D21*C21</f>
+        <v>10889.28</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" ref="H21:H23" si="8">G21/$G$27</f>
-        <v>0.36298775285795076</v>
+        <f t="shared" ref="H21:H23" si="9">G21/$G$27</f>
+        <v>0.3599710814028097</v>
       </c>
       <c r="I21" s="8">
-        <f t="shared" ref="I21:I23" si="9">G21/$F$31</f>
-        <v>0.10654207008868483</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I21:I23" si="10">G21/$F$31</f>
+        <v>0.10538499989295795</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21:J23" si="11">B21*D21</f>
+        <v>10749.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -15002,33 +15059,37 @@
       </c>
       <c r="C22">
         <f>_xll.RealtimeData(A22,"Last")</f>
-        <v>82.17</v>
+        <v>81.93</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>144</v>
       </c>
       <c r="E22" s="11">
         <v>0.39300000000000002</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="6"/>
-        <v>7.9735034347399036E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.0294406280668724E-3</v>
       </c>
       <c r="G22">
-        <f t="shared" si="7"/>
-        <v>11832.48</v>
+        <f t="shared" si="8"/>
+        <v>11797.920000000002</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="8"/>
-        <v>0.39571301536001169</v>
+        <f t="shared" si="9"/>
+        <v>0.39000834037731025</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" si="9"/>
-        <v>0.11614740025124161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0.11417869665736638</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="11"/>
+        <v>11738.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -15038,7 +15099,7 @@
       </c>
       <c r="C23">
         <f>_xll.RealtimeData(A23,"Last")</f>
-        <v>83.15</v>
+        <v>83.14</v>
       </c>
       <c r="D23">
         <f>ROUNDDOWN(($C$3*E23)/B23,0)</f>
@@ -15048,50 +15109,65 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="6"/>
-        <v>1.0835540573079783E-3</v>
+        <f t="shared" si="7"/>
+        <v>9.6315916205158558E-4</v>
       </c>
       <c r="G23">
         <f>D23*C23</f>
-        <v>2910.25</v>
+        <v>2909.9</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="8"/>
-        <v>9.7327339911115335E-2</v>
+        <f t="shared" si="9"/>
+        <v>9.6193673941163779E-2</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="9"/>
-        <v>2.8566959046723586E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>2.8161624201831371E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="11"/>
+        <v>2907.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="72"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>100</v>
       </c>
       <c r="G27">
-        <f>SUM(G20:G23)</f>
-        <v>29901.67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <f>SUM(G20:G23)+J28</f>
+        <v>30250.430000000011</v>
+      </c>
+      <c r="J27">
+        <f>SUM(J20:J23)</f>
+        <v>29645.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>106</v>
       </c>
       <c r="G28" s="8">
-        <f>G27/C3-1</f>
-        <v>-3.2776666666667342E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <f>G27/J27-1</f>
+        <v>2.0408211453911473E-2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28">
+        <f>C3-J27</f>
+        <v>354.58000000000538</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>101</v>
       </c>
       <c r="F31">
         <f>SUM(F13,G27)</f>
-        <v>101874.6866</v>
+        <v>103328.55730000001</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -15100,7 +15176,7 @@
       </c>
       <c r="F33" s="8">
         <f>F31/B1-1</f>
-        <v>1.8746866000000084E-2</v>
+        <v>3.3285573000000124E-2</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -15113,16 +15189,16 @@
       </c>
       <c r="C37">
         <f>_xll.RealtimeData(A37,"Last")</f>
-        <v>38.28</v>
+        <v>38.406599999999997</v>
       </c>
       <c r="D37" s="8">
         <f>C37/B37-1</f>
-        <v>5.2273915316258801E-4</v>
+        <v>3.8316779926816924E-3</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="8">
         <f>D37*$B$3+D40*$B$2</f>
-        <v>3.5084785951765229E-2</v>
+        <v>3.7793798699817888E-2</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -15137,11 +15213,11 @@
       </c>
       <c r="C38">
         <f>_xll.RealtimeData(A38,"Last")</f>
-        <v>285.63</v>
+        <v>286.56</v>
       </c>
       <c r="D38" s="8">
-        <f t="shared" ref="D38:D40" si="10">C38/B38-1</f>
-        <v>4.7299527004729836E-2</v>
+        <f t="shared" ref="D38:D40" si="12">C38/B38-1</f>
+        <v>5.0709492905070874E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -15154,11 +15230,11 @@
       </c>
       <c r="C39">
         <f>_xll.RealtimeData(A39,"Last")</f>
-        <v>180.14</v>
+        <v>181.07</v>
       </c>
       <c r="D39" s="8">
-        <f t="shared" si="10"/>
-        <v>5.9210913153407319E-2</v>
+        <f t="shared" si="12"/>
+        <v>6.4679249720703158E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -15171,11 +15247,11 @@
       </c>
       <c r="C40">
         <f>_xll.RealtimeData(A40,"Last")</f>
-        <v>46.930399999999999</v>
+        <v>47.04</v>
       </c>
       <c r="D40" s="8">
-        <f t="shared" si="10"/>
-        <v>4.9897091722594933E-2</v>
+        <f>C40/B40-1</f>
+        <v>5.2348993288590551E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
08092018 with and without shy
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -1031,299 +1031,533 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
       <tp>
-        <v>5.656108597285125E-3</v>
+        <v>1.8432047186041534E-3</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>change in percent</stp>
+        <tr r="L4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>3.6408788618569744E-3</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>change in percent</stp>
+        <tr r="L5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>2.0183039287329364E-3</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>change in percent</stp>
+        <tr r="K24" s="1"/>
+        <tr r="L3" s="1"/>
+      </tp>
+      <tp>
+        <v>6.5588106689989283E-4</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>change in percent</stp>
+        <tr r="L9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>-1.266784899923922E-3</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>change in percent</stp>
+        <tr r="L6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>3.6092396535131253E-4</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>change in percent</stp>
+        <tr r="L12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>1.3688780355448379E-3</v>
+        <stp/>
+        <stp>ACWI</stp>
+        <stp>change in percent</stp>
+        <tr r="K22" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>2.922267679719503E-3</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>change in percent</stp>
+        <tr r="L2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>4.3512313984855281E-4</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>change in percent</stp>
+        <tr r="L8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>1.5740285292670634E-3</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>change in percent</stp>
+        <tr r="L11" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>1.0080302314596505E-3</v>
+        <stp/>
+        <stp>AGG</stp>
+        <stp>change in percent</stp>
+        <tr r="K23" s="1"/>
+      </tp>
+      <tp>
+        <v>0.64367719000000001</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>0.10835541</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U12" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.20253165000000001</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U6" s="1"/>
+      </tp>
+      <tp>
+        <v>0.46378528000000002</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U11" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.5</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U9" s="1"/>
+      </tp>
+      <tp>
+        <v>1.7922794099999999</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U3" s="1"/>
+      </tp>
+      <tp>
+        <v>1.2266930000000001E-2</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U4" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.15633142</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U8" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.15744489</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U10" s="1"/>
+      </tp>
+      <tp>
+        <v>-0.61110167999999998</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U7" s="1"/>
+      </tp>
+      <tp>
+        <v>0.94117647000000004</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>mtd percent change</stp>
+        <tr r="U2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>-1.7076502732249146E-4</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>change in percent</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>2.9371893357434029E-3</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>change in percent</stp>
+        <tr r="L10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>-5.0761421319796898E-3</v>
         <stp/>
         <stp>GYLD</stp>
         <stp>change in percent</stp>
         <tr r="K26" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
       <tp>
-        <v>1</v>
+        <v>368.35</v>
+        <stp/>
+        <stp>ALGN</stp>
+        <stp>last</stp>
+        <tr r="C5" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>182.41</v>
+        <stp/>
+        <stp>QQQ</stp>
+        <stp>last</stp>
+        <tr r="C39" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>287.95</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>last</stp>
+        <tr r="J3" s="1"/>
+        <tr r="C21" s="4"/>
+        <tr r="C38" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>39.42</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>last</stp>
+        <tr r="J6" s="1"/>
+      </tp>
+      <tp>
+        <v>58.55</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>last</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>50.83</v>
+        <stp/>
+        <stp>STX</stp>
+        <stp>last</stp>
+        <tr r="C10" s="4"/>
+      </tp>
+      <tp>
+        <v>43.93</v>
+        <stp/>
+        <stp>CSCO</stp>
+        <stp>last</stp>
+        <tr r="C7" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>ISHARES TR-20 YR TR BD ETF</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>description</stp>
+        <tr r="B5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>17.11</v>
         <stp/>
         <stp>DBC</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U2" s="1"/>
+        <stp>close</stp>
+        <tr r="G2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>81.53</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>last</stp>
+        <tr r="J4" s="1"/>
+        <tr r="C22" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
+        <stp/>
+        <stp>RWX</stp>
+        <stp>description</stp>
+        <tr r="B6" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>52.15</v>
+        <stp/>
+        <stp>MU</stp>
+        <stp>last</stp>
+        <tr r="C9" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-1 3 YR TREAS BD</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>description</stp>
+        <tr r="B12" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>17.16</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>last</stp>
+        <tr r="J2" s="1"/>
+        <tr r="C20" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>38.529200000000003</v>
+        <stp/>
+        <stp>GAL</stp>
+        <stp>last</stp>
+        <tr r="C37" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>47.072000000000003</v>
+        <stp/>
+        <stp>QQQE</stp>
+        <stp>last</stp>
+        <tr r="C40" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>description</stp>
+        <tr r="B3" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-U.S. REAL ES ETF</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>description</stp>
+        <tr r="B4" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
+        <stp/>
+        <stp>GYLD</stp>
+        <stp>description</stp>
+        <tr r="L26" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>description</stp>
+        <tr r="B11" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>ISHARES TR-EUROPE ETF</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>description</stp>
+        <tr r="B9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>45.77</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>last</stp>
+        <tr r="J9" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>101.81</v>
+        <stp/>
+        <stp>IEF</stp>
+        <stp>last</stp>
+        <tr r="J11" s="1"/>
       </tp>
       <tp>
-        <v>-0.50925140000000002</v>
+        <v>44.39</v>
         <stp/>
-        <stp>EWJ</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U7" s="1"/>
+        <stp>EEM</stp>
+        <stp>last</stp>
+        <tr r="J10" s="1"/>
       </tp>
       <tp>
-        <v>-0.38236617000000001</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U10" s="1"/>
-      </tp>
-      <tp>
-        <v>-0.51241966000000005</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U8" s="1"/>
-      </tp>
-      <tp>
-        <v>1.6597143700000001</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U3" s="1"/>
-      </tp>
-      <tp>
-        <v>-8.58685E-2</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U4" s="1"/>
-      </tp>
-      <tp>
-        <v>-0.52173913000000005</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U9" s="1"/>
-      </tp>
-      <tp>
-        <v>0.27629761000000003</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>5.0632910000000003E-2</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U6" s="1"/>
-      </tp>
-      <tp>
-        <v>7.2236939999999999E-2</v>
-        <stp/>
-        <stp>SHY</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U12" s="1"/>
-      </tp>
-      <tp>
-        <v>0.29545838000000002</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>mtd percent change</stp>
-        <tr r="U5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-2.035278154681221E-4</v>
-        <stp/>
-        <stp>ACWI</stp>
-        <stp>change in percent</stp>
-        <tr r="K22" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>5.9078377313905375E-4</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>change in percent</stp>
-        <tr r="L11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>0</v>
-        <stp/>
-        <stp>AGG</stp>
-        <stp>change in percent</stp>
-        <tr r="K23" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-3.4907059952880967E-4</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>change in percent</stp>
-        <tr r="L8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-8.6605080831408197E-3</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>change in percent</stp>
-        <tr r="L2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-6.7689530685923057E-4</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>change in percent</stp>
-        <tr r="L10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-1.7059024223811006E-4</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>change in percent</stp>
-        <tr r="L7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-1.3094718463553536E-3</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>change in percent</stp>
-        <tr r="L9" s="1"/>
-      </tp>
-      <tp>
-        <v>3.6525550492211707E-4</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>change in percent</stp>
-        <tr r="K24" s="1"/>
-        <tr r="L3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>1.1797421420746694E-3</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>change in percent</stp>
-        <tr r="L5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>-5.1300842799560514E-3</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>change in percent</stp>
-        <tr r="L4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>5.0632911392412905E-4</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>change in percent</stp>
-        <tr r="L6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>1.2032246420412827E-4</v>
-        <stp/>
-        <stp>SHY</stp>
-        <stp>change in percent</stp>
-        <tr r="L12" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>517.48</v>
+        <v>526.24130000000002</v>
         <stp/>
         <stp>ISRG</stp>
         <stp>last</stp>
         <tr r="C8" s="4"/>
       </tp>
     </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>INVESCO DB COMMDY INDX TRCK-UNIT</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>description</stp>
+        <tr r="B2" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>ISHARES INC-MSCI JPN ETF NEW</v>
+        <stp/>
+        <stp>EWJ</stp>
+        <stp>description</stp>
+        <tr r="B7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>ISHARES TR-MSCI EMG MKT ETF</v>
+        <stp/>
+        <stp>EEM</stp>
+        <stp>description</stp>
+        <tr r="B10" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
       <tp>
-        <v>101.62</v>
+        <v>81.38</v>
+        <stp/>
+        <stp>IYR</stp>
+        <stp>close</stp>
+        <tr r="G4" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>83.15</v>
+        <stp/>
+        <stp>SHY</stp>
+        <stp>last</stp>
+        <tr r="J12" s="1"/>
+        <tr r="C23" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp t="s">
+        <v>SPDR GOLD TRUST-GOLD SHS</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>description</stp>
+        <tr r="B8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>287.37</v>
+        <stp/>
+        <stp>IVV</stp>
+        <stp>close</stp>
+        <tr r="G3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>119.2225</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>last</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+      <tp>
+        <v>114.96</v>
+        <stp/>
+        <stp>GLD</stp>
+        <stp>last</stp>
+        <tr r="J8" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>1899.1</v>
+        <stp/>
+        <stp>AMZN</stp>
+        <stp>last</stp>
+        <tr r="C6" s="4"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>118.79</v>
+        <stp/>
+        <stp>TLT</stp>
+        <stp>close</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
+      <tp>
+        <v>4.62</v>
+        <stp/>
+        <stp>IEV</stp>
+        <stp>dividend yield</stp>
+        <tr r="M9" s="1"/>
+      </tp>
+      <tp>
+        <v>2.36</v>
         <stp/>
         <stp>IEF</stp>
-        <stp>last</stp>
-        <tr r="J11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>44.29</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>last</stp>
-        <tr r="J10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>45.76</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>last</stp>
-        <tr r="J9" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>47.181800000000003</v>
-        <stp/>
-        <stp>QQQE</stp>
-        <stp>last</stp>
-        <tr r="C40" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>3.64</v>
-        <stp/>
-        <stp>RWX</stp>
         <stp>dividend yield</stp>
-        <tr r="M6" s="1"/>
-      </tp>
-      <tp>
-        <v>1.99</v>
-        <stp/>
-        <stp>SHY</stp>
-        <stp>dividend yield</stp>
-        <tr r="M12" s="1"/>
-      </tp>
-      <tp>
-        <v>2.7</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>dividend yield</stp>
-        <tr r="M5" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>--</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>dividend yield</stp>
-        <tr r="M2" s="1"/>
-      </tp>
-      <tp>
-        <v>1.57</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>dividend yield</stp>
-        <tr r="M7" s="1"/>
-      </tp>
-      <tp>
-        <v>1.31</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>dividend yield</stp>
-        <tr r="M10" s="1"/>
+        <tr r="M11" s="1"/>
       </tp>
       <tp>
         <v>1.78</v>
@@ -1340,300 +1574,48 @@
         <tr r="M4" s="1"/>
       </tp>
       <tp>
-        <v>2.36</v>
+        <v>1.31</v>
         <stp/>
-        <stp>IEF</stp>
+        <stp>EEM</stp>
         <stp>dividend yield</stp>
-        <tr r="M11" s="1"/>
+        <tr r="M10" s="1"/>
       </tp>
       <tp>
-        <v>4.62</v>
+        <v>1.57</v>
         <stp/>
-        <stp>IEV</stp>
+        <stp>EWJ</stp>
         <stp>dividend yield</stp>
-        <tr r="M9" s="1"/>
+        <tr r="M7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>--</v>
+        <stp/>
+        <stp>DBC</stp>
+        <stp>dividend yield</stp>
+        <tr r="M2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ARROW ETF TR-ARROW DJ GLB YLD</v>
-        <stp/>
-        <stp>GYLD</stp>
-        <stp>description</stp>
-        <tr r="L26" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>SPDR GOLD TRUST-GOLD SHS</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>description</stp>
-        <tr r="B8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
+    <main first="rtdsrv.c8521ef4ac614fa1809b0488ffe291a7">
       <tp>
-        <v>38.413200000000003</v>
-        <stp/>
-        <stp>GAL</stp>
-        <stp>last</stp>
-        <tr r="C37" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>17.170000000000002</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>last</stp>
-        <tr r="J2" s="1"/>
-        <tr r="C20" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-MSCI EMG MKT ETF</v>
-        <stp/>
-        <stp>EEM</stp>
-        <stp>description</stp>
-        <tr r="B10" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES INC-MSCI JPN ETF NEW</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>description</stp>
-        <tr r="B7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>INVESCO DB COMMDY INDX TRCK-UNIT</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>description</stp>
-        <tr r="B2" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>114.55</v>
-        <stp/>
-        <stp>GLD</stp>
-        <stp>last</stp>
-        <tr r="J8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>118.81</v>
+        <v>2.7</v>
         <stp/>
         <stp>TLT</stp>
-        <stp>last</stp>
-        <tr r="J5" s="1"/>
+        <stp>dividend yield</stp>
+        <tr r="M5" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
       <tp>
-        <v>1885.1020000000001</v>
-        <stp/>
-        <stp>AMZN</stp>
-        <stp>last</stp>
-        <tr r="C6" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>118.67</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>close</stp>
-        <tr r="G5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-EUROPE ETF</v>
-        <stp/>
-        <stp>IEV</stp>
-        <stp>description</stp>
-        <tr r="B9" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>ISHARES TR-BARCLAYS 7 10 YR</v>
-        <stp/>
-        <stp>IEF</stp>
-        <stp>description</stp>
-        <tr r="B11" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-CORE S&amp;P500 ETF</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>description</stp>
-        <tr r="B3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-U.S. REAL ES ETF</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>description</stp>
-        <tr r="B4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>287.47000000000003</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>close</stp>
-        <tr r="G3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>83.12</v>
+        <v>1.99</v>
         <stp/>
         <stp>SHY</stp>
-        <stp>last</stp>
-        <tr r="J12" s="1"/>
-        <tr r="C23" s="4"/>
+        <stp>dividend yield</stp>
+        <tr r="M12" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
       <tp>
-        <v>81.87</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>close</stp>
-        <tr r="G4" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>43.66</v>
-        <stp/>
-        <stp>CSCO</stp>
-        <stp>last</stp>
-        <tr r="C7" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>52.89</v>
-        <stp/>
-        <stp>MU</stp>
-        <stp>last</stp>
-        <tr r="C9" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-1 3 YR TREAS BD</v>
-        <stp/>
-        <stp>SHY</stp>
-        <stp>description</stp>
-        <tr r="B12" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>55.276000000000003</v>
-        <stp/>
-        <stp>STX</stp>
-        <stp>last</stp>
-        <tr r="C10" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>SPDR INDEX SHS FDS-DJ INTL RL ETF</v>
+        <v>3.64</v>
         <stp/>
         <stp>RWX</stp>
-        <stp>description</stp>
-        <tr r="B6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>287.57499999999999</v>
-        <stp/>
-        <stp>IVV</stp>
-        <stp>last</stp>
-        <tr r="J3" s="1"/>
-        <tr r="C21" s="4"/>
-        <tr r="C38" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>58.61</v>
-        <stp/>
-        <stp>EWJ</stp>
-        <stp>last</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>39.520000000000003</v>
-        <stp/>
-        <stp>RWX</stp>
-        <stp>last</stp>
-        <tr r="J6" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>365.29500000000002</v>
-        <stp/>
-        <stp>ALGN</stp>
-        <stp>last</stp>
-        <tr r="C5" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>182.11</v>
-        <stp/>
-        <stp>QQQ</stp>
-        <stp>last</stp>
-        <tr r="C39" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp t="s">
-        <v>ISHARES TR-20 YR TR BD ETF</v>
-        <stp/>
-        <stp>TLT</stp>
-        <stp>description</stp>
-        <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>81.45</v>
-        <stp/>
-        <stp>IYR</stp>
-        <stp>last</stp>
-        <tr r="J4" s="1"/>
-        <tr r="C22" s="4"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.837e2ef194634cc8be84be17451153bb">
-      <tp>
-        <v>17.32</v>
-        <stp/>
-        <stp>DBC</stp>
-        <stp>close</stp>
-        <tr r="G2" s="1"/>
+        <stp>dividend yield</stp>
+        <tr r="M6" s="1"/>
       </tp>
     </main>
   </volType>
@@ -1907,7 +1889,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,34 +1989,34 @@
       </c>
       <c r="E2" s="5">
         <f>G2/D2-1</f>
-        <v>-2.8430251248946714E-2</v>
+        <v>-4.0210253976297849E-2</v>
       </c>
       <c r="F2" s="5">
         <f>I2/$I$21</f>
-        <v>0.15192906733917794</v>
+        <v>0.15055309524357086</v>
       </c>
       <c r="G2" s="4">
         <f>_xll.RealtimeData(A2,"Close")</f>
-        <v>17.32</v>
+        <v>17.11</v>
       </c>
       <c r="H2" s="4">
         <v>176</v>
       </c>
       <c r="I2" s="4">
         <f>H2*G2</f>
-        <v>3048.32</v>
+        <v>3011.3599999999997</v>
       </c>
       <c r="J2" s="4">
         <f>_xll.RealtimeData(A2,"Last")</f>
-        <v>17.170000000000002</v>
+        <v>17.16</v>
       </c>
       <c r="K2" s="5">
         <f>J2/D2-1</f>
-        <v>-3.6844538911340208E-2</v>
+        <v>-3.7405491422166537E-2</v>
       </c>
       <c r="L2" s="8">
         <f>_xll.RealtimeData(A2,"Change in Percent")</f>
-        <v>-8.6605080831408197E-3</v>
+        <v>2.922267679719503E-3</v>
       </c>
       <c r="M2" s="29" t="str">
         <f>_xll.RealtimeData(A2,"Dividend Yield")</f>
@@ -2049,7 +2031,7 @@
       </c>
       <c r="P2" s="60">
         <f t="shared" ref="P2:P12" si="1">O2-F2</f>
-        <v>-9.9290673391779494E-3</v>
+        <v>-8.5530952435708685E-3</v>
       </c>
       <c r="Q2" s="31">
         <f>O2*Daily!$D$68</f>
@@ -2057,11 +2039,11 @@
       </c>
       <c r="R2">
         <f t="shared" ref="R2:R11" si="2">ROUND(Q2/J2,0)</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S2">
         <f t="shared" ref="S2:S11" si="3">R2-H2</f>
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="T2" t="str">
         <f t="shared" ref="T2:T12" si="4">A2</f>
@@ -2069,7 +2051,7 @@
       </c>
       <c r="U2">
         <f>_xll.RealtimeData(T2,"MTD Percent Change")</f>
-        <v>1</v>
+        <v>0.94117647000000004</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -2088,34 +2070,34 @@
       </c>
       <c r="E3" s="5">
         <f>G3/D3-1</f>
-        <v>7.9255667622142312E-2</v>
+        <v>7.888023517088727E-2</v>
       </c>
       <c r="F3" s="5">
         <f>I3/$I$21</f>
-        <v>0.41549982306707006</v>
+        <v>0.41664525212004005</v>
       </c>
       <c r="G3" s="4">
         <f>_xll.RealtimeData(A3,"Close")</f>
-        <v>287.47000000000003</v>
+        <v>287.37</v>
       </c>
       <c r="H3" s="4">
         <v>29</v>
       </c>
       <c r="I3" s="4">
         <f>H3*G3</f>
-        <v>8336.630000000001</v>
+        <v>8333.73</v>
       </c>
       <c r="J3" s="4">
         <f>_xll.RealtimeData(A3,"Last")</f>
-        <v>287.57499999999999</v>
+        <v>287.95</v>
       </c>
       <c r="K3" s="5">
         <f>J3/D3-1</f>
-        <v>7.9649871695959717E-2</v>
+        <v>8.1057743388165182E-2</v>
       </c>
       <c r="L3" s="8">
         <f>_xll.RealtimeData(A3,"Change in Percent")</f>
-        <v>3.6525550492211707E-4</v>
+        <v>2.0183039287329364E-3</v>
       </c>
       <c r="M3" s="29">
         <f>_xll.RealtimeData(A3,"Dividend Yield")</f>
@@ -2130,7 +2112,7 @@
       </c>
       <c r="P3" s="60">
         <f t="shared" si="1"/>
-        <v>-4.949982306707007E-2</v>
+        <v>-5.0645252120040063E-2</v>
       </c>
       <c r="Q3" s="31">
         <f>O3*Daily!$D$68</f>
@@ -2150,7 +2132,7 @@
       </c>
       <c r="U3">
         <f>_xll.RealtimeData(T3,"MTD Percent Change")</f>
-        <v>1.6597143700000001</v>
+        <v>1.7922794099999999</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -2169,34 +2151,34 @@
       </c>
       <c r="E4" s="5">
         <f>G4/D4-1</f>
-        <v>4.3860767563432379E-2</v>
+        <v>3.7613158230268784E-2</v>
       </c>
       <c r="F4" s="5">
         <f>I4/$I$21</f>
-        <v>0.22034280132176376</v>
+        <v>0.21970424927932128</v>
       </c>
       <c r="G4" s="4">
         <f>_xll.RealtimeData(A4,"Close")</f>
-        <v>81.87</v>
+        <v>81.38</v>
       </c>
       <c r="H4" s="4">
         <v>54</v>
       </c>
       <c r="I4" s="4">
         <f>H4*G4</f>
-        <v>4420.9800000000005</v>
+        <v>4394.5199999999995</v>
       </c>
       <c r="J4" s="4">
         <f>_xll.RealtimeData(A4,"Last")</f>
-        <v>81.45</v>
+        <v>81.53</v>
       </c>
       <c r="K4" s="5">
         <f>J4/D4-1</f>
-        <v>3.8505673849292377E-2</v>
+        <v>3.9525691699604737E-2</v>
       </c>
       <c r="L4" s="8">
         <f t="array" ref="L4">_xll.RealtimeData(A4,"Change in Percent")</f>
-        <v>-5.1300842799560514E-3</v>
+        <v>1.8432047186041534E-3</v>
       </c>
       <c r="M4" s="29">
         <f>_xll.RealtimeData(A4,"Dividend Yield")</f>
@@ -2211,7 +2193,7 @@
       </c>
       <c r="P4" s="60">
         <f t="shared" si="1"/>
-        <v>0.17265719867823626</v>
+        <v>0.17329575072067874</v>
       </c>
       <c r="Q4" s="31">
         <f>O4*Daily!$D$68</f>
@@ -2231,7 +2213,7 @@
       </c>
       <c r="U4">
         <f>_xll.RealtimeData(T4,"MTD Percent Change")</f>
-        <v>-8.58685E-2</v>
+        <v>1.2266930000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -2250,34 +2232,34 @@
       </c>
       <c r="E5" s="5">
         <f>G5/D5-1</f>
-        <v>-2.9631919197866119E-2</v>
+        <v>-2.8650675667940662E-2</v>
       </c>
       <c r="F5" s="5">
         <f>I5/$I$21</f>
-        <v>0.20700903603949339</v>
+        <v>0.2078619216697547</v>
       </c>
       <c r="G5" s="4">
         <f>_xll.RealtimeData(A5,"Close")</f>
-        <v>118.67</v>
+        <v>118.79</v>
       </c>
       <c r="H5" s="4">
         <v>35</v>
       </c>
       <c r="I5" s="4">
         <f>H5*G5</f>
-        <v>4153.45</v>
+        <v>4157.6500000000005</v>
       </c>
       <c r="J5" s="31">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>118.81</v>
+        <v>119.2225</v>
       </c>
       <c r="K5" s="5">
         <f>J5/D5-1</f>
-        <v>-2.8487135079619752E-2</v>
+        <v>-2.5114110445500937E-2</v>
       </c>
       <c r="L5" s="8">
         <f t="array" ref="L5">_xll.RealtimeData(A5,"Change in Percent")</f>
-        <v>1.1797421420746694E-3</v>
+        <v>3.6408788618569744E-3</v>
       </c>
       <c r="M5" s="29">
         <f>_xll.RealtimeData(A5,"Dividend Yield")</f>
@@ -2292,7 +2274,7 @@
       </c>
       <c r="P5" s="60">
         <f t="shared" si="1"/>
-        <v>-0.20700903603949339</v>
+        <v>-0.2078619216697547</v>
       </c>
       <c r="Q5" s="31">
         <f>O5*Daily!$D$68</f>
@@ -2312,7 +2294,7 @@
       </c>
       <c r="U5">
         <f>_xll.RealtimeData(T5,"MTD Percent Change")</f>
-        <v>0.29545838000000002</v>
+        <v>0.64367719000000001</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -2332,12 +2314,12 @@
       <c r="I6" s="4"/>
       <c r="J6" s="31">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>39.520000000000003</v>
+        <v>39.42</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="8">
         <f>_xll.RealtimeData(A6,"Change in Percent")</f>
-        <v>5.0632911392412905E-4</v>
+        <v>-1.266784899923922E-3</v>
       </c>
       <c r="M6" s="29">
         <f>_xll.RealtimeData(A6,"Dividend Yield")</f>
@@ -2372,7 +2354,7 @@
       </c>
       <c r="U6">
         <f>_xll.RealtimeData(T6,"MTD Percent Change")</f>
-        <v>5.0632910000000003E-2</v>
+        <v>-0.20253165000000001</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2392,12 +2374,12 @@
       <c r="I7" s="4"/>
       <c r="J7" s="31">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>58.61</v>
+        <v>58.55</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="8">
         <f>_xll.RealtimeData(A7,"Change in Percent")</f>
-        <v>-1.7059024223811006E-4</v>
+        <v>-1.7076502732249146E-4</v>
       </c>
       <c r="M7" s="29">
         <f>_xll.RealtimeData(A7,"Dividend Yield")</f>
@@ -2432,7 +2414,7 @@
       </c>
       <c r="U7">
         <f>_xll.RealtimeData(T7,"MTD Percent Change")</f>
-        <v>-0.50925140000000002</v>
+        <v>-0.61110167999999998</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2452,12 +2434,12 @@
       <c r="I8" s="4"/>
       <c r="J8" s="31">
         <f>_xll.RealtimeData(A8,"Last")</f>
-        <v>114.55</v>
+        <v>114.96</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="8">
         <f>_xll.RealtimeData(A8,"Change in Percent")</f>
-        <v>-3.4907059952880967E-4</v>
+        <v>4.3512313984855281E-4</v>
       </c>
       <c r="M8" s="29">
         <v>0</v>
@@ -2491,7 +2473,7 @@
       </c>
       <c r="U8">
         <f>_xll.RealtimeData(T8,"MTD Percent Change")</f>
-        <v>-0.51241966000000005</v>
+        <v>-0.15633142</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2511,12 +2493,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="31">
         <f>_xll.RealtimeData(A9,"Last")</f>
-        <v>45.76</v>
+        <v>45.77</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="8">
         <f>_xll.RealtimeData(A9,"Change in Percent")</f>
-        <v>-1.3094718463553536E-3</v>
+        <v>6.5588106689989283E-4</v>
       </c>
       <c r="M9" s="29">
         <f>_xll.RealtimeData(A9,"Dividend Yield")</f>
@@ -2551,7 +2533,7 @@
       </c>
       <c r="U9">
         <f>_xll.RealtimeData(T9,"MTD Percent Change")</f>
-        <v>-0.52173913000000005</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2565,12 +2547,12 @@
       <c r="G10" s="4"/>
       <c r="J10" s="31">
         <f>_xll.RealtimeData(A10,"Last")</f>
-        <v>44.29</v>
+        <v>44.39</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="8">
         <f t="array" ref="L10">_xll.RealtimeData(A10,"Change in Percent")</f>
-        <v>-6.7689530685923057E-4</v>
+        <v>2.9371893357434029E-3</v>
       </c>
       <c r="M10" s="29">
         <f>_xll.RealtimeData(A10,"Dividend Yield")</f>
@@ -2605,7 +2587,7 @@
       </c>
       <c r="U10">
         <f>_xll.RealtimeData(T10,"MTD Percent Change")</f>
-        <v>-0.38236617000000001</v>
+        <v>-0.15744489</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2619,12 +2601,12 @@
       <c r="G11" s="4"/>
       <c r="J11" s="31">
         <f>_xll.RealtimeData(A11,"Last")</f>
-        <v>101.62</v>
+        <v>101.81</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="8">
         <f t="array" ref="L11">_xll.RealtimeData(A11,"Change in Percent")</f>
-        <v>5.9078377313905375E-4</v>
+        <v>1.5740285292670634E-3</v>
       </c>
       <c r="M11" s="29">
         <f>_xll.RealtimeData(A11,"Dividend Yield")</f>
@@ -2659,7 +2641,7 @@
       </c>
       <c r="U11">
         <f>_xll.RealtimeData(T11,"MTD Percent Change")</f>
-        <v>0.27629761000000003</v>
+        <v>0.46378528000000002</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2672,11 +2654,11 @@
       </c>
       <c r="J12" s="31">
         <f>_xll.RealtimeData(A12,"Last")</f>
-        <v>83.12</v>
+        <v>83.15</v>
       </c>
       <c r="L12" s="8">
         <f t="array" ref="L12">_xll.RealtimeData(A12,"Change in Percent")</f>
-        <v>1.2032246420412827E-4</v>
+        <v>3.6092396535131253E-4</v>
       </c>
       <c r="M12" s="29">
         <f>_xll.RealtimeData(A12,"Dividend Yield")</f>
@@ -2711,7 +2693,7 @@
       </c>
       <c r="U12">
         <f>_xll.RealtimeData(T12,"MTD Percent Change")</f>
-        <v>7.2236939999999999E-2</v>
+        <v>0.10835541</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -2728,11 +2710,11 @@
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U14" s="29">
         <f t="array" ref="U14">MMULT(TRANSPOSE(O2:O12),U2:U12)</f>
-        <v>0.72286059597999996</v>
+        <v>0.80516941187999991</v>
       </c>
       <c r="V14" s="8">
         <f>U14*0.01</f>
-        <v>7.2286059597999998E-3</v>
+        <v>8.0516941187999992E-3</v>
       </c>
     </row>
     <row r="19" spans="5:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2742,7 +2724,7 @@
       </c>
       <c r="F20" s="11">
         <f>SUM(F2:F5)</f>
-        <v>0.99478072776750515</v>
+        <v>0.99476451831268686</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>14</v>
@@ -2761,32 +2743,32 @@
       </c>
       <c r="F21" s="11">
         <f>1-F20</f>
-        <v>5.2192722324948537E-3</v>
+        <v>5.2354816873131371E-3</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="6">
         <f>SUM(I2:I20)</f>
-        <v>20064.100000000002</v>
+        <v>20001.980000000003</v>
       </c>
       <c r="J21" t="s">
         <v>33</v>
       </c>
       <c r="K21" s="8">
         <f>SUMPRODUCT(K2:K7,F2:F7)</f>
-        <v>3.0084104834020471E-2</v>
+        <v>3.1604506581408849E-2</v>
       </c>
       <c r="M21" t="s">
         <v>34</v>
       </c>
       <c r="N21" s="8">
         <f t="array" ref="N21">MMULT(TRANSPOSE(F2:F5),L2:L5)</f>
-        <v>-2.0501791757417988E-3</v>
+        <v>2.4426331793152289E-3</v>
       </c>
       <c r="P21" s="8">
         <f t="array" ref="P21">SUMPRODUCT(L2:L12,O2:O12)</f>
-        <v>-3.1003198310710208E-3</v>
+        <v>1.9137721754176364E-3</v>
       </c>
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
@@ -2801,7 +2783,7 @@
       </c>
       <c r="K22" s="8">
         <f>_xll.RealtimeData(J22,"Change in Percent")</f>
-        <v>-2.035278154681221E-4</v>
+        <v>1.3688780355448379E-3</v>
       </c>
       <c r="L22" s="12">
         <v>0.6</v>
@@ -2813,7 +2795,7 @@
       </c>
       <c r="K23" s="8">
         <f>_xll.RealtimeData(J23,"Change in Percent")</f>
-        <v>0</v>
+        <v>1.0080302314596505E-3</v>
       </c>
       <c r="L23" s="12">
         <v>0.4</v>
@@ -2825,7 +2807,7 @@
       </c>
       <c r="K24" s="8">
         <f>_xll.RealtimeData(J24,"Change in Percent")</f>
-        <v>3.6525550492211707E-4</v>
+        <v>2.0183039287329364E-3</v>
       </c>
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
@@ -2834,7 +2816,7 @@
       </c>
       <c r="K25" s="8">
         <f t="array" ref="K25">SUMPRODUCT(K22:K23,L22:L23)</f>
-        <v>-1.2211668928087326E-4</v>
+        <v>1.2245389139107629E-3</v>
       </c>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
@@ -2843,14 +2825,14 @@
       </c>
       <c r="I26" s="6">
         <f>SUM(I2:I18)</f>
-        <v>19959.38</v>
+        <v>19897.260000000002</v>
       </c>
       <c r="J26" t="s">
         <v>56</v>
       </c>
       <c r="K26" s="8">
         <f>_xll.RealtimeData(J26,"Change in Percent")</f>
-        <v>5.656108597285125E-3</v>
+        <v>-5.0761421319796898E-3</v>
       </c>
       <c r="L26" t="str">
         <f>_xll.RealtimeData(J26,"Description")</f>
@@ -2863,7 +2845,7 @@
       </c>
       <c r="K27" s="8">
         <f>AVERAGE(L2:L11)</f>
-        <v>-1.3654509824018407E-3</v>
+        <v>1.4589327333426067E-3</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
@@ -2872,7 +2854,7 @@
       </c>
       <c r="K28" s="8">
         <f>SUMPRODUCT(F2:F7,M2:M7)*0.01</f>
-        <v>1.4064820550136812E-2</v>
+        <v>1.4105108194288766E-2</v>
       </c>
       <c r="L28" t="s">
         <v>65</v>
@@ -2885,7 +2867,7 @@
     <row r="29" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="5:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H30" s="30">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>61</v>
@@ -2906,19 +2888,19 @@
       </c>
       <c r="I31" s="21">
         <f>$N$21</f>
-        <v>-2.0501791757417988E-3</v>
+        <v>2.4426331793152289E-3</v>
       </c>
       <c r="J31" s="21">
         <f>LOOKUP(2,1/(Daily!E:E&lt;&gt;""),Daily!E:E)</f>
-        <v>-3.3668471564133329E-3</v>
+        <v>1.2018238089255284E-3</v>
       </c>
       <c r="K31" s="22">
         <f>VLOOKUP($H$30,Daily!$A:$AF,7,0)</f>
-        <v>6.5300105399139774E-3</v>
+        <v>7.739682270978987E-3</v>
       </c>
       <c r="L31" s="23">
         <f>VLOOKUP($H$30,Daily!$A:$AF,8,0)</f>
-        <v>-1.1014999999998665E-3</v>
+        <v>9.9000000000071253E-5</v>
       </c>
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.25">
@@ -2927,19 +2909,19 @@
       </c>
       <c r="I32" s="24">
         <f>$K$25</f>
-        <v>-1.2211668928087326E-4</v>
+        <v>1.2245389139107629E-3</v>
       </c>
       <c r="J32" s="24">
         <f>LOOKUP(2,1/(Daily!M:M&lt;&gt;""),Daily!M:M)</f>
-        <v>2.0640963040633674E-3</v>
+        <v>8.141112618722523E-5</v>
       </c>
       <c r="K32" s="14">
         <f>VLOOKUP($H$30,Daily!$A:$AF,25,0)</f>
-        <v>2.0770348177892251E-2</v>
+        <v>2.0853450241516081E-2</v>
       </c>
       <c r="L32" s="25">
         <f>VLOOKUP($H$30,Daily!$A:$AF,31,0)</f>
-        <v>1.4909969171992055E-2</v>
+        <v>1.4992594135561088E-2</v>
       </c>
     </row>
     <row r="33" spans="8:18" x14ac:dyDescent="0.25">
@@ -2948,19 +2930,19 @@
       </c>
       <c r="I33" s="24">
         <f>$K$24</f>
-        <v>3.6525550492211707E-4</v>
+        <v>2.0183039287329364E-3</v>
       </c>
       <c r="J33" s="24">
         <f>LOOKUP(2,1/(Daily!L:L&lt;&gt;""),Daily!L:L)</f>
-        <v>2.8606314320602788E-3</v>
+        <v>-3.4786238564032956E-4</v>
       </c>
       <c r="K33" s="14">
         <f>VLOOKUP($H$30,Daily!$A:$AF,24,0)</f>
-        <v>5.2810840505401746E-2</v>
+        <v>5.2444607214795713E-2</v>
       </c>
       <c r="L33" s="25">
         <f>VLOOKUP($H$30,Daily!$A:$AF,30,0)</f>
-        <v>7.9553775118956116E-2</v>
+        <v>7.917823896731635E-2</v>
       </c>
     </row>
     <row r="34" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2969,19 +2951,19 @@
       </c>
       <c r="I34" s="26">
         <f>$K$26</f>
-        <v>5.656108597285125E-3</v>
+        <v>-5.0761421319796898E-3</v>
       </c>
       <c r="J34" s="26">
         <f>LOOKUP(2,1/(Daily!N:N&lt;&gt;""),Daily!N:N)</f>
-        <v>1.1325028312569874E-3</v>
+        <v>2.8280542986425239E-3</v>
       </c>
       <c r="K34" s="27">
         <f>VLOOKUP($H$30,Daily!$A:$AF,26,0)</f>
-        <v>1.6091954022988686E-2</v>
+        <v>1.8965517241379404E-2</v>
       </c>
       <c r="L34" s="28">
         <f>VLOOKUP($H$30,Daily!$A:$AF,32,0)</f>
-        <v>2.5357740602259149E-2</v>
+        <v>2.8257507968215689E-2</v>
       </c>
     </row>
     <row r="35" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3016,7 +2998,7 @@
       </c>
       <c r="I37" s="46">
         <f>AVERAGE(Daily!E$3:E380)</f>
-        <v>-3.3586273287622106E-6</v>
+        <v>1.3858264617727656E-5</v>
       </c>
       <c r="J37" s="44"/>
       <c r="K37" s="22"/>
@@ -3024,23 +3006,23 @@
       <c r="M37" s="50"/>
       <c r="N37" s="38">
         <f>AVERAGE(Daily!J$3:J380)</f>
-        <v>3.5881890795098892E-4</v>
+        <v>3.5563128369900398E-4</v>
       </c>
       <c r="O37" s="22">
         <f>AVERAGE(Daily!K$3:K380)</f>
-        <v>1.3922856108751321E-5</v>
+        <v>1.3723958164340587E-5</v>
       </c>
       <c r="P37" s="22">
         <f>AVERAGE(Daily!L$3:L380)</f>
-        <v>1.1269554414813654E-3</v>
+        <v>1.1058866153796267E-3</v>
       </c>
       <c r="Q37" s="22">
         <f>AVERAGE(Daily!M$3:M380)</f>
-        <v>2.2086048721409385E-4</v>
+        <v>2.1886835348513859E-4</v>
       </c>
       <c r="R37" s="23">
         <f>AVERAGE(Daily!N$3:N380)</f>
-        <v>3.954067915191361E-4</v>
+        <v>4.3015889876375589E-4</v>
       </c>
     </row>
     <row r="38" spans="8:18" x14ac:dyDescent="0.25">
@@ -3049,7 +3031,7 @@
       </c>
       <c r="I38" s="47">
         <f>STDEV(Daily!E$3:E380)</f>
-        <v>5.0577016885652182E-3</v>
+        <v>5.0229837953902016E-3</v>
       </c>
       <c r="J38" s="45"/>
       <c r="K38" s="14"/>
@@ -3057,23 +3039,23 @@
       <c r="M38" s="51"/>
       <c r="N38" s="40">
         <f>STDEV(Daily!J$3:J380)</f>
-        <v>6.1213821536002747E-3</v>
+        <v>6.0769209420381181E-3</v>
       </c>
       <c r="O38" s="14">
         <f>STDEV(Daily!K$3:K380)</f>
-        <v>1.7914487310597524E-3</v>
+        <v>1.7784206186656198E-3</v>
       </c>
       <c r="P38" s="14">
         <f>STDEV(Daily!L$3:L380)</f>
-        <v>5.8639362604379613E-3</v>
+        <v>5.8239571569626879E-3</v>
       </c>
       <c r="Q38" s="14">
         <f>STDEV(Daily!M$3:M380)</f>
-        <v>3.5874621670105053E-3</v>
+        <v>3.5614101886676805E-3</v>
       </c>
       <c r="R38" s="25">
         <f>STDEV(Daily!N$3:N380)</f>
-        <v>8.1118091330334013E-3</v>
+        <v>8.0580607389400243E-3</v>
       </c>
     </row>
     <row r="39" spans="8:18" x14ac:dyDescent="0.25">
@@ -3082,7 +3064,7 @@
       </c>
       <c r="I39" s="48">
         <f>COUNTIF(Daily!E$3:E380,"&gt;0")</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J39" s="45"/>
       <c r="K39" s="14"/>
@@ -3090,7 +3072,7 @@
       <c r="M39" s="51"/>
       <c r="N39" s="41">
         <f>COUNTIF(Daily!J$3:J380,"&gt;0")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O39" s="33">
         <f>COUNTIF(Daily!K$3:K380,"&gt;0")</f>
@@ -3102,11 +3084,11 @@
       </c>
       <c r="Q39" s="33">
         <f>COUNTIF(Daily!M$3:M380,"&gt;0")</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R39" s="35">
         <f>COUNTIF(Daily!N$3:N380,"&gt;0")</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="8:18" x14ac:dyDescent="0.25">
@@ -3115,7 +3097,7 @@
       </c>
       <c r="I40" s="47">
         <f>SUMIF(Daily!E$3:E380,"&gt;0")</f>
-        <v>0.12857105398003066</v>
+        <v>0.12977287778895619</v>
       </c>
       <c r="J40" s="45"/>
       <c r="K40" s="14"/>
@@ -3123,7 +3105,7 @@
       <c r="M40" s="51"/>
       <c r="N40" s="40">
         <f>SUMIF(Daily!J$3:J380,"&gt;0")</f>
-        <v>0.17542992070108321</v>
+        <v>0.17556560591139525</v>
       </c>
       <c r="O40" s="14">
         <f>SUMIF(Daily!K$3:K380,"&gt;0")</f>
@@ -3135,11 +3117,11 @@
       </c>
       <c r="Q40" s="14">
         <f>SUMIF(Daily!M$3:M380,"&gt;0")</f>
-        <v>0.10314608985556732</v>
+        <v>0.10322750098175455</v>
       </c>
       <c r="R40" s="25">
         <f>SUMIF(Daily!N$3:N380,"&gt;0")</f>
-        <v>0.23054367253914801</v>
+        <v>0.23337172683779053</v>
       </c>
     </row>
     <row r="41" spans="8:18" x14ac:dyDescent="0.25">
@@ -3164,7 +3146,7 @@
       </c>
       <c r="P41" s="14">
         <f>SUMIF(Daily!L$3:L380,"&lt;0")</f>
-        <v>-0.12390186245204478</v>
+        <v>-0.12424972483768511</v>
       </c>
       <c r="Q41" s="14">
         <f>SUMIF(Daily!M$3:M380,"&lt;0")</f>
@@ -3181,7 +3163,7 @@
       </c>
       <c r="I42" s="48">
         <f>COUNT(Daily!E$3:E380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J42" s="45"/>
       <c r="K42" s="14"/>
@@ -3189,23 +3171,23 @@
       <c r="M42" s="51"/>
       <c r="N42" s="41">
         <f>COUNT(Daily!J$3:J380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O42" s="33">
         <f>COUNT(Daily!K$3:K380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P42" s="33">
         <f>COUNT(Daily!L$3:L380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q42" s="33">
         <f>COUNT(Daily!M$3:M380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R42" s="35">
         <f>COUNT(Daily!N$3:N380)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="8:18" x14ac:dyDescent="0.25">
@@ -3226,11 +3208,11 @@
       </c>
       <c r="O43" s="33">
         <f>O42-O39</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P43" s="33">
         <f>P42-P39</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q43" s="33">
         <f>Q42-Q39</f>
@@ -3247,7 +3229,7 @@
       </c>
       <c r="I44" s="49">
         <f>(I40/I41)*(I39/I43)*-1</f>
-        <v>1.2976610068018128</v>
+        <v>1.3433753358236642</v>
       </c>
       <c r="J44" s="45"/>
       <c r="K44" s="14"/>
@@ -3255,23 +3237,23 @@
       <c r="M44" s="51"/>
       <c r="N44" s="42">
         <f>(N40/N41)*(N39/N43)*-1</f>
-        <v>1.1985659190209796</v>
+        <v>1.2337641695070358</v>
       </c>
       <c r="O44" s="34">
         <f>(O40/O41)*(O39/O43)*-1</f>
-        <v>1.0504767113497246</v>
+        <v>1.0204630910254469</v>
       </c>
       <c r="P44" s="34">
         <f>(P40/P41)*(P39/P43)*-1</f>
-        <v>2.383260988303987</v>
+        <v>2.2946372344460482</v>
       </c>
       <c r="Q44" s="34">
         <f>(Q40/Q41)*(Q39/Q43)*-1</f>
-        <v>1.3566957281498768</v>
+        <v>1.3944629336879948</v>
       </c>
       <c r="R44" s="36">
         <f>(R40/R41)*(R39/R43)*-1</f>
-        <v>1.5644510855934295</v>
+        <v>1.6232330888179249</v>
       </c>
     </row>
     <row r="45" spans="8:18" x14ac:dyDescent="0.25">
@@ -3280,7 +3262,7 @@
       </c>
       <c r="I45" s="62">
         <f>I39/I42</f>
-        <v>0.56521739130434778</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J45" s="63"/>
       <c r="K45" s="64"/>
@@ -3288,23 +3270,23 @@
       <c r="M45" s="66"/>
       <c r="N45" s="67">
         <f>N39/N42</f>
-        <v>0.50724637681159424</v>
+        <v>0.51428571428571423</v>
       </c>
       <c r="O45" s="64">
         <f>O39/O42</f>
-        <v>0.50724637681159424</v>
+        <v>0.5</v>
       </c>
       <c r="P45" s="64">
         <f>P39/P42</f>
-        <v>0.59420289855072461</v>
+        <v>0.58571428571428574</v>
       </c>
       <c r="Q45" s="64">
         <f>Q39/Q42</f>
-        <v>0.53623188405797106</v>
+        <v>0.54285714285714282</v>
       </c>
       <c r="R45" s="68">
         <f>R39/R42</f>
-        <v>0.57971014492753625</v>
+        <v>0.58571428571428574</v>
       </c>
     </row>
     <row r="46" spans="8:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3355,10 +3337,10 @@
   <dimension ref="A1:AN72"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E85" sqref="E85"/>
+      <selection pane="bottomRight" activeCell="V83" sqref="V83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9374,7 +9356,7 @@
         <v>43291</v>
       </c>
       <c r="B51" s="4">
-        <f t="shared" ref="B51:B71" si="812">D51-C51</f>
+        <f t="shared" ref="B51:B72" si="812">D51-C51</f>
         <v>19902.79</v>
       </c>
       <c r="C51" s="4">
@@ -12226,7 +12208,140 @@
       </c>
     </row>
     <row r="72" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="A72" s="9">
+        <v>43320</v>
+      </c>
+      <c r="B72" s="4">
+        <f t="shared" si="812"/>
+        <v>19897.259999999998</v>
+      </c>
+      <c r="C72" s="4">
+        <v>104.72</v>
+      </c>
+      <c r="D72" s="4">
+        <f>20007.38-5.4</f>
+        <v>20001.98</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" ref="E72" si="1258">D72/D71-1</f>
+        <v>1.2018238089255284E-3</v>
+      </c>
+      <c r="F72" s="10">
+        <f t="shared" ref="F72" si="1259">F71*(1+E72)</f>
+        <v>100.00990000000002</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" ref="G72" si="1260">F72/F$45-1</f>
+        <v>7.739682270978987E-3</v>
+      </c>
+      <c r="H72" s="8">
+        <f t="shared" ref="H72" si="1261">F72/$F$2-1</f>
+        <v>9.9000000000071253E-5</v>
+      </c>
+      <c r="J72" s="11">
+        <f>VLOOKUP($A72,Prices!$A:$J,MATCH(J$1,Prices!$1:$1,0),0)</f>
+        <v>1.3568521031204206E-4</v>
+      </c>
+      <c r="K72" s="11">
+        <f>VLOOKUP($A72,Prices!$A:$J,MATCH(K$1,Prices!$1:$1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L72" s="11">
+        <f>VLOOKUP($A72,Prices!$A:$J,MATCH(L$1,Prices!$1:$1,0),0)</f>
+        <v>-3.4786238564032956E-4</v>
+      </c>
+      <c r="M72" s="11">
+        <f t="shared" ref="M72" si="1262">0.6*J72 + 0.4*K72</f>
+        <v>8.141112618722523E-5</v>
+      </c>
+      <c r="N72" s="11">
+        <f>VLOOKUP($A72,Prices!$A:$J,MATCH(N$1,Prices!$1:$1,0),0)</f>
+        <v>2.8280542986425239E-3</v>
+      </c>
+      <c r="P72" s="10">
+        <f t="shared" ref="P72" si="1263">P71*(1+J72)</f>
+        <v>102.38954389258075</v>
+      </c>
+      <c r="Q72" s="10">
+        <f t="shared" ref="Q72" si="1264">Q71*(1+K72)</f>
+        <v>100.08519683921634</v>
+      </c>
+      <c r="R72" s="10">
+        <f t="shared" ref="R72" si="1265">R71*(1+L72)</f>
+        <v>107.91782389673163</v>
+      </c>
+      <c r="S72" s="10">
+        <f t="shared" ref="S72" si="1266">S71*(1+M72)</f>
+        <v>101.4992594135561</v>
+      </c>
+      <c r="T72" s="10">
+        <f t="shared" ref="T72" si="1267">T71*(1+N72)</f>
+        <v>102.82575079682157</v>
+      </c>
+      <c r="V72" s="5">
+        <f t="shared" ref="V72" si="1268">P72/P$45-1</f>
+        <v>3.6417322834645605E-2</v>
+      </c>
+      <c r="W72" s="5">
+        <f t="shared" ref="W72" si="1269">Q72/Q$45-1</f>
+        <v>-2.2697538335092471E-3</v>
+      </c>
+      <c r="X72" s="5">
+        <f t="shared" ref="X72" si="1270">R72/R$45-1</f>
+        <v>5.2444607214795713E-2</v>
+      </c>
+      <c r="Y72" s="5">
+        <f t="shared" ref="Y72" si="1271">S72/S$45-1</f>
+        <v>2.0853450241516081E-2</v>
+      </c>
+      <c r="Z72" s="5">
+        <f t="shared" ref="Z72" si="1272">T72/T$45-1</f>
+        <v>1.8965517241379404E-2</v>
+      </c>
+      <c r="AB72" s="8">
+        <f t="shared" ref="AB72" si="1273">P72/$P$2-1</f>
+        <v>2.3895438925807477E-2</v>
+      </c>
+      <c r="AC72" s="8">
+        <f t="shared" ref="AC72" si="1274">Q72/$P$2-1</f>
+        <v>8.5196839216328257E-4</v>
+      </c>
+      <c r="AD72" s="8">
+        <f t="shared" ref="AD72" si="1275">R72/$P$2-1</f>
+        <v>7.917823896731635E-2</v>
+      </c>
+      <c r="AE72" s="8">
+        <f t="shared" ref="AE72" si="1276">S72/$P$2-1</f>
+        <v>1.4992594135561088E-2</v>
+      </c>
+      <c r="AF72" s="8">
+        <f t="shared" ref="AF72" si="1277">T72/$T$2-1</f>
+        <v>2.8257507968215689E-2</v>
+      </c>
+      <c r="AI72" s="8">
+        <f t="shared" ref="AI72" si="1278">MIN(0,(F72-MAX(F43:F72))/MAX(F43:F72))</f>
+        <v>-2.169069704561368E-3</v>
+      </c>
+      <c r="AJ72" s="8">
+        <f t="shared" ref="AJ72" si="1279">MIN(0,(P72-MAX(P43:P72))/MAX(P43:P72))</f>
+        <v>-2.3010286951812803E-3</v>
+      </c>
+      <c r="AK72" s="8">
+        <f t="shared" ref="AK72" si="1280">MIN(0,(Q72-MAX(Q43:Q72))/MAX(Q43:Q72))</f>
+        <v>-6.1966012580979037E-3</v>
+      </c>
+      <c r="AL72" s="8">
+        <f t="shared" ref="AL72" si="1281">MIN(0,(R72-MAX(R43:R72))/MAX(R43:R72))</f>
+        <v>-3.4786238564029221E-4</v>
+      </c>
+      <c r="AM72" s="8">
+        <f t="shared" ref="AM72" si="1282">MIN(0,(S72-MAX(S43:S72))/MAX(S43:S72))</f>
+        <v>-2.1628375853489398E-3</v>
+      </c>
+      <c r="AN72" s="8">
+        <f t="shared" ref="AN72" si="1283">MIN(0,(T72-MAX(T43:T72))/MAX(T43:T72))</f>
+        <v>-8.9435438792623365E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12239,7 +12354,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14864,37 +14979,40 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B73" t="str">
+      <c r="A73" s="13">
+        <v>43320</v>
+      </c>
+      <c r="B73">
         <f t="array" ref="B73">_xll.HistoricalData(B$1,"Adj. Close",$A73,$A73,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
-        <v>--</v>
-      </c>
-      <c r="C73" t="str">
+        <v>73.709999999999994</v>
+      </c>
+      <c r="C73">
         <f t="array" ref="C73">_xll.HistoricalData(C$1,"Adj. Close",$A73,$A73,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
-        <v>--</v>
-      </c>
-      <c r="D73" t="str">
+        <v>105.85</v>
+      </c>
+      <c r="D73">
         <f t="array" ref="D73">_xll.HistoricalData(D$1,"Adj. Close",$A73,$A73,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
-        <v>--</v>
-      </c>
-      <c r="E73" t="str">
+        <v>287.37</v>
+      </c>
+      <c r="E73">
         <f t="array" ref="E73">_xll.HistoricalData(E$1,"Adj. Close",$A73,$A73,"Daily","RemoveHeaders = True","ReverseOrder =True","RemoveDates =""True")</f>
-        <v>--</v>
-      </c>
-      <c r="G73" s="5" t="e">
+        <v>17.73</v>
+      </c>
+      <c r="G73" s="5">
         <f t="shared" ref="G73:G78" si="220">B73/B72-1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H73" s="5" t="e">
+        <v>1.3568521031204206E-4</v>
+      </c>
+      <c r="H73" s="5">
         <f t="shared" ref="H73:H78" si="221">C73/C72-1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I73" s="5" t="e">
+        <v>0</v>
+      </c>
+      <c r="I73" s="5">
         <f t="shared" ref="I73:I78" si="222">D73/D72-1</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J73" s="5" t="e">
+        <v>-3.4786238564032956E-4</v>
+      </c>
+      <c r="J73" s="5">
         <f t="shared" ref="J73:J78" si="223">E73/E72-1</f>
-        <v>#VALUE!</v>
+        <v>2.8280542986425239E-3</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -15076,8 +15194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15115,7 +15233,7 @@
       </c>
       <c r="G2" s="74">
         <f>SUM(G5:G10)</f>
-        <v>0.99278984877899346</v>
+        <v>0.99273339871534994</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -15167,7 +15285,7 @@
       </c>
       <c r="C5">
         <f>_xll.RealtimeData(A5,"Last")</f>
-        <v>365.29500000000002</v>
+        <v>368.35</v>
       </c>
       <c r="D5">
         <f>ROUNDDOWN(($C$2/6)/B5,0)</f>
@@ -15175,19 +15293,19 @@
       </c>
       <c r="E5" s="8">
         <f>C5/B5-1</f>
-        <v>0.10045187528242217</v>
+        <v>0.10965506853441798</v>
       </c>
       <c r="F5">
         <f>C5*D5</f>
-        <v>12785.325000000001</v>
+        <v>12892.25</v>
       </c>
       <c r="G5" s="73">
         <f>F5/$F$13</f>
-        <v>0.17375855589639394</v>
+        <v>0.1765834927563581</v>
       </c>
       <c r="H5" s="8">
         <f>F5/$F$31</f>
-        <v>0.12317991370418636</v>
+        <v>0.12486849146082236</v>
       </c>
       <c r="I5">
         <f>B5*D5</f>
@@ -15204,7 +15322,7 @@
       </c>
       <c r="C6">
         <f>_xll.RealtimeData(A6,"Last")</f>
-        <v>1885.1020000000001</v>
+        <v>1899.1</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D10" si="0">ROUNDDOWN(($C$2/6)/B6,0)</f>
@@ -15212,19 +15330,19 @@
       </c>
       <c r="E6" s="8">
         <f t="shared" ref="E6:E10" si="1">C6/B6-1</f>
-        <v>0.15677397184619735</v>
+        <v>0.16536370442188986</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F9" si="2">C6*D6</f>
-        <v>13195.714</v>
+        <v>13293.699999999999</v>
       </c>
       <c r="G6" s="73">
         <f t="shared" ref="G6:G10" si="3">F6/$F$13</f>
-        <v>0.17933593464865602</v>
+        <v>0.18208210185616922</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" ref="H6:H10" si="4">F6/$F$31</f>
-        <v>0.12713379689488721</v>
+        <v>0.12875675424636771</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I10" si="5">B6*D6</f>
@@ -15241,7 +15359,7 @@
       </c>
       <c r="C7">
         <f>_xll.RealtimeData(A7,"Last")</f>
-        <v>43.66</v>
+        <v>43.93</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -15249,19 +15367,19 @@
       </c>
       <c r="E7" s="8">
         <f t="shared" si="1"/>
-        <v>3.0202925908447309E-2</v>
+        <v>3.657385559226034E-2</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>12006.499999999998</v>
+        <v>12080.75</v>
       </c>
       <c r="G7" s="73">
         <f t="shared" si="3"/>
-        <v>0.16317395931429615</v>
+        <v>0.16546848146106174</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="4"/>
-        <v>0.11567634251685532</v>
+        <v>0.11700867018676568</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
@@ -15278,7 +15396,7 @@
       </c>
       <c r="C8">
         <f>_xll.RealtimeData(A8,"Last")</f>
-        <v>517.48</v>
+        <v>526.24130000000002</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -15286,19 +15404,19 @@
       </c>
       <c r="E8" s="8">
         <f t="shared" si="1"/>
-        <v>0.12576413514042684</v>
+        <v>0.14482411295059494</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>12937</v>
+        <v>13156.032500000001</v>
       </c>
       <c r="G8" s="73">
         <f t="shared" si="3"/>
-        <v>0.17581989019689748</v>
+        <v>0.18019648778655098</v>
       </c>
       <c r="H8" s="8">
         <f t="shared" si="4"/>
-        <v>0.12464122293262463</v>
+        <v>0.12742336922449934</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
@@ -15315,7 +15433,7 @@
       </c>
       <c r="C9">
         <f>_xll.RealtimeData(A9,"Last")</f>
-        <v>52.89</v>
+        <v>52.15</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -15323,19 +15441,19 @@
       </c>
       <c r="E9" s="8">
         <f t="shared" si="1"/>
-        <v>-8.1611390866469957E-2</v>
+        <v>-9.4460843896509883E-2</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>10683.78</v>
+        <v>10534.3</v>
       </c>
       <c r="G9" s="73">
         <f t="shared" si="3"/>
-        <v>0.14519757490050317</v>
+        <v>0.14428695439068456</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="4"/>
-        <v>0.10293262771454868</v>
+        <v>0.10203045625051801</v>
       </c>
       <c r="I9">
         <f t="shared" si="5"/>
@@ -15352,7 +15470,7 @@
       </c>
       <c r="C10">
         <f>_xll.RealtimeData(A10,"Last")</f>
-        <v>55.276000000000003</v>
+        <v>50.83</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -15360,19 +15478,19 @@
       </c>
       <c r="E10" s="8">
         <f t="shared" si="1"/>
-        <v>-1.9059449866903222E-2</v>
+        <v>-9.7959183673469452E-2</v>
       </c>
       <c r="F10">
         <f>C10*D10</f>
-        <v>11442.132000000001</v>
+        <v>10521.81</v>
       </c>
       <c r="G10" s="73">
         <f t="shared" si="3"/>
-        <v>0.15550393382224684</v>
+        <v>0.14411588046452528</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="4"/>
-        <v>0.11023895226377972</v>
+        <v>0.10190948377028024</v>
       </c>
       <c r="I10">
         <f t="shared" si="5"/>
@@ -15391,7 +15509,7 @@
       </c>
       <c r="F13" s="75">
         <f>SUM(F5:F10)+I13</f>
-        <v>73580.981</v>
+        <v>73009.372499999998</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -15407,7 +15525,7 @@
       </c>
       <c r="F14" s="8">
         <f>F13/C2-1</f>
-        <v>5.1156871428571504E-2</v>
+        <v>4.2991035714285752E-2</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -15418,7 +15536,7 @@
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H17" s="11">
         <f>SUM(H20:H23)</f>
-        <v>0.98826396513016102</v>
+        <v>0.98827340449280265</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -15460,7 +15578,7 @@
       </c>
       <c r="C20">
         <f>_xll.RealtimeData(A20,"Last")</f>
-        <v>17.170000000000002</v>
+        <v>17.16</v>
       </c>
       <c r="D20">
         <f>ROUNDDOWN(($C$3*E20)/B20,0)</f>
@@ -15471,19 +15589,19 @@
       </c>
       <c r="F20" s="8">
         <f>C20/B20-1</f>
-        <v>1.0000000000000009E-2</v>
+        <v>9.4117647058824527E-3</v>
       </c>
       <c r="G20">
         <f>D20*C20</f>
-        <v>4292.5</v>
+        <v>4290</v>
       </c>
       <c r="H20" s="8">
         <f>G20/$G$27</f>
-        <v>0.14207493281849853</v>
+        <v>0.14187798162862031</v>
       </c>
       <c r="I20" s="8">
         <f>G20/$F$31</f>
-        <v>4.1355990526265068E-2</v>
+        <v>4.1550996014421686E-2</v>
       </c>
       <c r="J20">
         <f>B20*D20</f>
@@ -15500,7 +15618,7 @@
       </c>
       <c r="C21">
         <f>_xll.RealtimeData(A21,"Last")</f>
-        <v>287.57499999999999</v>
+        <v>287.95</v>
       </c>
       <c r="D21">
         <f t="shared" ref="D21:D22" si="6">ROUNDDOWN(($C$3*E21)/B21,0)</f>
@@ -15511,19 +15629,19 @@
       </c>
       <c r="F21" s="8">
         <f t="shared" ref="F21:F23" si="7">C21/B21-1</f>
-        <v>1.6597143665158409E-2</v>
+        <v>1.7922794117646967E-2</v>
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G22" si="8">D21*C21</f>
-        <v>10927.85</v>
+        <v>10942.1</v>
       </c>
       <c r="H21" s="8">
         <f t="shared" ref="H21:H23" si="9">G21/$G$27</f>
-        <v>0.36169447981377501</v>
+        <v>0.36187483980851431</v>
       </c>
       <c r="I21" s="8">
         <f t="shared" ref="I21:I23" si="10">G21/$F$31</f>
-        <v>0.10528411440243349</v>
+        <v>0.10598022225860222</v>
       </c>
       <c r="J21">
         <f t="shared" ref="J21:J23" si="11">B21*D21</f>
@@ -15540,7 +15658,7 @@
       </c>
       <c r="C22">
         <f>_xll.RealtimeData(A22,"Last")</f>
-        <v>81.45</v>
+        <v>81.53</v>
       </c>
       <c r="D22">
         <f t="shared" si="6"/>
@@ -15551,19 +15669,19 @@
       </c>
       <c r="F22" s="8">
         <f t="shared" si="7"/>
-        <v>-8.5868498527963411E-4</v>
+        <v>1.226692836113763E-4</v>
       </c>
       <c r="G22">
         <f t="shared" si="8"/>
-        <v>11728.800000000001</v>
+        <v>11740.32</v>
       </c>
       <c r="H22" s="8">
         <f t="shared" si="9"/>
-        <v>0.3882046527761458</v>
+        <v>0.38827340449280268</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="10"/>
-        <v>0.11300084838310025</v>
+        <v>0.11371141947040447</v>
       </c>
       <c r="J22">
         <f t="shared" si="11"/>
@@ -15580,7 +15698,7 @@
       </c>
       <c r="C23">
         <f>_xll.RealtimeData(A23,"Last")</f>
-        <v>83.12</v>
+        <v>83.15</v>
       </c>
       <c r="D23">
         <f>ROUNDDOWN(($C$3*E23)/B23,0)</f>
@@ -15591,19 +15709,19 @@
       </c>
       <c r="F23" s="8">
         <f t="shared" si="7"/>
-        <v>7.2236937153857816E-4</v>
+        <v>1.0835540573079783E-3</v>
       </c>
       <c r="G23">
         <f>D23*C23</f>
-        <v>2909.2000000000003</v>
+        <v>2910.25</v>
       </c>
       <c r="H23" s="8">
         <f t="shared" si="9"/>
-        <v>9.6289899721741637E-2</v>
+        <v>9.6247178562865326E-2</v>
       </c>
       <c r="I23" s="8">
         <f t="shared" si="10"/>
-        <v>2.8028619135471253E-2</v>
+        <v>2.8187362739154009E-2</v>
       </c>
       <c r="J23">
         <f t="shared" si="11"/>
@@ -15619,7 +15737,7 @@
       </c>
       <c r="G27">
         <f>SUM(G20:G23)+J28</f>
-        <v>30212.930000000008</v>
+        <v>30237.250000000004</v>
       </c>
       <c r="J27">
         <f>SUM(J20:J23)</f>
@@ -15632,7 +15750,7 @@
       </c>
       <c r="G28" s="8">
         <f>G27/J27-1</f>
-        <v>1.9143260577856758E-2</v>
+        <v>1.9963623386007212E-2</v>
       </c>
       <c r="I28" t="s">
         <v>26</v>
@@ -15648,7 +15766,7 @@
       </c>
       <c r="F31" s="75">
         <f>SUM(F13,G27)</f>
-        <v>103793.91100000001</v>
+        <v>103246.6225</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -15657,11 +15775,11 @@
       </c>
       <c r="F33" s="8">
         <f>F31/B1-1</f>
-        <v>3.7939110000000165E-2</v>
+        <v>3.2466225000000071E-2</v>
       </c>
       <c r="H33" s="11">
         <f>F33-F37</f>
-        <v>-2.1270215314619159E-3</v>
+        <v>-6.7900095707164945E-3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -15674,16 +15792,16 @@
       </c>
       <c r="C37">
         <f>_xll.RealtimeData(A37,"Last")</f>
-        <v>38.413200000000003</v>
+        <v>38.529200000000003</v>
       </c>
       <c r="D37" s="8">
         <f>C37/B37-1</f>
-        <v>4.0041819132254908E-3</v>
+        <v>7.0360690015682792E-3</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="8">
         <f>D37*$B$3+D40*$B$2</f>
-        <v>4.0066131531462081E-2</v>
+        <v>3.9256234570716565E-2</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
@@ -15698,11 +15816,11 @@
       </c>
       <c r="C38">
         <f>_xll.RealtimeData(A38,"Last")</f>
-        <v>287.57499999999999</v>
+        <v>287.95</v>
       </c>
       <c r="D38" s="8">
         <f t="shared" ref="D38:D39" si="12">C38/B38-1</f>
-        <v>5.4431122355443007E-2</v>
+        <v>5.5806108605580551E-2</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -15715,11 +15833,11 @@
       </c>
       <c r="C39">
         <f>_xll.RealtimeData(A39,"Last")</f>
-        <v>182.11</v>
+        <v>182.41</v>
       </c>
       <c r="D39" s="8">
         <f t="shared" si="12"/>
-        <v>7.0794378785206113E-2</v>
+        <v>7.2558358323043581E-2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -15732,11 +15850,11 @@
       </c>
       <c r="C40">
         <f>_xll.RealtimeData(A40,"Last")</f>
-        <v>47.181800000000003</v>
+        <v>47.072000000000003</v>
       </c>
       <c r="D40" s="8">
         <f>C40/B40-1</f>
-        <v>5.5521252796420617E-2</v>
+        <v>5.30648769574944E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>